<commit_message>
Actualización con nuevos cambios
</commit_message>
<xml_diff>
--- a/Tutoriales/pandas/Comandos Pandas.xlsx
+++ b/Tutoriales/pandas/Comandos Pandas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoseMaría\Documents\CURSOS\data_science\mitrabajo\Mirepositorio\Tutoriales\pandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617DF95B-F3D9-4178-9C3B-36E185AA7BD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA3016B-9E68-4565-BBF6-4DDEF81B7ACB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF4018AA-EEB9-4756-B82D-183D37B3B80A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{AF4018AA-EEB9-4756-B82D-183D37B3B80A}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERALES" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="CONCEPTOS" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GENERALES!$A$2:$D$201</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GENERALES!$A$2:$D$203</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="590">
   <si>
     <t>FUNCIONES DE PANDAS</t>
   </si>
@@ -4180,9 +4180,6 @@
     <t>Para visualización de graficas</t>
   </si>
   <si>
-    <t>import matplotlib.pyplot as plt</t>
-  </si>
-  <si>
     <t>s.plot.bar(y="Quantity", stacked=True)</t>
   </si>
   <si>
@@ -5518,9 +5515,6 @@
       </rPr>
       <t>.sort_values(["quantity"],ascending=True)</t>
     </r>
-  </si>
-  <si>
-    <t>chipo_quantity.plot(kind='bar')                                     plt.xlabel('Item Name')                                       plt.ylabel('Quantity')                                                                                                           plt.title('Most boughts')                                                          plt.show()</t>
   </si>
   <si>
     <t>Diagrama tipo de barras con etiquetas y título</t>
@@ -5551,6 +5545,550 @@
   <si>
     <r>
       <rPr>
+        <sz val="20"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>df</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.set_index</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>('App'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>).T.plot(kind='bar', stacked=True)</t>
+    </r>
+  </si>
+  <si>
+    <t>males = (titanic['Sex'] == 'male').sum()                                                                         females = (titanic['Sex'] == 'female').sum()                                                               proportions = [males, females]                                                                                   plt.pie(  proportions, labels = ['Males', 'Females'], shadow = False, colors = ['blue','red'],explode = (0.15 , 0),    autopct = '%1.1f%%'startangle = 90,plt.axis('equal')plt.title("Sex Proportion")plt.tight_layout()                              plt.show()</t>
+  </si>
+  <si>
+    <t>Diagrama de quesos con dos categorias</t>
+  </si>
+  <si>
+    <t>scatterplot diagrama de puntos</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lm = sns.lmplot(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF001080"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Age'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF001080"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Fare'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF001080"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> =</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> titanic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF001080"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Sex'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF001080"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fit_reg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>False</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)                                                                                               lm.set(title = 'Fare x Age')                                                                                                                                                                                                                     axes = lm.axes                                                                                                                                                                                                                                             axes[0,0].set_ylim(-5,)                                                                                                                                                                                                        axes[0,0].set_xlim(-5,85)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>df = titanic.Fare.sort_values(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF001080"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ascending</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>False</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)                                                                                                                                                                           binsVal = np.arange(0,600,10)                                                                                                                                                                                                                           plt.hist(df, bins = binsVal)                                                                                                                                                                                                                         plt.xlabel('Fare')                                                                                                                                                                                                                                            plt.ylabel('Frequency')                                                                                                                                                                                                                                                 plt.title('Fare Payed Histrogram')                                                                                                                                                                                                        plt.show()</t>
+    </r>
+  </si>
+  <si>
+    <t>np arange (crea bins intervalo)  plt.hist (crea el plot)</t>
+  </si>
+  <si>
+    <t>Distribución de edades por generos</t>
+  </si>
+  <si>
+    <t>En horizontal diagrama de barras</t>
+  </si>
+  <si>
+    <t>Muestra de generos en dos columnas</t>
+  </si>
+  <si>
+    <r>
+      <t>appl_open =</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t> apple</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>'Adj Close</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>'].plot(title = "Apple Stock")                                                                                                    fig = appl_open.get_figure ()                                                                                                          fig.set_size_inches(13.5, 9)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>revenue_per_price</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.plot()                                                                                                                                  plt.xlabel('Unit Price (in intervals of '+str(price_interval)+')')                                                                      plt.ylabel('Revenue')                                                                                                                                                                            plt.show()</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>plt.bar(chipo_quantity.index, chipo_quantity.quantity,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>label=0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>color="red</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">")   plt.legend()                                                                                    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>plt.xticks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(rotation="vertical")                                                                                                                             plt.ylabel("-label")                                                                                                                          plt.xlabel("100000label")                                                                                                                                   plt.show()</t>
+    </r>
+  </si>
+  <si>
+    <t>LEN  COLUMNS</t>
+  </si>
+  <si>
+    <t>Agrupo la tabla por columna ("age) y  count saca los valores sin los nulos. Da una cifra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cada valor toma como uno, cuenta valores Ej Cuantes edades hay?   Toma valores que no se repiten como 50,60,40 cont count son 3, no incluye los Nan. Además me </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Muestra los valores con todos los elementos de la columna indicando cuantas veces se repiten cada uno.                                                                                                   Ej [1123344455] devuelve: 1-2 , 2-1,3-2,4-3,5-2   Ejemplo cual es el plato más pedido, como se habrá pedido varias veces cada plato, agrupa nombre del plato con el número de veces que se ha pedido cada uno en la serie.</t>
+  </si>
+  <si>
+    <t>DATAFRAME  ULTIMAS FILAS  PONER LAS PRIMERAS</t>
+  </si>
+  <si>
+    <t>CAMBIA LAS COLUMNAS DE LA DCHA A LA IZDA</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>df</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.loc[:, ::-1]</t>
+    </r>
+  </si>
+  <si>
+    <t>day_stats['mean'] = data.mean(axis = 1)</t>
+  </si>
+  <si>
+    <t>titanic_7 = pd.pivot_table(titanic, values='survived', index=['pclass'],columns=['sex'], aggfunc=np.sum)</t>
+  </si>
+  <si>
+    <t>df_2=df.pivot_table("new_deaths",index=["date"],columns=['location'])</t>
+  </si>
+  <si>
+    <t>Cambio indice "location a columnas, cambio columna "date a indice  y tome los valores de new_deaths</t>
+  </si>
+  <si>
+    <t>GROUPBAY + SUM</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>usuarios_age=usuarios</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.groupby("name").sum()</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Agrupo la tabla por colum ("name) y .SUM saca los valores fila por fila. </t>
+  </si>
+  <si>
+    <t>df_2['mean']=df_2.mean(axis=1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Añade una columna que llamo "mean"con el calculo de  la media </t>
+  </si>
+  <si>
+    <t>chipo.columns</t>
+  </si>
+  <si>
+    <t>chipo.shape</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="18"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
@@ -5617,7 +6155,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">drop("United Kingdom", axis=0)                                                                                </t>
+      <t xml:space="preserve">drop("United Kingdom", axis=0)                                                                                                                      </t>
     </r>
     <r>
       <rPr>
@@ -5671,555 +6209,32 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>df</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.set_index</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>('App'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>).T.plot(kind='bar', stacked=True)</t>
-    </r>
-  </si>
-  <si>
-    <t>males = (titanic['Sex'] == 'male').sum()                                                                         females = (titanic['Sex'] == 'female').sum()                                                               proportions = [males, females]                                                                                   plt.pie(  proportions, labels = ['Males', 'Females'], shadow = False, colors = ['blue','red'],explode = (0.15 , 0),    autopct = '%1.1f%%'startangle = 90,plt.axis('equal')plt.title("Sex Proportion")plt.tight_layout()                              plt.show()</t>
-  </si>
-  <si>
-    <t>Diagrama de quesos con dos categorias</t>
-  </si>
-  <si>
-    <t>scatterplot diagrama de puntos</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>lm = sns.lmplot(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF001080"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'Age'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF001080"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>y</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'Fare'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF001080"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> =</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> titanic</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF001080"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>hue</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'Sex'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF001080"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>fit_reg</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>False</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)                                                                                               lm.set(title = 'Fare x Age')                                                                                                                                                                                                                     axes = lm.axes                                                                                                                                                                                                                                             axes[0,0].set_ylim(-5,)                                                                                                                                                                                                        axes[0,0].set_xlim(-5,85)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>df = titanic.Fare.sort_values(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF001080"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ascending</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>False</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)                                                                                                                                                                           binsVal = np.arange(0,600,10)                                                                                                                                                                                                                           plt.hist(df, bins = binsVal)                                                                                                                                                                                                                         plt.xlabel('Fare')                                                                                                                                                                                                                                            plt.ylabel('Frequency')                                                                                                                                                                                                                                                 plt.title('Fare Payed Histrogram')                                                                                                                                                                                                        plt.show()</t>
-    </r>
-  </si>
-  <si>
-    <t>np arange (crea bins intervalo)  plt.hist (crea el plot)</t>
-  </si>
-  <si>
-    <t>Distribución de edades por generos</t>
-  </si>
-  <si>
-    <t>En horizontal diagrama de barras</t>
-  </si>
-  <si>
-    <t>Muestra de generos en dos columnas</t>
-  </si>
-  <si>
-    <r>
-      <t>appl_open =</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t> apple</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>'Adj Close</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>'].plot(title = "Apple Stock")                                                                                                    fig = appl_open.get_figure ()                                                                                                          fig.set_size_inches(13.5, 9)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>revenue_per_price</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.plot()                                                                                                                                  plt.xlabel('Unit Price (in intervals of '+str(price_interval)+')')                                                                      plt.ylabel('Revenue')                                                                                                                                                                            plt.show()</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>plt.bar(chipo_quantity.index, chipo_quantity.quantity,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>label=0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>color="red</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">")   plt.legend()                                                                                    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>plt.xticks</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(rotation="vertical")                                                                                                                             plt.ylabel("-label")                                                                                                                          plt.xlabel("100000label")                                                                                                                                   plt.show()</t>
-    </r>
-  </si>
-  <si>
-    <t>LEN  COLUMNS</t>
-  </si>
-  <si>
-    <t>Agrupo la tabla por columna ("age) y  count saca los valores sin los nulos. Da una cifra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cada valor toma como uno, cuenta valores Ej Cuantes edades hay?   Toma valores que no se repiten como 50,60,40 cont count son 3, no incluye los Nan. Además me </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Muestra los valores con todos los elementos de la columna indicando cuantas veces se repiten cada uno.                                                                                                   Ej [1123344455] devuelve: 1-2 , 2-1,3-2,4-3,5-2   Ejemplo cual es el plato más pedido, como se habrá pedido varias veces cada plato, agrupa nombre del plato con el número de veces que se ha pedido cada uno en la serie.</t>
-  </si>
-  <si>
-    <t>DATAFRAME  ULTIMAS FILAS  PONER LAS PRIMERAS</t>
-  </si>
-  <si>
-    <t>CAMBIA LAS COLUMNAS DE LA DCHA A LA IZDA</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>df</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.loc[:, ::-1]</t>
-    </r>
-  </si>
-  <si>
-    <t>day_stats['mean'] = data.mean(axis = 1)</t>
-  </si>
-  <si>
-    <t>titanic_7 = pd.pivot_table(titanic, values='survived', index=['pclass'],columns=['sex'], aggfunc=np.sum)</t>
-  </si>
-  <si>
-    <t>df_2=df.pivot_table("new_deaths",index=["date"],columns=['location'])</t>
-  </si>
-  <si>
-    <t>Cambio indice "location a columnas, cambio columna "date a indice  y tome los valores de new_deaths</t>
-  </si>
-  <si>
-    <t>GROUPBAY + SUM</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>usuarios_age=usuarios</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.groupby("name").sum()</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Agrupo la tabla por colum ("name) y .SUM saca los valores fila por fila. </t>
-  </si>
-  <si>
-    <t>df_2['mean']=df_2.mean(axis=1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Añade una columna que llamo "mean"con el calculo de  la media </t>
-  </si>
-  <si>
-    <t>chipo.columns</t>
-  </si>
-  <si>
-    <t>chipo.shape</t>
+    <t>chipo_quantity.plot(kind='bar')                                                               plt.xlabel('Item Name')                                                           plt.ylabel('Quantity')                                                                                                           plt.title('Most boughts')                                                          plt.show()</t>
+  </si>
+  <si>
+    <t>import matplotlib.pyplot as plt</t>
+  </si>
+  <si>
+    <t>df = df.drop(df[df.score &lt; 50].index)</t>
+  </si>
+  <si>
+    <t>Eliminar todas las filas donde la columna 'puntuación' es &lt;50:</t>
+  </si>
+  <si>
+    <t>def.loc[~(def==0).all(axis=1)]</t>
+  </si>
+  <si>
+    <t>Eliminamos las filas cuyos valores son 0 en todas sus columnas</t>
+  </si>
+  <si>
+    <t>BORRAR CON CODICION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="57">
+  <fonts count="58">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6591,6 +6606,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="20">
     <fill>
@@ -6744,7 +6766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7153,6 +7175,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="45" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="57" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7171,8 +7196,9 @@
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7539,7 +7565,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13287375" y="13848182"/>
+          <a:off x="15297150" y="16454857"/>
           <a:ext cx="2635250" cy="2178866"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7627,7 +7653,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13242015" y="29797375"/>
+          <a:off x="15251790" y="53397150"/>
           <a:ext cx="3054150" cy="1698625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8111,7 +8137,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13197747" y="10985501"/>
+          <a:off x="15207522" y="13598526"/>
           <a:ext cx="2841866" cy="2286000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8993,10 +9019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265136A6-C067-4B28-9F45-A6266FF6FD67}">
-  <dimension ref="A1:D204"/>
+  <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A43" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9008,16 +9034,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="33.75" customHeight="1">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="179" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="103" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B2" s="88" t="s">
         <v>2</v>
@@ -9031,7 +9057,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="103" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B3" s="88" t="s">
         <v>2</v>
@@ -9045,7 +9071,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="103" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B4" s="88" t="s">
         <v>2</v>
@@ -9059,7 +9085,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="103" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B5" s="88" t="s">
         <v>2</v>
@@ -9073,7 +9099,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="103" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B6" s="88" t="s">
         <v>2</v>
@@ -9087,7 +9113,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="103" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B7" s="88" t="s">
         <v>2</v>
@@ -9101,13 +9127,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="103" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B8" s="88" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="90" t="s">
-        <v>411</v>
+        <v>584</v>
       </c>
       <c r="D8" s="90" t="s">
         <v>410</v>
@@ -9115,10 +9141,10 @@
     </row>
     <row r="9" spans="1:4" s="4" customFormat="1">
       <c r="A9" s="91" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B9" s="97" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C9" s="128" t="s">
         <v>4</v>
@@ -9129,13 +9155,13 @@
     </row>
     <row r="10" spans="1:4" s="4" customFormat="1">
       <c r="A10" s="91" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B10" s="97" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C10" s="69" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D10" s="128" t="s">
         <v>313</v>
@@ -9143,10 +9169,10 @@
     </row>
     <row r="11" spans="1:4" s="4" customFormat="1">
       <c r="A11" s="91" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B11" s="97" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C11" s="69" t="s">
         <v>373</v>
@@ -9157,10 +9183,10 @@
     </row>
     <row r="12" spans="1:4" s="4" customFormat="1" ht="30">
       <c r="A12" s="91" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B12" s="97" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C12" s="92" t="s">
         <v>378</v>
@@ -9171,10 +9197,10 @@
     </row>
     <row r="13" spans="1:4" s="4" customFormat="1">
       <c r="A13" s="91" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B13" s="97" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C13" s="69" t="s">
         <v>257</v>
@@ -9185,10 +9211,10 @@
     </row>
     <row r="14" spans="1:4" s="4" customFormat="1">
       <c r="A14" s="91" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B14" s="97" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C14" s="69" t="s">
         <v>88</v>
@@ -9199,10 +9225,10 @@
     </row>
     <row r="15" spans="1:4" s="3" customFormat="1" ht="30">
       <c r="A15" s="91" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B15" s="97" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C15" s="94" t="s">
         <v>55</v>
@@ -9213,10 +9239,10 @@
     </row>
     <row r="16" spans="1:4" s="3" customFormat="1" ht="17.25" customHeight="1">
       <c r="A16" s="91" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B16" s="97" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C16" s="96" t="s">
         <v>327</v>
@@ -9227,10 +9253,10 @@
     </row>
     <row r="17" spans="1:4" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A17" s="91" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B17" s="97" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C17" s="96" t="s">
         <v>190</v>
@@ -9244,7 +9270,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="98" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C18" s="99" t="s">
         <v>10</v>
@@ -9258,10 +9284,10 @@
         <v>7</v>
       </c>
       <c r="B19" s="98" t="s">
-        <v>472</v>
-      </c>
-      <c r="C19" s="183" t="s">
-        <v>584</v>
+        <v>471</v>
+      </c>
+      <c r="C19" s="177" t="s">
+        <v>581</v>
       </c>
       <c r="D19" s="99" t="s">
         <v>12</v>
@@ -9272,7 +9298,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="98" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C20" s="99" t="s">
         <v>15</v>
@@ -9286,7 +9312,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="98" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C21" s="99" t="s">
         <v>63</v>
@@ -9300,7 +9326,7 @@
         <v>7</v>
       </c>
       <c r="B22" s="98" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C22" s="99" t="s">
         <v>13</v>
@@ -9314,7 +9340,7 @@
         <v>7</v>
       </c>
       <c r="B23" s="98" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C23" s="99" t="s">
         <v>64</v>
@@ -9339,7 +9365,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="100" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B25" s="102" t="s">
         <v>33</v>
@@ -9353,7 +9379,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="100" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B26" s="102" t="s">
         <v>33</v>
@@ -9367,16 +9393,16 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="100" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B27" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="182" t="s">
-        <v>583</v>
+      <c r="C27" s="176" t="s">
+        <v>580</v>
       </c>
       <c r="D27" s="101" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -9384,13 +9410,13 @@
         <v>8</v>
       </c>
       <c r="B28" s="102" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C28" s="101" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D28" s="101" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -9398,21 +9424,21 @@
         <v>8</v>
       </c>
       <c r="B29" s="102" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C29" s="101" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D29" s="101" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="3" customFormat="1">
       <c r="A30" s="148" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B30" s="151" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C30" s="149" t="s">
         <v>280</v>
@@ -9423,10 +9449,10 @@
     </row>
     <row r="31" spans="1:4" s="3" customFormat="1">
       <c r="A31" s="148" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B31" s="151" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C31" s="149" t="s">
         <v>281</v>
@@ -9437,24 +9463,24 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="148" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B32" s="102" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C32" s="101" t="s">
+        <v>517</v>
+      </c>
+      <c r="D32" s="101" t="s">
         <v>518</v>
-      </c>
-      <c r="D32" s="101" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="61" t="s">
+        <v>480</v>
+      </c>
+      <c r="B33" s="72" t="s">
         <v>481</v>
-      </c>
-      <c r="B33" s="72" t="s">
-        <v>482</v>
       </c>
       <c r="C33" s="86" t="s">
         <v>18</v>
@@ -9465,7 +9491,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="61" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B34" s="72" t="s">
         <v>56</v>
@@ -9479,7 +9505,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="61" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B35" s="72" t="s">
         <v>60</v>
@@ -9493,7 +9519,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="61" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B36" s="72" t="s">
         <v>60</v>
@@ -9507,10 +9533,10 @@
     </row>
     <row r="37" spans="1:4" s="3" customFormat="1" ht="29.25" customHeight="1">
       <c r="A37" s="142" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B37" s="130" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>181</v>
@@ -9521,33 +9547,33 @@
     </row>
     <row r="38" spans="1:4" s="3" customFormat="1" ht="30">
       <c r="A38" s="142" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B38" s="130" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C38" s="13" t="s">
+        <v>456</v>
+      </c>
+      <c r="D38" s="13" t="s">
         <v>457</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="61" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B39" s="72" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="C39" s="86" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="D39" s="104"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="61" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B40" s="72" t="s">
         <v>6</v>
@@ -9561,7 +9587,7 @@
     </row>
     <row r="41" spans="1:4" s="108" customFormat="1" ht="14.25" customHeight="1">
       <c r="A41" s="61" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B41" s="72" t="s">
         <v>114</v>
@@ -9575,7 +9601,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="61" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B42" s="72" t="s">
         <v>114</v>
@@ -9589,7 +9615,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="61" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B43" s="72" t="s">
         <v>114</v>
@@ -9603,7 +9629,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="61" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B44" s="72" t="s">
         <v>92</v>
@@ -9617,7 +9643,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="143" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B45" s="72" t="s">
         <v>273</v>
@@ -9631,7 +9657,7 @@
     </row>
     <row r="46" spans="1:4" s="4" customFormat="1" ht="30">
       <c r="A46" s="143" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B46" s="73" t="s">
         <v>273</v>
@@ -9645,21 +9671,21 @@
     </row>
     <row r="47" spans="1:4" s="4" customFormat="1">
       <c r="A47" s="143" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B47" s="73" t="s">
         <v>273</v>
       </c>
       <c r="C47" s="144" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="D47" s="145" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="3" customFormat="1">
       <c r="A48" s="8" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>245</v>
@@ -9673,7 +9699,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="61" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B49" s="72" t="s">
         <v>347</v>
@@ -9687,7 +9713,7 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="61" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B50" s="72" t="s">
         <v>351</v>
@@ -9704,7 +9730,7 @@
         <v>39</v>
       </c>
       <c r="B51" s="72" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C51" s="62" t="s">
         <v>381</v>
@@ -9715,10 +9741,10 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="61" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B52" s="72" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C52" s="86" t="s">
         <v>67</v>
@@ -9729,7 +9755,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="61" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B53" s="72" t="s">
         <v>6</v>
@@ -9743,7 +9769,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="61" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B54" s="72" t="s">
         <v>6</v>
@@ -9752,12 +9778,12 @@
         <v>125</v>
       </c>
       <c r="D54" s="104" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="61" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B55" s="72" t="s">
         <v>6</v>
@@ -9771,7 +9797,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="61" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B56" s="72" t="s">
         <v>6</v>
@@ -9785,7 +9811,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="61" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B57" s="72" t="s">
         <v>6</v>
@@ -9799,7 +9825,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="61" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B58" s="72" t="s">
         <v>6</v>
@@ -9813,7 +9839,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="61" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B59" s="72" t="s">
         <v>114</v>
@@ -9827,7 +9853,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="61" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B60" s="72" t="s">
         <v>114</v>
@@ -9841,7 +9867,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="61" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B61" s="72" t="s">
         <v>114</v>
@@ -9855,7 +9881,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="61" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B62" s="72" t="s">
         <v>114</v>
@@ -9869,7 +9895,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="61" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B63" s="72" t="s">
         <v>114</v>
@@ -9883,7 +9909,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="61" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B64" s="72" t="s">
         <v>114</v>
@@ -9897,7 +9923,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="61" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B65" s="72" t="s">
         <v>114</v>
@@ -9911,10 +9937,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="105" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B66" s="110" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C66" s="106" t="s">
         <v>156</v>
@@ -9925,10 +9951,10 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="105" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B67" s="110" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C67" s="106" t="s">
         <v>159</v>
@@ -9939,10 +9965,10 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="105" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B68" s="110" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C68" s="106" t="s">
         <v>162</v>
@@ -9953,10 +9979,10 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="105" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B69" s="110" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C69" s="147" t="s">
         <v>94</v>
@@ -9967,7 +9993,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="105" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B70" s="110" t="s">
         <v>186</v>
@@ -9981,7 +10007,7 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="105" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B71" s="110" t="s">
         <v>114</v>
@@ -9995,7 +10021,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="105" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B72" s="110" t="s">
         <v>114</v>
@@ -10009,10 +10035,10 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="105" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B73" s="110" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C73" s="147" t="s">
         <v>96</v>
@@ -10023,10 +10049,10 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="105" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B74" s="110" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C74" s="147" t="s">
         <v>250</v>
@@ -10037,7 +10063,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="80" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B75" s="77" t="s">
         <v>71</v>
@@ -10051,7 +10077,7 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="80" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B76" s="77" t="s">
         <v>84</v>
@@ -10065,7 +10091,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="80" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B77" s="77" t="s">
         <v>390</v>
@@ -10079,7 +10105,7 @@
     </row>
     <row r="78" spans="1:4" s="4" customFormat="1" ht="30">
       <c r="A78" s="125" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B78" s="126" t="s">
         <v>45</v>
@@ -10093,13 +10119,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="80" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B79" s="77" t="s">
         <v>118</v>
       </c>
       <c r="C79" s="78" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D79" s="78" t="s">
         <v>28</v>
@@ -10107,13 +10133,13 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="80" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B80" s="77" t="s">
         <v>26</v>
       </c>
       <c r="C80" s="78" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D80" s="78" t="s">
         <v>117</v>
@@ -10121,7 +10147,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="80" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B81" s="77" t="s">
         <v>26</v>
@@ -10135,7 +10161,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="80" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B82" s="77" t="s">
         <v>53</v>
@@ -10149,7 +10175,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="80" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B83" s="77" t="s">
         <v>122</v>
@@ -10197,7 +10223,7 @@
         <v>214</v>
       </c>
       <c r="C86" s="79" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D86" s="78" t="s">
         <v>216</v>
@@ -10222,13 +10248,13 @@
         <v>212</v>
       </c>
       <c r="B88" s="77" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C88" s="78" t="s">
+        <v>533</v>
+      </c>
+      <c r="D88" s="78" t="s">
         <v>534</v>
-      </c>
-      <c r="D88" s="78" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -10236,13 +10262,13 @@
         <v>212</v>
       </c>
       <c r="B89" s="77" t="s">
+        <v>537</v>
+      </c>
+      <c r="C89" s="78" t="s">
+        <v>536</v>
+      </c>
+      <c r="D89" s="78" t="s">
         <v>538</v>
-      </c>
-      <c r="C89" s="78" t="s">
-        <v>537</v>
-      </c>
-      <c r="D89" s="78" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -10250,13 +10276,13 @@
         <v>212</v>
       </c>
       <c r="B90" s="77" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C90" s="78" t="s">
+        <v>539</v>
+      </c>
+      <c r="D90" s="78" t="s">
         <v>540</v>
-      </c>
-      <c r="D90" s="78" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -10264,13 +10290,13 @@
         <v>212</v>
       </c>
       <c r="B91" s="77" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C91" s="78" t="s">
+        <v>542</v>
+      </c>
+      <c r="D91" s="78" t="s">
         <v>543</v>
-      </c>
-      <c r="D91" s="78" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -10278,13 +10304,13 @@
         <v>361</v>
       </c>
       <c r="B92" s="175" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="C92" s="174" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="D92" s="82" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -10298,7 +10324,7 @@
         <v>78</v>
       </c>
       <c r="D93" s="82" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -10359,7 +10385,7 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="115" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B98" s="114" t="s">
         <v>40</v>
@@ -10373,7 +10399,7 @@
     </row>
     <row r="99" spans="1:4" s="3" customFormat="1">
       <c r="A99" s="115" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B99" s="146" t="s">
         <v>272</v>
@@ -10387,7 +10413,7 @@
     </row>
     <row r="100" spans="1:4" s="3" customFormat="1">
       <c r="A100" s="115" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B100" s="146" t="s">
         <v>272</v>
@@ -10401,7 +10427,7 @@
     </row>
     <row r="101" spans="1:4" s="3" customFormat="1">
       <c r="A101" s="115" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B101" s="146" t="s">
         <v>259</v>
@@ -10415,7 +10441,7 @@
     </row>
     <row r="102" spans="1:4" s="3" customFormat="1">
       <c r="A102" s="115" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B102" s="146" t="s">
         <v>269</v>
@@ -10429,7 +10455,7 @@
     </row>
     <row r="103" spans="1:4" s="3" customFormat="1">
       <c r="A103" s="115" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B103" s="146" t="s">
         <v>269</v>
@@ -10443,13 +10469,13 @@
     </row>
     <row r="104" spans="1:4" s="4" customFormat="1" ht="39.75" customHeight="1">
       <c r="A104" s="120" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B104" s="121" t="s">
         <v>222</v>
       </c>
       <c r="C104" s="122" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D104" s="123" t="s">
         <v>223</v>
@@ -10457,7 +10483,7 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="120" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B105" s="36" t="s">
         <v>149</v>
@@ -10471,7 +10497,7 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="120" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B106" s="36" t="s">
         <v>150</v>
@@ -10485,7 +10511,7 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="120" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B107" s="36" t="s">
         <v>151</v>
@@ -10499,7 +10525,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="120" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B108" s="36" t="s">
         <v>148</v>
@@ -10513,13 +10539,13 @@
     </row>
     <row r="109" spans="1:4" ht="15.75">
       <c r="A109" s="168" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B109" s="168" t="s">
         <v>217</v>
       </c>
       <c r="C109" s="172" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="D109" s="169" t="s">
         <v>218</v>
@@ -10527,16 +10553,16 @@
     </row>
     <row r="110" spans="1:4" ht="30">
       <c r="A110" s="170" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B110" s="170" t="s">
         <v>217</v>
       </c>
       <c r="C110" s="173" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="D110" s="171" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="111" spans="1:4" s="3" customFormat="1">
@@ -10754,7 +10780,7 @@
         <v>1</v>
       </c>
       <c r="B126" s="72" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C126" s="62" t="s">
         <v>69</v>
@@ -10768,7 +10794,7 @@
         <v>1</v>
       </c>
       <c r="B127" s="72" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C127" s="62" t="s">
         <v>73</v>
@@ -10782,7 +10808,7 @@
         <v>1</v>
       </c>
       <c r="B128" s="72" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C128" s="62" t="s">
         <v>169</v>
@@ -10841,7 +10867,7 @@
         <v>76</v>
       </c>
       <c r="C132" s="85" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D132" s="62" t="s">
         <v>240</v>
@@ -10992,13 +11018,13 @@
         <v>80</v>
       </c>
       <c r="B143" s="83" t="s">
+        <v>426</v>
+      </c>
+      <c r="C143" s="82" t="s">
         <v>427</v>
       </c>
-      <c r="C143" s="82" t="s">
-        <v>428</v>
-      </c>
       <c r="D143" s="82" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -11057,46 +11083,46 @@
         <v>208</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" ht="15.75">
       <c r="A148" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="B148" s="131" t="s">
+      <c r="B148" s="83" t="s">
         <v>207</v>
       </c>
-      <c r="C148" s="132" t="s">
+      <c r="C148" s="82" t="s">
+        <v>585</v>
+      </c>
+      <c r="D148" s="178" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B149" s="83" t="s">
+        <v>589</v>
+      </c>
+      <c r="C149" s="82" t="s">
+        <v>587</v>
+      </c>
+      <c r="D149" s="185" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B150" s="131" t="s">
+        <v>207</v>
+      </c>
+      <c r="C150" s="132" t="s">
         <v>209</v>
       </c>
-      <c r="D148" s="132" t="s">
+      <c r="D150" s="132" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4">
-      <c r="A149" s="68" t="s">
-        <v>8</v>
-      </c>
-      <c r="B149" s="71" t="s">
-        <v>514</v>
-      </c>
-      <c r="C149" s="70" t="s">
-        <v>66</v>
-      </c>
-      <c r="D149" s="70" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4">
-      <c r="A150" s="68" t="s">
-        <v>8</v>
-      </c>
-      <c r="B150" s="71" t="s">
-        <v>514</v>
-      </c>
-      <c r="C150" s="70" t="s">
-        <v>517</v>
-      </c>
-      <c r="D150" s="70" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -11104,13 +11130,13 @@
         <v>8</v>
       </c>
       <c r="B151" s="71" t="s">
+        <v>513</v>
+      </c>
+      <c r="C151" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="D151" s="70" t="s">
         <v>514</v>
-      </c>
-      <c r="C151" s="70" t="s">
-        <v>524</v>
-      </c>
-      <c r="D151" s="70" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -11118,13 +11144,13 @@
         <v>8</v>
       </c>
       <c r="B152" s="71" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="C152" s="70" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D152" s="70" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -11132,13 +11158,13 @@
         <v>8</v>
       </c>
       <c r="B153" s="71" t="s">
-        <v>455</v>
+        <v>513</v>
       </c>
       <c r="C153" s="70" t="s">
-        <v>290</v>
+        <v>523</v>
       </c>
       <c r="D153" s="70" t="s">
-        <v>450</v>
+        <v>522</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -11146,13 +11172,13 @@
         <v>8</v>
       </c>
       <c r="B154" s="71" t="s">
-        <v>455</v>
+        <v>520</v>
       </c>
       <c r="C154" s="70" t="s">
-        <v>456</v>
+        <v>517</v>
       </c>
       <c r="D154" s="70" t="s">
-        <v>454</v>
+        <v>518</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -11160,13 +11186,13 @@
         <v>8</v>
       </c>
       <c r="B155" s="71" t="s">
-        <v>292</v>
+        <v>454</v>
       </c>
       <c r="C155" s="70" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D155" s="70" t="s">
-        <v>294</v>
+        <v>449</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -11174,13 +11200,13 @@
         <v>8</v>
       </c>
       <c r="B156" s="71" t="s">
-        <v>8</v>
-      </c>
-      <c r="C156" s="69" t="s">
-        <v>9</v>
+        <v>454</v>
+      </c>
+      <c r="C156" s="70" t="s">
+        <v>455</v>
       </c>
       <c r="D156" s="70" t="s">
-        <v>11</v>
+        <v>453</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -11188,13 +11214,13 @@
         <v>8</v>
       </c>
       <c r="B157" s="71" t="s">
-        <v>8</v>
-      </c>
-      <c r="C157" s="69" t="s">
-        <v>20</v>
+        <v>292</v>
+      </c>
+      <c r="C157" s="70" t="s">
+        <v>293</v>
       </c>
       <c r="D157" s="70" t="s">
-        <v>65</v>
+        <v>294</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -11205,10 +11231,10 @@
         <v>8</v>
       </c>
       <c r="C158" s="69" t="s">
-        <v>394</v>
+        <v>9</v>
       </c>
       <c r="D158" s="70" t="s">
-        <v>395</v>
+        <v>11</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -11219,10 +11245,10 @@
         <v>8</v>
       </c>
       <c r="C159" s="69" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D159" s="70" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -11233,10 +11259,10 @@
         <v>8</v>
       </c>
       <c r="C160" s="69" t="s">
-        <v>363</v>
+        <v>394</v>
       </c>
       <c r="D160" s="70" t="s">
-        <v>364</v>
+        <v>395</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -11247,10 +11273,10 @@
         <v>8</v>
       </c>
       <c r="C161" s="69" t="s">
-        <v>365</v>
+        <v>9</v>
       </c>
       <c r="D161" s="70" t="s">
-        <v>366</v>
+        <v>11</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -11258,13 +11284,13 @@
         <v>8</v>
       </c>
       <c r="B162" s="71" t="s">
-        <v>445</v>
+        <v>8</v>
       </c>
       <c r="C162" s="69" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D162" s="70" t="s">
-        <v>444</v>
+        <v>364</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -11272,97 +11298,97 @@
         <v>8</v>
       </c>
       <c r="B163" s="71" t="s">
-        <v>445</v>
+        <v>8</v>
       </c>
       <c r="C163" s="69" t="s">
         <v>365</v>
       </c>
       <c r="D163" s="70" t="s">
-        <v>446</v>
+        <v>366</v>
       </c>
     </row>
     <row r="164" spans="1:4">
-      <c r="A164" s="72" t="s">
-        <v>331</v>
-      </c>
-      <c r="B164" s="61" t="s">
-        <v>509</v>
-      </c>
-      <c r="C164" s="62" t="s">
-        <v>178</v>
-      </c>
-      <c r="D164" s="62" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A165" s="72" t="s">
-        <v>331</v>
-      </c>
-      <c r="B165" s="130" t="s">
-        <v>439</v>
-      </c>
-      <c r="C165" s="13" t="s">
-        <v>429</v>
-      </c>
-      <c r="D165" s="13" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" s="3" customFormat="1" ht="30">
+      <c r="A164" s="68" t="s">
+        <v>8</v>
+      </c>
+      <c r="B164" s="71" t="s">
+        <v>444</v>
+      </c>
+      <c r="C164" s="69" t="s">
+        <v>365</v>
+      </c>
+      <c r="D164" s="70" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" s="68" t="s">
+        <v>8</v>
+      </c>
+      <c r="B165" s="71" t="s">
+        <v>444</v>
+      </c>
+      <c r="C165" s="69" t="s">
+        <v>365</v>
+      </c>
+      <c r="D165" s="70" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
       <c r="A166" s="72" t="s">
         <v>331</v>
       </c>
-      <c r="B166" s="130" t="s">
-        <v>439</v>
-      </c>
-      <c r="C166" s="13" t="s">
-        <v>451</v>
-      </c>
-      <c r="D166" s="13" t="s">
+      <c r="B166" s="61" t="s">
+        <v>508</v>
+      </c>
+      <c r="C166" s="62" t="s">
+        <v>178</v>
+      </c>
+      <c r="D166" s="62" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A167" s="72" t="s">
+        <v>331</v>
+      </c>
+      <c r="B167" s="130" t="s">
+        <v>438</v>
+      </c>
+      <c r="C167" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="D167" s="13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" s="3" customFormat="1" ht="30">
+      <c r="A168" s="72" t="s">
+        <v>331</v>
+      </c>
+      <c r="B168" s="130" t="s">
+        <v>438</v>
+      </c>
+      <c r="C168" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="D168" s="13" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="167" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A167" s="73" t="s">
-        <v>331</v>
-      </c>
-      <c r="B167" s="130" t="s">
-        <v>439</v>
-      </c>
-      <c r="C167" s="63" t="s">
-        <v>353</v>
-      </c>
-      <c r="D167" s="13" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A168" s="73" t="s">
-        <v>331</v>
-      </c>
-      <c r="B168" s="130" t="s">
-        <v>439</v>
-      </c>
-      <c r="C168" s="63" t="s">
-        <v>430</v>
-      </c>
-      <c r="D168" s="13" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" s="3" customFormat="1" ht="76.5" customHeight="1">
+    <row r="169" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
       <c r="A169" s="73" t="s">
         <v>331</v>
       </c>
       <c r="B169" s="130" t="s">
-        <v>510</v>
-      </c>
-      <c r="C169" s="13" t="s">
-        <v>334</v>
+        <v>438</v>
+      </c>
+      <c r="C169" s="63" t="s">
+        <v>353</v>
       </c>
       <c r="D169" s="13" t="s">
-        <v>333</v>
+        <v>352</v>
       </c>
     </row>
     <row r="170" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
@@ -11370,55 +11396,55 @@
         <v>331</v>
       </c>
       <c r="B170" s="130" t="s">
-        <v>511</v>
-      </c>
-      <c r="C170" s="13" t="s">
-        <v>335</v>
+        <v>438</v>
+      </c>
+      <c r="C170" s="63" t="s">
+        <v>429</v>
       </c>
       <c r="D170" s="13" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" s="3" customFormat="1" ht="76.5" customHeight="1">
       <c r="A171" s="73" t="s">
         <v>331</v>
       </c>
       <c r="B171" s="130" t="s">
+        <v>509</v>
+      </c>
+      <c r="C171" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="D171" s="13" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
+      <c r="A172" s="73" t="s">
+        <v>331</v>
+      </c>
+      <c r="B172" s="130" t="s">
+        <v>510</v>
+      </c>
+      <c r="C172" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="D172" s="13" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
+      <c r="A173" s="73" t="s">
+        <v>331</v>
+      </c>
+      <c r="B173" s="130" t="s">
+        <v>431</v>
+      </c>
+      <c r="C173" s="13" t="s">
         <v>432</v>
       </c>
-      <c r="C171" s="13" t="s">
-        <v>433</v>
-      </c>
-      <c r="D171" s="13" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4">
-      <c r="A172" s="75" t="s">
-        <v>189</v>
-      </c>
-      <c r="B172" s="11" t="s">
-        <v>322</v>
-      </c>
-      <c r="C172" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="D172" s="12" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" s="4" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A173" s="75" t="s">
-        <v>189</v>
-      </c>
-      <c r="B173" s="64" t="s">
-        <v>322</v>
-      </c>
-      <c r="C173" s="65" t="s">
-        <v>434</v>
-      </c>
-      <c r="D173" s="66" t="s">
-        <v>435</v>
+      <c r="D173" s="13" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -11429,192 +11455,192 @@
         <v>322</v>
       </c>
       <c r="C174" s="12" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="D174" s="12" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" s="4" customFormat="1" ht="39.75" customHeight="1">
       <c r="A175" s="75" t="s">
         <v>189</v>
       </c>
-      <c r="B175" s="11" t="s">
+      <c r="B175" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="C175" s="12" t="s">
-        <v>346</v>
-      </c>
-      <c r="D175" s="12" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" s="4" customFormat="1">
+      <c r="C175" s="65" t="s">
+        <v>433</v>
+      </c>
+      <c r="D175" s="66" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
       <c r="A176" s="75" t="s">
         <v>189</v>
       </c>
-      <c r="B176" s="74" t="s">
+      <c r="B176" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="C176" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="D176" s="12" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" s="75" t="s">
+        <v>189</v>
+      </c>
+      <c r="B177" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="C177" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="D177" s="12" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" s="4" customFormat="1">
+      <c r="A178" s="75" t="s">
+        <v>189</v>
+      </c>
+      <c r="B178" s="74" t="s">
         <v>317</v>
       </c>
-      <c r="C176" s="66" t="s">
+      <c r="C178" s="66" t="s">
         <v>316</v>
       </c>
-      <c r="D176" s="66" t="s">
+      <c r="D178" s="66" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="177" spans="1:4">
-      <c r="A177" s="76" t="s">
+    <row r="179" spans="1:4">
+      <c r="A179" s="76" t="s">
         <v>189</v>
       </c>
-      <c r="B177" s="11" t="s">
+      <c r="B179" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="C177" s="12" t="s">
+      <c r="C179" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="D177" s="66" t="s">
+      <c r="D179" s="66" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="178" spans="1:4">
-      <c r="A178" s="114" t="s">
+    <row r="180" spans="1:4">
+      <c r="A180" s="114" t="s">
         <v>193</v>
       </c>
-      <c r="B178" s="114" t="s">
+      <c r="B180" s="114" t="s">
         <v>191</v>
       </c>
-      <c r="C178" s="116" t="s">
+      <c r="C180" s="116" t="s">
         <v>195</v>
       </c>
-      <c r="D178" s="116" t="s">
+      <c r="D180" s="116" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="179" spans="1:4">
-      <c r="A179" s="114" t="s">
+    <row r="181" spans="1:4">
+      <c r="A181" s="114" t="s">
         <v>193</v>
       </c>
-      <c r="B179" s="114" t="s">
+      <c r="B181" s="114" t="s">
         <v>191</v>
       </c>
-      <c r="C179" s="116" t="s">
+      <c r="C181" s="116" t="s">
         <v>197</v>
       </c>
-      <c r="D179" s="116" t="s">
+      <c r="D181" s="116" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="180" spans="1:4" s="3" customFormat="1">
-      <c r="A180" s="133" t="s">
-        <v>253</v>
-      </c>
-      <c r="B180" s="158" t="s">
-        <v>255</v>
-      </c>
-      <c r="C180" s="134" t="s">
-        <v>256</v>
-      </c>
-      <c r="D180" s="135" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" s="87" customFormat="1">
-      <c r="A181" s="133" t="s">
-        <v>253</v>
-      </c>
-      <c r="B181" s="158" t="s">
-        <v>296</v>
-      </c>
-      <c r="C181" s="134" t="s">
-        <v>295</v>
-      </c>
-      <c r="D181" s="135" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" s="87" customFormat="1">
+    <row r="182" spans="1:4" s="3" customFormat="1">
       <c r="A182" s="133" t="s">
         <v>253</v>
       </c>
       <c r="B182" s="158" t="s">
+        <v>255</v>
+      </c>
+      <c r="C182" s="134" t="s">
+        <v>256</v>
+      </c>
+      <c r="D182" s="135" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" s="87" customFormat="1">
+      <c r="A183" s="133" t="s">
+        <v>253</v>
+      </c>
+      <c r="B183" s="158" t="s">
+        <v>296</v>
+      </c>
+      <c r="C183" s="134" t="s">
+        <v>295</v>
+      </c>
+      <c r="D183" s="135" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" s="87" customFormat="1">
+      <c r="A184" s="133" t="s">
+        <v>253</v>
+      </c>
+      <c r="B184" s="158" t="s">
         <v>289</v>
       </c>
-      <c r="C182" s="134" t="s">
+      <c r="C184" s="134" t="s">
         <v>288</v>
       </c>
-      <c r="D182" s="135" t="s">
+      <c r="D184" s="135" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="183" spans="1:4" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A183" s="136" t="s">
+    <row r="185" spans="1:4" s="4" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A185" s="136" t="s">
         <v>253</v>
       </c>
-      <c r="B183" s="158" t="s">
-        <v>471</v>
-      </c>
-      <c r="C183" s="137" t="s">
+      <c r="B185" s="158" t="s">
+        <v>470</v>
+      </c>
+      <c r="C185" s="137" t="s">
         <v>380</v>
       </c>
-      <c r="D183" s="138" t="s">
+      <c r="D185" s="138" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="184" spans="1:4" s="39" customFormat="1" ht="144.75" customHeight="1">
-      <c r="A184" s="139" t="s">
-        <v>253</v>
-      </c>
-      <c r="B184" s="159" t="s">
-        <v>512</v>
-      </c>
-      <c r="C184" s="137" t="s">
-        <v>496</v>
-      </c>
-      <c r="D184" s="138" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4">
-      <c r="A185" s="160" t="s">
-        <v>253</v>
-      </c>
-      <c r="B185" s="161" t="s">
-        <v>520</v>
-      </c>
-      <c r="C185" s="162" t="s">
-        <v>522</v>
-      </c>
-      <c r="D185" s="162" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" s="39" customFormat="1" ht="28.5" customHeight="1">
+    <row r="186" spans="1:4" s="39" customFormat="1" ht="144.75" customHeight="1">
       <c r="A186" s="139" t="s">
         <v>253</v>
       </c>
       <c r="B186" s="159" t="s">
-        <v>442</v>
-      </c>
-      <c r="C186" s="140" t="s">
-        <v>466</v>
+        <v>511</v>
+      </c>
+      <c r="C186" s="137" t="s">
+        <v>495</v>
       </c>
       <c r="D186" s="138" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" s="39" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A187" s="139" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" s="160" t="s">
         <v>253</v>
       </c>
-      <c r="B187" s="159" t="s">
-        <v>442</v>
-      </c>
-      <c r="C187" s="140" t="s">
-        <v>467</v>
-      </c>
-      <c r="D187" s="138" t="s">
-        <v>440</v>
+      <c r="B187" s="161" t="s">
+        <v>519</v>
+      </c>
+      <c r="C187" s="162" t="s">
+        <v>521</v>
+      </c>
+      <c r="D187" s="162" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="188" spans="1:4" s="39" customFormat="1" ht="28.5" customHeight="1">
@@ -11622,69 +11648,69 @@
         <v>253</v>
       </c>
       <c r="B188" s="159" t="s">
-        <v>443</v>
-      </c>
-      <c r="C188" s="141" t="s">
-        <v>448</v>
+        <v>441</v>
+      </c>
+      <c r="C188" s="140" t="s">
+        <v>465</v>
       </c>
       <c r="D188" s="138" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" s="4" customFormat="1" ht="38.25" customHeight="1">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" s="39" customFormat="1" ht="28.5" customHeight="1">
       <c r="A189" s="139" t="s">
         <v>253</v>
       </c>
       <c r="B189" s="159" t="s">
-        <v>245</v>
-      </c>
-      <c r="C189" s="137" t="s">
-        <v>465</v>
+        <v>441</v>
+      </c>
+      <c r="C189" s="140" t="s">
+        <v>466</v>
       </c>
       <c r="D189" s="138" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" s="39" customFormat="1" ht="28.5" customHeight="1">
       <c r="A190" s="139" t="s">
         <v>253</v>
       </c>
       <c r="B190" s="159" t="s">
+        <v>442</v>
+      </c>
+      <c r="C190" s="141" t="s">
         <v>447</v>
       </c>
-      <c r="C190" s="137" t="s">
-        <v>525</v>
-      </c>
       <c r="D190" s="138" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" s="4" customFormat="1" ht="38.25" customHeight="1">
       <c r="A191" s="139" t="s">
         <v>253</v>
       </c>
       <c r="B191" s="159" t="s">
-        <v>463</v>
+        <v>245</v>
       </c>
       <c r="C191" s="137" t="s">
         <v>464</v>
       </c>
       <c r="D191" s="138" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1">
       <c r="A192" s="139" t="s">
         <v>253</v>
       </c>
       <c r="B192" s="159" t="s">
-        <v>530</v>
+        <v>446</v>
       </c>
       <c r="C192" s="137" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="D192" s="138" t="s">
-        <v>532</v>
+        <v>458</v>
       </c>
     </row>
     <row r="193" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
@@ -11692,55 +11718,55 @@
         <v>253</v>
       </c>
       <c r="B193" s="159" t="s">
-        <v>528</v>
+        <v>462</v>
       </c>
       <c r="C193" s="137" t="s">
-        <v>527</v>
+        <v>463</v>
       </c>
       <c r="D193" s="138" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
       <c r="A194" s="139" t="s">
         <v>253</v>
       </c>
       <c r="B194" s="159" t="s">
-        <v>462</v>
+        <v>529</v>
       </c>
       <c r="C194" s="137" t="s">
+        <v>528</v>
+      </c>
+      <c r="D194" s="138" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
+      <c r="A195" s="139" t="s">
+        <v>253</v>
+      </c>
+      <c r="B195" s="159" t="s">
+        <v>527</v>
+      </c>
+      <c r="C195" s="137" t="s">
+        <v>526</v>
+      </c>
+      <c r="D195" s="138" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="A196" s="139" t="s">
+        <v>253</v>
+      </c>
+      <c r="B196" s="159" t="s">
+        <v>461</v>
+      </c>
+      <c r="C196" s="137" t="s">
+        <v>459</v>
+      </c>
+      <c r="D196" s="138" t="s">
         <v>460</v>
-      </c>
-      <c r="D194" s="138" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4">
-      <c r="A195" s="124" t="s">
-        <v>224</v>
-      </c>
-      <c r="B195" s="124" t="s">
-        <v>225</v>
-      </c>
-      <c r="C195" s="37" t="s">
-        <v>251</v>
-      </c>
-      <c r="D195" s="37" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4">
-      <c r="A196" s="124" t="s">
-        <v>224</v>
-      </c>
-      <c r="B196" s="124" t="s">
-        <v>225</v>
-      </c>
-      <c r="C196" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="D196" s="37" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -11750,11 +11776,11 @@
       <c r="B197" s="124" t="s">
         <v>225</v>
       </c>
-      <c r="C197" s="157" t="s">
-        <v>303</v>
+      <c r="C197" s="37" t="s">
+        <v>251</v>
       </c>
       <c r="D197" s="37" t="s">
-        <v>304</v>
+        <v>226</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -11764,11 +11790,11 @@
       <c r="B198" s="124" t="s">
         <v>225</v>
       </c>
-      <c r="C198" s="157" t="s">
-        <v>310</v>
+      <c r="C198" s="37" t="s">
+        <v>227</v>
       </c>
       <c r="D198" s="37" t="s">
-        <v>306</v>
+        <v>263</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -11779,10 +11805,10 @@
         <v>225</v>
       </c>
       <c r="C199" s="157" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D199" s="37" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -11793,10 +11819,10 @@
         <v>225</v>
       </c>
       <c r="C200" s="157" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D200" s="37" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -11807,10 +11833,10 @@
         <v>225</v>
       </c>
       <c r="C201" s="157" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D201" s="37" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -11820,25 +11846,53 @@
       <c r="B202" s="124" t="s">
         <v>225</v>
       </c>
-      <c r="C202" s="37" t="s">
+      <c r="C202" s="157" t="s">
+        <v>308</v>
+      </c>
+      <c r="D202" s="37" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" s="124" t="s">
+        <v>224</v>
+      </c>
+      <c r="B203" s="124" t="s">
+        <v>225</v>
+      </c>
+      <c r="C203" s="157" t="s">
+        <v>311</v>
+      </c>
+      <c r="D203" s="37" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204" s="124" t="s">
+        <v>224</v>
+      </c>
+      <c r="B204" s="124" t="s">
+        <v>225</v>
+      </c>
+      <c r="C204" s="37" t="s">
         <v>397</v>
       </c>
-      <c r="D202" s="37"/>
-    </row>
-    <row r="203" spans="1:4">
-      <c r="A203" s="5"/>
-      <c r="B203" s="5"/>
-      <c r="C203" s="6"/>
-      <c r="D203" s="6"/>
-    </row>
-    <row r="204" spans="1:4">
-      <c r="A204" s="5"/>
-      <c r="B204" s="5"/>
-      <c r="C204" s="6"/>
-      <c r="D204" s="6"/>
+      <c r="D204" s="37"/>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205" s="5"/>
+      <c r="B205" s="5"/>
+      <c r="C205" s="6"/>
+      <c r="D205" s="6"/>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206" s="5"/>
+      <c r="B206" s="5"/>
+      <c r="C206" s="6"/>
+      <c r="D206" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D201" xr:uid="{85ED3410-72EE-453D-8BB3-FB7E07F682B1}"/>
+  <autoFilter ref="A2:D203" xr:uid="{85ED3410-72EE-453D-8BB3-FB7E07F682B1}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
@@ -11852,8 +11906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C42D88-9A2B-46D3-B46D-33526406379A}">
   <dimension ref="A1:E223"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26.25"/>
@@ -11867,13 +11921,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33.75" customHeight="1">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="181" t="s">
         <v>224</v>
       </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="179"/>
-      <c r="E1" s="180"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="183"/>
     </row>
     <row r="2" spans="1:5" ht="207" customHeight="1">
       <c r="A2" s="44" t="s">
@@ -11911,11 +11965,11 @@
         <v>225</v>
       </c>
       <c r="C4" s="165" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="167" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="207" customHeight="1">
@@ -11941,11 +11995,11 @@
         <v>225</v>
       </c>
       <c r="C6" s="163" t="s">
-        <v>549</v>
+        <v>583</v>
       </c>
       <c r="D6" s="44"/>
       <c r="E6" s="55" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="207" customHeight="1">
@@ -11956,11 +12010,11 @@
         <v>225</v>
       </c>
       <c r="C7" s="163" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D7" s="44"/>
       <c r="E7" s="55" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="207" customHeight="1">
@@ -11971,11 +12025,11 @@
         <v>225</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>553</v>
+        <v>582</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="55" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="207" customHeight="1">
@@ -11986,11 +12040,11 @@
         <v>225</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D9" s="44"/>
       <c r="E9" s="55" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="207" customHeight="1">
@@ -12001,11 +12055,11 @@
         <v>225</v>
       </c>
       <c r="C10" s="55" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D10" s="44"/>
       <c r="E10" s="55" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="207" customHeight="1">
@@ -12016,11 +12070,11 @@
         <v>225</v>
       </c>
       <c r="C11" s="165" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="D11" s="44"/>
       <c r="E11" s="166" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="207" customHeight="1">
@@ -12047,7 +12101,7 @@
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="58" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="207" customHeight="1">
@@ -12060,7 +12114,7 @@
       <c r="C14" s="59"/>
       <c r="D14" s="6"/>
       <c r="E14" s="58" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="207" customHeight="1">
@@ -12073,7 +12127,7 @@
       <c r="C15" s="59"/>
       <c r="D15" s="6"/>
       <c r="E15" s="58" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="207" customHeight="1">
@@ -12091,11 +12145,11 @@
         <v>225</v>
       </c>
       <c r="C17" s="55" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D17" s="44"/>
       <c r="E17" s="67" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="207" customHeight="1">
@@ -12106,11 +12160,11 @@
         <v>225</v>
       </c>
       <c r="C18" s="55" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D18" s="44"/>
       <c r="E18" s="55" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="207" customHeight="1">
@@ -12121,11 +12175,11 @@
         <v>225</v>
       </c>
       <c r="C19" s="55" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D19" s="44"/>
       <c r="E19" s="55" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="207" customHeight="1">
@@ -12133,14 +12187,14 @@
         <v>224</v>
       </c>
       <c r="B20" s="45" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D20" s="44"/>
       <c r="E20" s="55" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="207" customHeight="1">
@@ -12148,7 +12202,7 @@
         <v>224</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C21" s="59" t="s">
         <v>310</v>
@@ -12163,10 +12217,10 @@
         <v>224</v>
       </c>
       <c r="B22" s="45" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="D22" s="44"/>
       <c r="E22" s="55" t="s">
@@ -12178,14 +12232,14 @@
         <v>224</v>
       </c>
       <c r="B23" s="45" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C23" s="47" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D23" s="44"/>
       <c r="E23" s="55" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="207" customHeight="1">
@@ -12226,11 +12280,11 @@
         <v>225</v>
       </c>
       <c r="C26" s="55" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D26" s="44"/>
       <c r="E26" s="55" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="207" customHeight="1">
@@ -12241,11 +12295,11 @@
         <v>225</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D27" s="44"/>
       <c r="E27" s="55" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="207" customHeight="1">
@@ -12256,11 +12310,11 @@
         <v>225</v>
       </c>
       <c r="C28" s="44" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D28" s="44"/>
       <c r="E28" s="55" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="207" customHeight="1">
@@ -13175,7 +13229,7 @@
   <dimension ref="A1:C212"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -13187,11 +13241,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="33.75" customHeight="1">
-      <c r="A1" s="181" t="s">
+      <c r="A1" s="184" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="181"/>
+      <c r="B1" s="184"/>
+      <c r="C1" s="184"/>
     </row>
     <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="17" t="s">
@@ -13256,7 +13310,7 @@
         <v>359</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="41" customFormat="1" ht="67.5" customHeight="1">
@@ -13267,7 +13321,7 @@
         <v>360</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="19" customFormat="1" ht="20.100000000000001" customHeight="1">
@@ -13286,10 +13340,10 @@
         <v>358</v>
       </c>
       <c r="B10" s="38" t="s">
+        <v>418</v>
+      </c>
+      <c r="C10" s="35" t="s">
         <v>419</v>
-      </c>
-      <c r="C10" s="35" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1">

</xml_diff>

<commit_message>
Mi repositorio con trabajo proy conj filtrado end
</commit_message>
<xml_diff>
--- a/Tutoriales/pandas/Comandos Pandas.xlsx
+++ b/Tutoriales/pandas/Comandos Pandas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoseMaría\Documents\CURSOS\data_science\mitrabajo\Mirepositorio\Tutoriales\pandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FD1F1A-35EA-4D45-8A53-52DEE5B2BED0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78676BB1-9249-4862-B4AC-B008A1352094}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{AF4018AA-EEB9-4756-B82D-183D37B3B80A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF4018AA-EEB9-4756-B82D-183D37B3B80A}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERALES" sheetId="1" r:id="rId1"/>
@@ -9755,8 +9755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265136A6-C067-4B28-9F45-A6266FF6FD67}">
   <dimension ref="A1:D208"/>
   <sheetViews>
-    <sheetView topLeftCell="C181" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="D188" sqref="D188"/>
+    <sheetView tabSelected="1" topLeftCell="C175" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="D184" sqref="D184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12684,8 +12684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C42D88-9A2B-46D3-B46D-33526406379A}">
   <dimension ref="A1:E228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A22" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26.25"/>

</xml_diff>

<commit_message>
Actualización repositorio web scraping
</commit_message>
<xml_diff>
--- a/Tutoriales/pandas/Comandos Pandas.xlsx
+++ b/Tutoriales/pandas/Comandos Pandas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoseMaría\Documents\CURSOS\data_science\mitrabajo\mi_repositorio\Tutoriales\pandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590BBD9F-CAB2-4696-9507-7D1DB3BFE62B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C13966-A4EF-441D-9240-B845EED8F319}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{AF4018AA-EEB9-4756-B82D-183D37B3B80A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF4018AA-EEB9-4756-B82D-183D37B3B80A}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERALES" sheetId="1" r:id="rId1"/>
@@ -9900,8 +9900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265136A6-C067-4B28-9F45-A6266FF6FD67}">
   <dimension ref="A1:D219"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12982,7 +12982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C42D88-9A2B-46D3-B46D-33526406379A}">
   <dimension ref="A1:E228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Vacunas actualizado 18 de agosto 21:13
</commit_message>
<xml_diff>
--- a/Tutoriales/pandas/Comandos Pandas.xlsx
+++ b/Tutoriales/pandas/Comandos Pandas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoseMaría\Documents\CURSOS\data_science\mitrabajo\mi_repositorio\Tutoriales\pandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C13966-A4EF-441D-9240-B845EED8F319}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C286080B-7CBF-4FF5-BDA9-B3E3E37FB40F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF4018AA-EEB9-4756-B82D-183D37B3B80A}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="CONCEPTOS" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GENERALES!$A$2:$D$210</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GENERALES!$A$2:$D$213</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="644">
   <si>
     <t>FUNCIONES DE PANDAS</t>
   </si>
@@ -6451,6 +6451,46 @@
   </si>
   <si>
     <t>plt.pie tipo de representación. IMPORTANTE: CON EL autopct="%1.2f%%" LE DIGO QUE TOME UN EMTERO Y DOS DECIMALES EN EL TANTO PORCIENTO</t>
+  </si>
+  <si>
+    <t>resident_age.loc[:,["rango_edad","municipio_nombre","poblacion_empadronada"]]</t>
+  </si>
+  <si>
+    <t>Muestra todas las filas de tres columnas alternas llamadas por su nombre</t>
+  </si>
+  <si>
+    <t>resident_age1=resident_age1.pivot_table('poblacion_empadronada', index='rango_edad',columns=['municipio_nombre',"sexo"],aggfunc=np.sum)</t>
+  </si>
+  <si>
+    <t>Cambio indice , en esta caso pongo rango edad y en columans municipio_nombre y sexo y me suma los valores de numero de defunciones</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pd.to_numeric</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(chipo)</t>
+    </r>
+  </si>
+  <si>
+    <t>Cambia el tipo de dato dataframe a numerico</t>
+  </si>
+  <si>
+    <t>TO_NUMERIC</t>
   </si>
 </sst>
 </file>
@@ -7098,7 +7138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="65" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="212">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7592,6 +7632,9 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9898,10 +9941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265136A6-C067-4B28-9F45-A6266FF6FD67}">
-  <dimension ref="A1:D219"/>
+  <dimension ref="A1:D222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10340,18 +10383,18 @@
         <v>607</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="3" customFormat="1">
+    <row r="32" spans="1:4">
       <c r="A32" s="147" t="s">
         <v>496</v>
       </c>
-      <c r="B32" s="150" t="s">
-        <v>495</v>
-      </c>
-      <c r="C32" s="148" t="s">
-        <v>277</v>
-      </c>
-      <c r="D32" s="149" t="s">
-        <v>276</v>
+      <c r="B32" s="101" t="s">
+        <v>643</v>
+      </c>
+      <c r="C32" s="212" t="s">
+        <v>641</v>
+      </c>
+      <c r="D32" s="100" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="3" customFormat="1">
@@ -10359,41 +10402,41 @@
         <v>496</v>
       </c>
       <c r="B33" s="150" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C33" s="148" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D33" s="149" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="3" customFormat="1">
       <c r="A34" s="147" t="s">
         <v>496</v>
       </c>
-      <c r="B34" s="101" t="s">
+      <c r="B34" s="150" t="s">
+        <v>494</v>
+      </c>
+      <c r="C34" s="148" t="s">
+        <v>278</v>
+      </c>
+      <c r="D34" s="149" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="147" t="s">
+        <v>496</v>
+      </c>
+      <c r="B35" s="101" t="s">
         <v>512</v>
       </c>
-      <c r="C34" s="100" t="s">
+      <c r="C35" s="100" t="s">
         <v>510</v>
       </c>
-      <c r="D34" s="100" t="s">
+      <c r="D35" s="100" t="s">
         <v>511</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="60" t="s">
-        <v>473</v>
-      </c>
-      <c r="B35" s="71" t="s">
-        <v>474</v>
-      </c>
-      <c r="C35" s="85" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" s="103" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -10401,13 +10444,13 @@
         <v>473</v>
       </c>
       <c r="B36" s="71" t="s">
-        <v>56</v>
+        <v>474</v>
       </c>
       <c r="C36" s="85" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="D36" s="103" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -10415,13 +10458,13 @@
         <v>473</v>
       </c>
       <c r="B37" s="71" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C37" s="85" t="s">
-        <v>257</v>
+        <v>57</v>
       </c>
       <c r="D37" s="103" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -10432,27 +10475,27 @@
         <v>60</v>
       </c>
       <c r="C38" s="85" t="s">
+        <v>257</v>
+      </c>
+      <c r="D38" s="103" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="60" t="s">
+        <v>473</v>
+      </c>
+      <c r="B39" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="D38" s="103" t="s">
+      <c r="D39" s="103" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:4" s="3" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A39" s="141" t="s">
-        <v>473</v>
-      </c>
-      <c r="B39" s="129" t="s">
-        <v>559</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="3" customFormat="1" ht="30">
+    <row r="40" spans="1:4" s="3" customFormat="1" ht="29.25" customHeight="1">
       <c r="A40" s="141" t="s">
         <v>473</v>
       </c>
@@ -10460,67 +10503,67 @@
         <v>559</v>
       </c>
       <c r="C40" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="3" customFormat="1" ht="30">
+      <c r="A41" s="141" t="s">
+        <v>473</v>
+      </c>
+      <c r="B41" s="129" t="s">
+        <v>559</v>
+      </c>
+      <c r="C41" s="12" t="s">
         <v>449</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D41" s="12" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="4" customFormat="1">
-      <c r="A41" s="141" t="s">
+    <row r="42" spans="1:4" s="4" customFormat="1">
+      <c r="A42" s="141" t="s">
         <v>483</v>
       </c>
-      <c r="B41" s="142" t="s">
+      <c r="B42" s="142" t="s">
         <v>594</v>
       </c>
-      <c r="C41" s="188" t="s">
+      <c r="C42" s="188" t="s">
         <v>593</v>
       </c>
-      <c r="D41" s="188" t="s">
+      <c r="D42" s="188" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="60" t="s">
-        <v>476</v>
-      </c>
-      <c r="B42" s="71" t="s">
-        <v>560</v>
-      </c>
-      <c r="C42" s="85" t="s">
-        <v>561</v>
-      </c>
-      <c r="D42" s="103"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="60" t="s">
         <v>476</v>
       </c>
       <c r="B43" s="71" t="s">
-        <v>6</v>
+        <v>560</v>
       </c>
       <c r="C43" s="85" t="s">
-        <v>125</v>
-      </c>
-      <c r="D43" s="103" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="107" customFormat="1" ht="14.25" customHeight="1">
+        <v>561</v>
+      </c>
+      <c r="D43" s="103"/>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="60" t="s">
         <v>476</v>
       </c>
       <c r="B44" s="71" t="s">
-        <v>114</v>
+        <v>6</v>
       </c>
       <c r="C44" s="85" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D44" s="103" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="107" customFormat="1" ht="14.25" customHeight="1">
       <c r="A45" s="60" t="s">
         <v>476</v>
       </c>
@@ -10528,10 +10571,10 @@
         <v>114</v>
       </c>
       <c r="C45" s="85" t="s">
-        <v>35</v>
+        <v>116</v>
       </c>
       <c r="D45" s="103" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -10542,10 +10585,10 @@
         <v>114</v>
       </c>
       <c r="C46" s="85" t="s">
-        <v>129</v>
+        <v>35</v>
       </c>
       <c r="D46" s="103" t="s">
-        <v>130</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -10556,10 +10599,10 @@
         <v>114</v>
       </c>
       <c r="C47" s="85" t="s">
-        <v>610</v>
+        <v>129</v>
       </c>
       <c r="D47" s="103" t="s">
-        <v>611</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -10567,44 +10610,44 @@
         <v>476</v>
       </c>
       <c r="B48" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="85" t="s">
+        <v>610</v>
+      </c>
+      <c r="D48" s="103" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="60" t="s">
+        <v>476</v>
+      </c>
+      <c r="B49" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="85" t="s">
+      <c r="C49" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="D48" s="103" t="s">
+      <c r="D49" s="103" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="142" t="s">
-        <v>489</v>
-      </c>
-      <c r="B49" s="71" t="s">
-        <v>270</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="D49" s="103" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="4" customFormat="1" ht="30">
+    <row r="50" spans="1:4">
       <c r="A50" s="142" t="s">
         <v>489</v>
       </c>
-      <c r="B50" s="72" t="s">
+      <c r="B50" s="71" t="s">
         <v>270</v>
       </c>
-      <c r="C50" s="143" t="s">
-        <v>388</v>
-      </c>
-      <c r="D50" s="144" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" s="4" customFormat="1">
+      <c r="C50" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="D50" s="103" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="4" customFormat="1" ht="30">
       <c r="A51" s="142" t="s">
         <v>489</v>
       </c>
@@ -10612,38 +10655,38 @@
         <v>270</v>
       </c>
       <c r="C51" s="143" t="s">
+        <v>388</v>
+      </c>
+      <c r="D51" s="144" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="4" customFormat="1">
+      <c r="A52" s="142" t="s">
+        <v>489</v>
+      </c>
+      <c r="B52" s="72" t="s">
+        <v>270</v>
+      </c>
+      <c r="C52" s="143" t="s">
         <v>569</v>
       </c>
-      <c r="D51" s="144" t="s">
+      <c r="D52" s="144" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="52" spans="1:4" s="3" customFormat="1">
-      <c r="A52" s="7" t="s">
+    <row r="53" spans="1:4" s="3" customFormat="1">
+      <c r="A53" s="7" t="s">
         <v>498</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B53" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="C52" s="151" t="s">
+      <c r="C53" s="151" t="s">
         <v>244</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="D53" s="12" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="60" t="s">
-        <v>492</v>
-      </c>
-      <c r="B53" s="71" t="s">
-        <v>343</v>
-      </c>
-      <c r="C53" s="61" t="s">
-        <v>190</v>
-      </c>
-      <c r="D53" s="61" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -10651,41 +10694,41 @@
         <v>492</v>
       </c>
       <c r="B54" s="71" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C54" s="61" t="s">
-        <v>346</v>
+        <v>190</v>
       </c>
       <c r="D54" s="61" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="60" t="s">
-        <v>39</v>
+        <v>492</v>
       </c>
       <c r="B55" s="71" t="s">
-        <v>480</v>
+        <v>347</v>
       </c>
       <c r="C55" s="61" t="s">
-        <v>377</v>
+        <v>346</v>
       </c>
       <c r="D55" s="61" t="s">
-        <v>378</v>
+        <v>345</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="60" t="s">
-        <v>478</v>
+        <v>39</v>
       </c>
       <c r="B56" s="71" t="s">
-        <v>475</v>
-      </c>
-      <c r="C56" s="85" t="s">
-        <v>67</v>
-      </c>
-      <c r="D56" s="103" t="s">
-        <v>68</v>
+        <v>480</v>
+      </c>
+      <c r="C56" s="61" t="s">
+        <v>377</v>
+      </c>
+      <c r="D56" s="61" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -10693,13 +10736,13 @@
         <v>478</v>
       </c>
       <c r="B57" s="71" t="s">
-        <v>6</v>
+        <v>475</v>
       </c>
       <c r="C57" s="85" t="s">
-        <v>115</v>
+        <v>67</v>
       </c>
       <c r="D57" s="103" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -10710,10 +10753,10 @@
         <v>6</v>
       </c>
       <c r="C58" s="85" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D58" s="103" t="s">
-        <v>477</v>
+        <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -10724,10 +10767,10 @@
         <v>6</v>
       </c>
       <c r="C59" s="85" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D59" s="103" t="s">
-        <v>134</v>
+        <v>477</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -10738,10 +10781,10 @@
         <v>6</v>
       </c>
       <c r="C60" s="85" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D60" s="103" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -10752,10 +10795,10 @@
         <v>6</v>
       </c>
       <c r="C61" s="85" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D61" s="103" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -10766,10 +10809,10 @@
         <v>6</v>
       </c>
       <c r="C62" s="85" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="D62" s="103" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -10777,13 +10820,13 @@
         <v>478</v>
       </c>
       <c r="B63" s="71" t="s">
-        <v>114</v>
+        <v>6</v>
       </c>
       <c r="C63" s="85" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="D63" s="103" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -10794,10 +10837,10 @@
         <v>114</v>
       </c>
       <c r="C64" s="85" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D64" s="103" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -10808,10 +10851,10 @@
         <v>114</v>
       </c>
       <c r="C65" s="85" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D65" s="103" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -10822,10 +10865,10 @@
         <v>114</v>
       </c>
       <c r="C66" s="85" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="D66" s="103" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -10836,10 +10879,10 @@
         <v>114</v>
       </c>
       <c r="C67" s="85" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="D67" s="103" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -10850,10 +10893,10 @@
         <v>114</v>
       </c>
       <c r="C68" s="85" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D68" s="103" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -10864,38 +10907,38 @@
         <v>114</v>
       </c>
       <c r="C69" s="85" t="s">
+        <v>142</v>
+      </c>
+      <c r="D69" s="103" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="60" t="s">
+        <v>478</v>
+      </c>
+      <c r="B70" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="C70" s="85" t="s">
+        <v>637</v>
+      </c>
+      <c r="D70" s="103" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="60" t="s">
+        <v>478</v>
+      </c>
+      <c r="B71" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="C71" s="85" t="s">
         <v>144</v>
       </c>
-      <c r="D69" s="108" t="s">
+      <c r="D71" s="108" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="104" t="s">
-        <v>472</v>
-      </c>
-      <c r="B70" s="109" t="s">
-        <v>479</v>
-      </c>
-      <c r="C70" s="105" t="s">
-        <v>154</v>
-      </c>
-      <c r="D70" s="106" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="104" t="s">
-        <v>472</v>
-      </c>
-      <c r="B71" s="109" t="s">
-        <v>479</v>
-      </c>
-      <c r="C71" s="105" t="s">
-        <v>157</v>
-      </c>
-      <c r="D71" s="106" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -10906,10 +10949,10 @@
         <v>479</v>
       </c>
       <c r="C72" s="105" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D72" s="106" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -10919,11 +10962,11 @@
       <c r="B73" s="109" t="s">
         <v>479</v>
       </c>
-      <c r="C73" s="146" t="s">
-        <v>94</v>
-      </c>
-      <c r="D73" s="146" t="s">
-        <v>95</v>
+      <c r="C73" s="105" t="s">
+        <v>157</v>
+      </c>
+      <c r="D73" s="106" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -10931,13 +10974,13 @@
         <v>472</v>
       </c>
       <c r="B74" s="109" t="s">
-        <v>184</v>
+        <v>479</v>
       </c>
       <c r="C74" s="105" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="D74" s="106" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -10945,13 +10988,13 @@
         <v>472</v>
       </c>
       <c r="B75" s="109" t="s">
-        <v>114</v>
-      </c>
-      <c r="C75" s="105" t="s">
-        <v>158</v>
-      </c>
-      <c r="D75" s="106" t="s">
-        <v>159</v>
+        <v>479</v>
+      </c>
+      <c r="C75" s="146" t="s">
+        <v>94</v>
+      </c>
+      <c r="D75" s="146" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -10959,13 +11002,13 @@
         <v>472</v>
       </c>
       <c r="B76" s="109" t="s">
-        <v>114</v>
+        <v>184</v>
       </c>
       <c r="C76" s="105" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="D76" s="106" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -10973,13 +11016,13 @@
         <v>472</v>
       </c>
       <c r="B77" s="109" t="s">
-        <v>490</v>
-      </c>
-      <c r="C77" s="146" t="s">
-        <v>96</v>
-      </c>
-      <c r="D77" s="146" t="s">
-        <v>97</v>
+        <v>114</v>
+      </c>
+      <c r="C77" s="105" t="s">
+        <v>158</v>
+      </c>
+      <c r="D77" s="106" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -10987,97 +11030,97 @@
         <v>472</v>
       </c>
       <c r="B78" s="109" t="s">
+        <v>114</v>
+      </c>
+      <c r="C78" s="105" t="s">
+        <v>163</v>
+      </c>
+      <c r="D78" s="106" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="104" t="s">
+        <v>472</v>
+      </c>
+      <c r="B79" s="109" t="s">
+        <v>490</v>
+      </c>
+      <c r="C79" s="146" t="s">
+        <v>96</v>
+      </c>
+      <c r="D79" s="146" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="104" t="s">
+        <v>472</v>
+      </c>
+      <c r="B80" s="109" t="s">
         <v>491</v>
       </c>
-      <c r="C78" s="146" t="s">
+      <c r="C80" s="146" t="s">
         <v>247</v>
       </c>
-      <c r="D78" s="146" t="s">
+      <c r="D80" s="146" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="79" t="s">
-        <v>484</v>
-      </c>
-      <c r="B79" s="76" t="s">
-        <v>71</v>
-      </c>
-      <c r="C79" s="77" t="s">
-        <v>83</v>
-      </c>
-      <c r="D79" s="77" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="79" t="s">
-        <v>484</v>
-      </c>
-      <c r="B80" s="76" t="s">
-        <v>84</v>
-      </c>
-      <c r="C80" s="78" t="s">
-        <v>81</v>
-      </c>
-      <c r="D80" s="77" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="79" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B81" s="76" t="s">
-        <v>386</v>
+        <v>71</v>
       </c>
       <c r="C81" s="77" t="s">
-        <v>385</v>
+        <v>83</v>
       </c>
       <c r="D81" s="77" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" s="4" customFormat="1" ht="30">
-      <c r="A82" s="124" t="s">
-        <v>483</v>
-      </c>
-      <c r="B82" s="125" t="s">
-        <v>45</v>
-      </c>
-      <c r="C82" s="126" t="s">
-        <v>44</v>
-      </c>
-      <c r="D82" s="126" t="s">
-        <v>350</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="79" t="s">
+        <v>484</v>
+      </c>
+      <c r="B82" s="76" t="s">
+        <v>84</v>
+      </c>
+      <c r="C82" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="D82" s="77" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="79" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B83" s="76" t="s">
-        <v>118</v>
+        <v>386</v>
       </c>
       <c r="C83" s="77" t="s">
-        <v>539</v>
+        <v>385</v>
       </c>
       <c r="D83" s="77" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="79" t="s">
-        <v>481</v>
-      </c>
-      <c r="B84" s="76" t="s">
-        <v>26</v>
-      </c>
-      <c r="C84" s="77" t="s">
-        <v>540</v>
-      </c>
-      <c r="D84" s="77" t="s">
-        <v>117</v>
+        <v>387</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" s="4" customFormat="1" ht="30">
+      <c r="A84" s="124" t="s">
+        <v>483</v>
+      </c>
+      <c r="B84" s="125" t="s">
+        <v>45</v>
+      </c>
+      <c r="C84" s="126" t="s">
+        <v>44</v>
+      </c>
+      <c r="D84" s="126" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -11085,97 +11128,97 @@
         <v>481</v>
       </c>
       <c r="B85" s="76" t="s">
-        <v>26</v>
+        <v>118</v>
       </c>
       <c r="C85" s="77" t="s">
-        <v>120</v>
+        <v>539</v>
       </c>
       <c r="D85" s="77" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="79" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B86" s="76" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="C86" s="77" t="s">
-        <v>52</v>
+        <v>540</v>
       </c>
       <c r="D86" s="77" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="79" t="s">
-        <v>612</v>
-      </c>
-      <c r="B87" s="79" t="s">
-        <v>613</v>
+        <v>481</v>
+      </c>
+      <c r="B87" s="76" t="s">
+        <v>26</v>
       </c>
       <c r="C87" s="77" t="s">
-        <v>615</v>
+        <v>120</v>
       </c>
       <c r="D87" s="77" t="s">
-        <v>614</v>
+        <v>119</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="79" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="B88" s="76" t="s">
-        <v>122</v>
+        <v>53</v>
       </c>
       <c r="C88" s="77" t="s">
-        <v>601</v>
-      </c>
-      <c r="D88" s="128" t="s">
-        <v>602</v>
+        <v>52</v>
+      </c>
+      <c r="D88" s="77" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="79" t="s">
-        <v>249</v>
-      </c>
-      <c r="B89" s="76" t="s">
-        <v>230</v>
+        <v>612</v>
+      </c>
+      <c r="B89" s="79" t="s">
+        <v>613</v>
       </c>
       <c r="C89" s="77" t="s">
-        <v>246</v>
+        <v>615</v>
       </c>
       <c r="D89" s="77" t="s">
-        <v>229</v>
+        <v>614</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="79" t="s">
-        <v>210</v>
+        <v>487</v>
       </c>
       <c r="B90" s="76" t="s">
-        <v>209</v>
+        <v>122</v>
       </c>
       <c r="C90" s="77" t="s">
-        <v>211</v>
-      </c>
-      <c r="D90" s="77" t="s">
-        <v>213</v>
+        <v>601</v>
+      </c>
+      <c r="D90" s="128" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="79" t="s">
-        <v>210</v>
+        <v>249</v>
       </c>
       <c r="B91" s="76" t="s">
-        <v>212</v>
-      </c>
-      <c r="C91" s="78" t="s">
-        <v>525</v>
+        <v>230</v>
+      </c>
+      <c r="C91" s="77" t="s">
+        <v>246</v>
       </c>
       <c r="D91" s="77" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -11183,13 +11226,13 @@
         <v>210</v>
       </c>
       <c r="B92" s="76" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
       <c r="C92" s="77" t="s">
-        <v>245</v>
+        <v>211</v>
       </c>
       <c r="D92" s="77" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -11197,13 +11240,13 @@
         <v>210</v>
       </c>
       <c r="B93" s="76" t="s">
-        <v>528</v>
-      </c>
-      <c r="C93" s="77" t="s">
-        <v>526</v>
+        <v>212</v>
+      </c>
+      <c r="C93" s="78" t="s">
+        <v>525</v>
       </c>
       <c r="D93" s="77" t="s">
-        <v>527</v>
+        <v>214</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -11211,13 +11254,13 @@
         <v>210</v>
       </c>
       <c r="B94" s="76" t="s">
-        <v>530</v>
+        <v>232</v>
       </c>
       <c r="C94" s="77" t="s">
-        <v>529</v>
+        <v>245</v>
       </c>
       <c r="D94" s="77" t="s">
-        <v>531</v>
+        <v>231</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -11225,13 +11268,13 @@
         <v>210</v>
       </c>
       <c r="B95" s="76" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="C95" s="77" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="D95" s="77" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -11239,139 +11282,139 @@
         <v>210</v>
       </c>
       <c r="B96" s="76" t="s">
+        <v>530</v>
+      </c>
+      <c r="C96" s="77" t="s">
+        <v>529</v>
+      </c>
+      <c r="D96" s="77" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="79" t="s">
+        <v>210</v>
+      </c>
+      <c r="B97" s="76" t="s">
+        <v>534</v>
+      </c>
+      <c r="C97" s="77" t="s">
+        <v>532</v>
+      </c>
+      <c r="D97" s="77" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="79" t="s">
+        <v>210</v>
+      </c>
+      <c r="B98" s="76" t="s">
         <v>537</v>
       </c>
-      <c r="C96" s="77" t="s">
+      <c r="C98" s="77" t="s">
         <v>535</v>
       </c>
-      <c r="D96" s="77" t="s">
+      <c r="D98" s="77" t="s">
         <v>536</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="80" t="s">
-        <v>357</v>
-      </c>
-      <c r="B97" s="174" t="s">
-        <v>566</v>
-      </c>
-      <c r="C97" s="173" t="s">
-        <v>567</v>
-      </c>
-      <c r="D97" s="81" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="80" t="s">
-        <v>357</v>
-      </c>
-      <c r="B98" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="C98" s="81" t="s">
-        <v>78</v>
-      </c>
-      <c r="D98" s="81" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="80" t="s">
         <v>357</v>
       </c>
-      <c r="B99" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="C99" s="81" t="s">
-        <v>351</v>
+      <c r="B99" s="174" t="s">
+        <v>566</v>
+      </c>
+      <c r="C99" s="173" t="s">
+        <v>567</v>
       </c>
       <c r="D99" s="81" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" s="4" customFormat="1" ht="30">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" s="80" t="s">
         <v>357</v>
       </c>
-      <c r="B100" s="112" t="s">
+      <c r="B100" s="82" t="s">
         <v>79</v>
       </c>
-      <c r="C100" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="D100" s="9" t="s">
-        <v>392</v>
+      <c r="C100" s="81" t="s">
+        <v>78</v>
+      </c>
+      <c r="D100" s="81" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="80" t="s">
         <v>357</v>
       </c>
-      <c r="B101" s="110" t="s">
-        <v>380</v>
-      </c>
-      <c r="C101" s="98" t="s">
-        <v>381</v>
-      </c>
-      <c r="D101" s="111" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
+      <c r="B101" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="C101" s="81" t="s">
+        <v>351</v>
+      </c>
+      <c r="D101" s="81" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" s="4" customFormat="1" ht="30">
       <c r="A102" s="80" t="s">
         <v>357</v>
       </c>
-      <c r="B102" s="110" t="s">
+      <c r="B102" s="112" t="s">
+        <v>79</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="D102" s="9" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="80" t="s">
+        <v>357</v>
+      </c>
+      <c r="B103" s="110" t="s">
         <v>380</v>
       </c>
-      <c r="C102" s="98" t="s">
+      <c r="C103" s="98" t="s">
+        <v>381</v>
+      </c>
+      <c r="D103" s="111" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="80" t="s">
+        <v>357</v>
+      </c>
+      <c r="B104" s="110" t="s">
+        <v>380</v>
+      </c>
+      <c r="C104" s="98" t="s">
         <v>383</v>
       </c>
-      <c r="D102" s="111" t="s">
+      <c r="D104" s="111" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="114" t="s">
-        <v>486</v>
-      </c>
-      <c r="B103" s="113" t="s">
-        <v>40</v>
-      </c>
-      <c r="C103" s="115" t="s">
-        <v>37</v>
-      </c>
-      <c r="D103" s="115" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" s="3" customFormat="1">
-      <c r="A104" s="114" t="s">
-        <v>486</v>
-      </c>
-      <c r="B104" s="145" t="s">
-        <v>269</v>
-      </c>
-      <c r="C104" s="116" t="s">
-        <v>263</v>
-      </c>
-      <c r="D104" s="117" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" s="3" customFormat="1">
+    <row r="105" spans="1:4">
       <c r="A105" s="114" t="s">
         <v>486</v>
       </c>
-      <c r="B105" s="145" t="s">
-        <v>269</v>
-      </c>
-      <c r="C105" s="116" t="s">
-        <v>264</v>
-      </c>
-      <c r="D105" s="117" t="s">
-        <v>262</v>
+      <c r="B105" s="113" t="s">
+        <v>40</v>
+      </c>
+      <c r="C105" s="115" t="s">
+        <v>37</v>
+      </c>
+      <c r="D105" s="115" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="106" spans="1:4" s="3" customFormat="1">
@@ -11379,13 +11422,13 @@
         <v>486</v>
       </c>
       <c r="B106" s="145" t="s">
-        <v>256</v>
-      </c>
-      <c r="C106" s="118" t="s">
-        <v>258</v>
+        <v>269</v>
+      </c>
+      <c r="C106" s="116" t="s">
+        <v>263</v>
       </c>
       <c r="D106" s="117" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="107" spans="1:4" s="3" customFormat="1">
@@ -11393,13 +11436,13 @@
         <v>486</v>
       </c>
       <c r="B107" s="145" t="s">
-        <v>266</v>
-      </c>
-      <c r="C107" s="118" t="s">
-        <v>265</v>
+        <v>269</v>
+      </c>
+      <c r="C107" s="116" t="s">
+        <v>264</v>
       </c>
       <c r="D107" s="117" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="108" spans="1:4" s="3" customFormat="1">
@@ -11407,55 +11450,55 @@
         <v>486</v>
       </c>
       <c r="B108" s="145" t="s">
+        <v>256</v>
+      </c>
+      <c r="C108" s="118" t="s">
+        <v>258</v>
+      </c>
+      <c r="D108" s="117" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" s="3" customFormat="1">
+      <c r="A109" s="114" t="s">
+        <v>486</v>
+      </c>
+      <c r="B109" s="145" t="s">
         <v>266</v>
       </c>
-      <c r="C108" s="118" t="s">
+      <c r="C109" s="118" t="s">
+        <v>265</v>
+      </c>
+      <c r="D109" s="117" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" s="3" customFormat="1">
+      <c r="A110" s="114" t="s">
+        <v>486</v>
+      </c>
+      <c r="B110" s="145" t="s">
+        <v>266</v>
+      </c>
+      <c r="C110" s="118" t="s">
         <v>259</v>
       </c>
-      <c r="D108" s="117" t="s">
+      <c r="D110" s="117" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="109" spans="1:4" s="4" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A109" s="119" t="s">
-        <v>493</v>
-      </c>
-      <c r="B109" s="120" t="s">
-        <v>220</v>
-      </c>
-      <c r="C109" s="121" t="s">
-        <v>485</v>
-      </c>
-      <c r="D109" s="122" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4">
-      <c r="A110" s="119" t="s">
-        <v>493</v>
-      </c>
-      <c r="B110" s="35" t="s">
-        <v>147</v>
-      </c>
-      <c r="C110" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="D110" s="36" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" s="4" customFormat="1" ht="39.75" customHeight="1">
       <c r="A111" s="119" t="s">
         <v>493</v>
       </c>
-      <c r="B111" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="C111" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="D111" s="36" t="s">
-        <v>111</v>
+      <c r="B111" s="120" t="s">
+        <v>220</v>
+      </c>
+      <c r="C111" s="121" t="s">
+        <v>485</v>
+      </c>
+      <c r="D111" s="122" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -11463,13 +11506,13 @@
         <v>493</v>
       </c>
       <c r="B112" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C112" s="36" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D112" s="36" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -11477,111 +11520,107 @@
         <v>493</v>
       </c>
       <c r="B113" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="C113" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="D113" s="36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="119" t="s">
+        <v>493</v>
+      </c>
+      <c r="B114" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="C114" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D114" s="36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="119" t="s">
+        <v>493</v>
+      </c>
+      <c r="B115" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="C113" s="36" t="s">
+      <c r="C115" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="D113" s="36" t="s">
+      <c r="D115" s="36" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15.75">
-      <c r="A114" s="167" t="s">
+    <row r="116" spans="1:4" ht="15.75">
+      <c r="A116" s="167" t="s">
         <v>497</v>
       </c>
-      <c r="B114" s="167" t="s">
+      <c r="B116" s="167" t="s">
         <v>215</v>
       </c>
-      <c r="C114" s="171" t="s">
+      <c r="C116" s="171" t="s">
         <v>563</v>
       </c>
-      <c r="D114" s="168" t="s">
+      <c r="D116" s="168" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="30">
-      <c r="A115" s="169" t="s">
+    <row r="117" spans="1:4" ht="30">
+      <c r="A117" s="169" t="s">
         <v>497</v>
       </c>
-      <c r="B115" s="169" t="s">
+      <c r="B117" s="169" t="s">
         <v>215</v>
       </c>
-      <c r="C115" s="172" t="s">
+      <c r="C117" s="172" t="s">
         <v>564</v>
       </c>
-      <c r="D115" s="170" t="s">
+      <c r="D117" s="170" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="31.5">
-      <c r="A116" s="169" t="s">
+    <row r="118" spans="1:4" ht="31.5">
+      <c r="A118" s="169"/>
+      <c r="B118" s="169"/>
+      <c r="C118" s="172" t="s">
+        <v>639</v>
+      </c>
+      <c r="D118" s="170" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="31.5">
+      <c r="A119" s="169" t="s">
         <v>497</v>
       </c>
-      <c r="B116" s="169" t="s">
+      <c r="B119" s="169" t="s">
         <v>215</v>
       </c>
-      <c r="C116" s="172" t="s">
+      <c r="C119" s="172" t="s">
         <v>608</v>
       </c>
-      <c r="D116" s="170" t="s">
+      <c r="D119" s="170" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="117" spans="1:4" s="3" customFormat="1">
-      <c r="A117" s="152" t="s">
+    <row r="120" spans="1:4" s="3" customFormat="1">
+      <c r="A120" s="152" t="s">
         <v>39</v>
       </c>
-      <c r="B117" s="153" t="s">
+      <c r="B120" s="153" t="s">
         <v>242</v>
       </c>
-      <c r="C117" s="154" t="s">
+      <c r="C120" s="154" t="s">
         <v>244</v>
       </c>
-      <c r="D117" s="155" t="s">
+      <c r="D120" s="155" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="A118" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="B118" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="C118" s="61" t="s">
-        <v>42</v>
-      </c>
-      <c r="D118" s="61" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4">
-      <c r="A119" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="B119" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="C119" s="61" t="s">
-        <v>275</v>
-      </c>
-      <c r="D119" s="61" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="A120" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="B120" s="71" t="s">
-        <v>21</v>
-      </c>
-      <c r="C120" s="61" t="s">
-        <v>23</v>
-      </c>
-      <c r="D120" s="61" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -11589,13 +11628,13 @@
         <v>1</v>
       </c>
       <c r="B121" s="71" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C121" s="61" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D121" s="61" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -11603,13 +11642,13 @@
         <v>1</v>
       </c>
       <c r="B122" s="71" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C122" s="61" t="s">
-        <v>46</v>
+        <v>275</v>
       </c>
       <c r="D122" s="61" t="s">
-        <v>48</v>
+        <v>274</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -11617,13 +11656,13 @@
         <v>1</v>
       </c>
       <c r="B123" s="71" t="s">
-        <v>298</v>
+        <v>21</v>
       </c>
       <c r="C123" s="61" t="s">
-        <v>294</v>
+        <v>23</v>
       </c>
       <c r="D123" s="61" t="s">
-        <v>299</v>
+        <v>22</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -11631,13 +11670,13 @@
         <v>1</v>
       </c>
       <c r="B124" s="71" t="s">
-        <v>295</v>
+        <v>24</v>
       </c>
       <c r="C124" s="61" t="s">
-        <v>183</v>
+        <v>25</v>
       </c>
       <c r="D124" s="61" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -11645,13 +11684,13 @@
         <v>1</v>
       </c>
       <c r="B125" s="71" t="s">
-        <v>295</v>
+        <v>47</v>
       </c>
       <c r="C125" s="61" t="s">
-        <v>104</v>
+        <v>46</v>
       </c>
       <c r="D125" s="61" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -11659,13 +11698,13 @@
         <v>1</v>
       </c>
       <c r="B126" s="71" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C126" s="61" t="s">
-        <v>239</v>
+        <v>294</v>
       </c>
       <c r="D126" s="61" t="s">
-        <v>240</v>
+        <v>299</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -11673,13 +11712,13 @@
         <v>1</v>
       </c>
       <c r="B127" s="71" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C127" s="61" t="s">
-        <v>587</v>
+        <v>183</v>
       </c>
       <c r="D127" s="61" t="s">
-        <v>241</v>
+        <v>102</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -11687,13 +11726,13 @@
         <v>1</v>
       </c>
       <c r="B128" s="71" t="s">
-        <v>87</v>
+        <v>295</v>
       </c>
       <c r="C128" s="61" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="D128" s="61" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -11701,13 +11740,13 @@
         <v>1</v>
       </c>
       <c r="B129" s="71" t="s">
-        <v>31</v>
+        <v>296</v>
       </c>
       <c r="C129" s="61" t="s">
-        <v>29</v>
+        <v>239</v>
       </c>
       <c r="D129" s="61" t="s">
-        <v>30</v>
+        <v>240</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -11715,13 +11754,13 @@
         <v>1</v>
       </c>
       <c r="B130" s="71" t="s">
-        <v>49</v>
+        <v>297</v>
       </c>
       <c r="C130" s="61" t="s">
-        <v>50</v>
+        <v>587</v>
       </c>
       <c r="D130" s="61" t="s">
-        <v>51</v>
+        <v>241</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -11729,13 +11768,13 @@
         <v>1</v>
       </c>
       <c r="B131" s="71" t="s">
-        <v>280</v>
-      </c>
-      <c r="C131" s="83" t="s">
-        <v>281</v>
-      </c>
-      <c r="D131" s="83" t="s">
-        <v>282</v>
+        <v>87</v>
+      </c>
+      <c r="C131" s="61" t="s">
+        <v>85</v>
+      </c>
+      <c r="D131" s="61" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -11743,13 +11782,13 @@
         <v>1</v>
       </c>
       <c r="B132" s="71" t="s">
-        <v>499</v>
+        <v>31</v>
       </c>
       <c r="C132" s="61" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="D132" s="61" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -11757,13 +11796,13 @@
         <v>1</v>
       </c>
       <c r="B133" s="71" t="s">
-        <v>500</v>
+        <v>49</v>
       </c>
       <c r="C133" s="61" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="D133" s="61" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -11771,13 +11810,13 @@
         <v>1</v>
       </c>
       <c r="B134" s="71" t="s">
-        <v>500</v>
-      </c>
-      <c r="C134" s="61" t="s">
-        <v>167</v>
-      </c>
-      <c r="D134" s="61" t="s">
-        <v>166</v>
+        <v>280</v>
+      </c>
+      <c r="C134" s="83" t="s">
+        <v>281</v>
+      </c>
+      <c r="D134" s="83" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -11785,13 +11824,13 @@
         <v>1</v>
       </c>
       <c r="B135" s="71" t="s">
-        <v>76</v>
+        <v>499</v>
       </c>
       <c r="C135" s="61" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D135" s="61" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -11799,13 +11838,13 @@
         <v>1</v>
       </c>
       <c r="B136" s="71" t="s">
-        <v>76</v>
+        <v>500</v>
       </c>
       <c r="C136" s="61" t="s">
-        <v>164</v>
+        <v>73</v>
       </c>
       <c r="D136" s="61" t="s">
-        <v>165</v>
+        <v>74</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -11813,13 +11852,13 @@
         <v>1</v>
       </c>
       <c r="B137" s="71" t="s">
-        <v>76</v>
+        <v>500</v>
       </c>
       <c r="C137" s="61" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D137" s="61" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -11829,11 +11868,11 @@
       <c r="B138" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="C138" s="84" t="s">
-        <v>562</v>
+      <c r="C138" s="61" t="s">
+        <v>75</v>
       </c>
       <c r="D138" s="61" t="s">
-        <v>238</v>
+        <v>77</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -11841,13 +11880,13 @@
         <v>1</v>
       </c>
       <c r="B139" s="71" t="s">
-        <v>170</v>
+        <v>76</v>
       </c>
       <c r="C139" s="61" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D139" s="61" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -11855,13 +11894,13 @@
         <v>1</v>
       </c>
       <c r="B140" s="71" t="s">
-        <v>174</v>
+        <v>76</v>
       </c>
       <c r="C140" s="61" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D140" s="61" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -11869,13 +11908,13 @@
         <v>1</v>
       </c>
       <c r="B141" s="71" t="s">
-        <v>218</v>
-      </c>
-      <c r="C141" s="61" t="s">
-        <v>217</v>
+        <v>76</v>
+      </c>
+      <c r="C141" s="84" t="s">
+        <v>562</v>
       </c>
       <c r="D141" s="61" t="s">
-        <v>219</v>
+        <v>238</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -11883,13 +11922,13 @@
         <v>1</v>
       </c>
       <c r="B142" s="71" t="s">
-        <v>227</v>
-      </c>
-      <c r="C142" s="85" t="s">
-        <v>228</v>
+        <v>170</v>
+      </c>
+      <c r="C142" s="61" t="s">
+        <v>172</v>
       </c>
       <c r="D142" s="61" t="s">
-        <v>226</v>
+        <v>171</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -11897,13 +11936,13 @@
         <v>1</v>
       </c>
       <c r="B143" s="71" t="s">
-        <v>233</v>
-      </c>
-      <c r="C143" s="85" t="s">
-        <v>365</v>
+        <v>174</v>
+      </c>
+      <c r="C143" s="61" t="s">
+        <v>173</v>
       </c>
       <c r="D143" s="61" t="s">
-        <v>234</v>
+        <v>175</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -11911,13 +11950,13 @@
         <v>1</v>
       </c>
       <c r="B144" s="71" t="s">
-        <v>235</v>
-      </c>
-      <c r="C144" s="85" t="s">
-        <v>363</v>
+        <v>218</v>
+      </c>
+      <c r="C144" s="61" t="s">
+        <v>217</v>
       </c>
       <c r="D144" s="61" t="s">
-        <v>364</v>
+        <v>219</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -11925,55 +11964,55 @@
         <v>1</v>
       </c>
       <c r="B145" s="71" t="s">
+        <v>227</v>
+      </c>
+      <c r="C145" s="85" t="s">
+        <v>228</v>
+      </c>
+      <c r="D145" s="61" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B146" s="71" t="s">
+        <v>233</v>
+      </c>
+      <c r="C146" s="85" t="s">
+        <v>365</v>
+      </c>
+      <c r="D146" s="61" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B147" s="71" t="s">
         <v>235</v>
       </c>
-      <c r="C145" s="85" t="s">
+      <c r="C147" s="85" t="s">
+        <v>363</v>
+      </c>
+      <c r="D147" s="61" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B148" s="71" t="s">
+        <v>235</v>
+      </c>
+      <c r="C148" s="85" t="s">
         <v>236</v>
       </c>
-      <c r="D145" s="61" t="s">
+      <c r="D148" s="61" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4">
-      <c r="A146" s="80" t="s">
-        <v>80</v>
-      </c>
-      <c r="B146" s="82" t="s">
-        <v>106</v>
-      </c>
-      <c r="C146" s="81" t="s">
-        <v>107</v>
-      </c>
-      <c r="D146" s="81" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4">
-      <c r="A147" s="80" t="s">
-        <v>80</v>
-      </c>
-      <c r="B147" s="82" t="s">
-        <v>181</v>
-      </c>
-      <c r="C147" s="81" t="s">
-        <v>99</v>
-      </c>
-      <c r="D147" s="81" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4">
-      <c r="A148" s="80" t="s">
-        <v>80</v>
-      </c>
-      <c r="B148" s="82" t="s">
-        <v>182</v>
-      </c>
-      <c r="C148" s="81" t="s">
-        <v>288</v>
-      </c>
-      <c r="D148" s="81" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -11981,13 +12020,13 @@
         <v>80</v>
       </c>
       <c r="B149" s="82" t="s">
-        <v>421</v>
+        <v>106</v>
       </c>
       <c r="C149" s="81" t="s">
-        <v>422</v>
+        <v>107</v>
       </c>
       <c r="D149" s="81" t="s">
-        <v>420</v>
+        <v>105</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -11995,13 +12034,13 @@
         <v>80</v>
       </c>
       <c r="B150" s="82" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="C150" s="81" t="s">
-        <v>198</v>
+        <v>99</v>
       </c>
       <c r="D150" s="81" t="s">
-        <v>200</v>
+        <v>98</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -12009,13 +12048,13 @@
         <v>80</v>
       </c>
       <c r="B151" s="82" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="C151" s="81" t="s">
-        <v>201</v>
+        <v>288</v>
       </c>
       <c r="D151" s="81" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -12023,13 +12062,13 @@
         <v>80</v>
       </c>
       <c r="B152" s="82" t="s">
-        <v>199</v>
+        <v>421</v>
       </c>
       <c r="C152" s="81" t="s">
-        <v>202</v>
+        <v>422</v>
       </c>
       <c r="D152" s="81" t="s">
-        <v>204</v>
+        <v>420</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -12037,27 +12076,27 @@
         <v>80</v>
       </c>
       <c r="B153" s="82" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C153" s="81" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D153" s="81" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" ht="15.75">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
       <c r="A154" s="80" t="s">
         <v>80</v>
       </c>
       <c r="B154" s="82" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C154" s="81" t="s">
-        <v>576</v>
-      </c>
-      <c r="D154" s="177" t="s">
-        <v>577</v>
+        <v>201</v>
+      </c>
+      <c r="D154" s="81" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -12065,69 +12104,69 @@
         <v>80</v>
       </c>
       <c r="B155" s="82" t="s">
-        <v>580</v>
+        <v>199</v>
       </c>
       <c r="C155" s="81" t="s">
-        <v>578</v>
-      </c>
-      <c r="D155" s="178" t="s">
-        <v>579</v>
+        <v>202</v>
+      </c>
+      <c r="D155" s="81" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="B156" s="130" t="s">
+      <c r="B156" s="82" t="s">
         <v>205</v>
       </c>
-      <c r="C156" s="131" t="s">
+      <c r="C156" s="81" t="s">
+        <v>197</v>
+      </c>
+      <c r="D156" s="81" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="15.75">
+      <c r="A157" s="80" t="s">
+        <v>80</v>
+      </c>
+      <c r="B157" s="82" t="s">
+        <v>205</v>
+      </c>
+      <c r="C157" s="81" t="s">
+        <v>576</v>
+      </c>
+      <c r="D157" s="177" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="80" t="s">
+        <v>80</v>
+      </c>
+      <c r="B158" s="82" t="s">
+        <v>580</v>
+      </c>
+      <c r="C158" s="81" t="s">
+        <v>578</v>
+      </c>
+      <c r="D158" s="178" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="80" t="s">
+        <v>80</v>
+      </c>
+      <c r="B159" s="130" t="s">
+        <v>205</v>
+      </c>
+      <c r="C159" s="131" t="s">
         <v>207</v>
       </c>
-      <c r="D156" s="131" t="s">
+      <c r="D159" s="131" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4">
-      <c r="A157" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="B157" s="70" t="s">
-        <v>506</v>
-      </c>
-      <c r="C157" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="D157" s="69" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4">
-      <c r="A158" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="B158" s="70" t="s">
-        <v>506</v>
-      </c>
-      <c r="C158" s="69" t="s">
-        <v>509</v>
-      </c>
-      <c r="D158" s="69" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4">
-      <c r="A159" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="B159" s="70" t="s">
-        <v>506</v>
-      </c>
-      <c r="C159" s="69" t="s">
-        <v>516</v>
-      </c>
-      <c r="D159" s="69" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -12135,13 +12174,13 @@
         <v>8</v>
       </c>
       <c r="B160" s="70" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="C160" s="69" t="s">
-        <v>510</v>
+        <v>66</v>
       </c>
       <c r="D160" s="69" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -12149,13 +12188,13 @@
         <v>8</v>
       </c>
       <c r="B161" s="70" t="s">
-        <v>447</v>
+        <v>506</v>
       </c>
       <c r="C161" s="69" t="s">
-        <v>287</v>
+        <v>509</v>
       </c>
       <c r="D161" s="69" t="s">
-        <v>443</v>
+        <v>508</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -12163,13 +12202,13 @@
         <v>8</v>
       </c>
       <c r="B162" s="70" t="s">
-        <v>447</v>
+        <v>506</v>
       </c>
       <c r="C162" s="69" t="s">
-        <v>448</v>
+        <v>516</v>
       </c>
       <c r="D162" s="69" t="s">
-        <v>446</v>
+        <v>515</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -12177,13 +12216,13 @@
         <v>8</v>
       </c>
       <c r="B163" s="70" t="s">
-        <v>289</v>
+        <v>513</v>
       </c>
       <c r="C163" s="69" t="s">
-        <v>290</v>
+        <v>510</v>
       </c>
       <c r="D163" s="69" t="s">
-        <v>291</v>
+        <v>511</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -12191,13 +12230,13 @@
         <v>8</v>
       </c>
       <c r="B164" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C164" s="68" t="s">
-        <v>9</v>
+        <v>447</v>
+      </c>
+      <c r="C164" s="69" t="s">
+        <v>287</v>
       </c>
       <c r="D164" s="69" t="s">
-        <v>11</v>
+        <v>443</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -12205,13 +12244,13 @@
         <v>8</v>
       </c>
       <c r="B165" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C165" s="68" t="s">
-        <v>20</v>
+        <v>447</v>
+      </c>
+      <c r="C165" s="69" t="s">
+        <v>448</v>
       </c>
       <c r="D165" s="69" t="s">
-        <v>65</v>
+        <v>446</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -12219,13 +12258,13 @@
         <v>8</v>
       </c>
       <c r="B166" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C166" s="68" t="s">
-        <v>390</v>
+        <v>289</v>
+      </c>
+      <c r="C166" s="69" t="s">
+        <v>290</v>
       </c>
       <c r="D166" s="69" t="s">
-        <v>391</v>
+        <v>291</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -12250,10 +12289,10 @@
         <v>8</v>
       </c>
       <c r="C168" s="68" t="s">
-        <v>359</v>
+        <v>20</v>
       </c>
       <c r="D168" s="69" t="s">
-        <v>360</v>
+        <v>65</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -12264,10 +12303,10 @@
         <v>8</v>
       </c>
       <c r="C169" s="68" t="s">
-        <v>361</v>
+        <v>390</v>
       </c>
       <c r="D169" s="69" t="s">
-        <v>362</v>
+        <v>391</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -12275,13 +12314,13 @@
         <v>8</v>
       </c>
       <c r="B170" s="70" t="s">
-        <v>438</v>
+        <v>8</v>
       </c>
       <c r="C170" s="68" t="s">
-        <v>361</v>
+        <v>9</v>
       </c>
       <c r="D170" s="69" t="s">
-        <v>437</v>
+        <v>11</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -12289,97 +12328,97 @@
         <v>8</v>
       </c>
       <c r="B171" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C171" s="68" t="s">
+        <v>359</v>
+      </c>
+      <c r="D171" s="69" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="B172" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C172" s="68" t="s">
+        <v>361</v>
+      </c>
+      <c r="D172" s="69" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="B173" s="70" t="s">
         <v>438</v>
       </c>
-      <c r="C171" s="68" t="s">
+      <c r="C173" s="68" t="s">
         <v>361</v>
       </c>
-      <c r="D171" s="69" t="s">
+      <c r="D173" s="69" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="B174" s="70" t="s">
+        <v>438</v>
+      </c>
+      <c r="C174" s="68" t="s">
+        <v>361</v>
+      </c>
+      <c r="D174" s="69" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="172" spans="1:4">
-      <c r="A172" s="71" t="s">
+    <row r="175" spans="1:4">
+      <c r="A175" s="71" t="s">
         <v>327</v>
       </c>
-      <c r="B172" s="60" t="s">
+      <c r="B175" s="60" t="s">
         <v>501</v>
       </c>
-      <c r="C172" s="61" t="s">
+      <c r="C175" s="61" t="s">
         <v>176</v>
       </c>
-      <c r="D172" s="61" t="s">
+      <c r="D175" s="61" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="173" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A173" s="71" t="s">
-        <v>327</v>
-      </c>
-      <c r="B173" s="129" t="s">
-        <v>432</v>
-      </c>
-      <c r="C173" s="12" t="s">
-        <v>423</v>
-      </c>
-      <c r="D173" s="12" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" s="3" customFormat="1" ht="30">
-      <c r="A174" s="71" t="s">
-        <v>327</v>
-      </c>
-      <c r="B174" s="129" t="s">
-        <v>432</v>
-      </c>
-      <c r="C174" s="12" t="s">
-        <v>444</v>
-      </c>
-      <c r="D174" s="12" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A175" s="72" t="s">
-        <v>327</v>
-      </c>
-      <c r="B175" s="129" t="s">
-        <v>432</v>
-      </c>
-      <c r="C175" s="62" t="s">
-        <v>349</v>
-      </c>
-      <c r="D175" s="12" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A176" s="72" t="s">
+    <row r="176" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A176" s="71" t="s">
         <v>327</v>
       </c>
       <c r="B176" s="129" t="s">
         <v>432</v>
       </c>
-      <c r="C176" s="62" t="s">
-        <v>424</v>
+      <c r="C176" s="12" t="s">
+        <v>423</v>
       </c>
       <c r="D176" s="12" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" s="3" customFormat="1" ht="76.5" customHeight="1">
-      <c r="A177" s="72" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" s="3" customFormat="1" ht="30">
+      <c r="A177" s="71" t="s">
         <v>327</v>
       </c>
       <c r="B177" s="129" t="s">
-        <v>502</v>
+        <v>432</v>
       </c>
       <c r="C177" s="12" t="s">
-        <v>330</v>
+        <v>444</v>
       </c>
       <c r="D177" s="12" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="178" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
@@ -12387,13 +12426,13 @@
         <v>327</v>
       </c>
       <c r="B178" s="129" t="s">
-        <v>503</v>
-      </c>
-      <c r="C178" s="12" t="s">
-        <v>331</v>
+        <v>432</v>
+      </c>
+      <c r="C178" s="62" t="s">
+        <v>349</v>
       </c>
       <c r="D178" s="12" t="s">
-        <v>431</v>
+        <v>348</v>
       </c>
     </row>
     <row r="179" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
@@ -12401,55 +12440,55 @@
         <v>327</v>
       </c>
       <c r="B179" s="129" t="s">
-        <v>426</v>
-      </c>
-      <c r="C179" s="12" t="s">
-        <v>427</v>
+        <v>432</v>
+      </c>
+      <c r="C179" s="62" t="s">
+        <v>424</v>
       </c>
       <c r="D179" s="12" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="180" spans="1:4">
-      <c r="A180" s="74" t="s">
-        <v>187</v>
-      </c>
-      <c r="B180" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="C180" s="11" t="s">
-        <v>328</v>
-      </c>
-      <c r="D180" s="11" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" s="4" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A181" s="74" t="s">
-        <v>187</v>
-      </c>
-      <c r="B181" s="63" t="s">
-        <v>318</v>
-      </c>
-      <c r="C181" s="64" t="s">
-        <v>428</v>
-      </c>
-      <c r="D181" s="65" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4">
-      <c r="A182" s="74" t="s">
-        <v>187</v>
-      </c>
-      <c r="B182" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="C182" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="D182" s="11" t="s">
-        <v>320</v>
+    <row r="180" spans="1:4" s="3" customFormat="1" ht="76.5" customHeight="1">
+      <c r="A180" s="72" t="s">
+        <v>327</v>
+      </c>
+      <c r="B180" s="129" t="s">
+        <v>502</v>
+      </c>
+      <c r="C180" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="D180" s="12" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
+      <c r="A181" s="72" t="s">
+        <v>327</v>
+      </c>
+      <c r="B181" s="129" t="s">
+        <v>503</v>
+      </c>
+      <c r="C181" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="D181" s="12" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
+      <c r="A182" s="72" t="s">
+        <v>327</v>
+      </c>
+      <c r="B182" s="129" t="s">
+        <v>426</v>
+      </c>
+      <c r="C182" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="D182" s="12" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -12460,318 +12499,318 @@
         <v>318</v>
       </c>
       <c r="C183" s="11" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="D183" s="11" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" s="4" customFormat="1">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" s="4" customFormat="1" ht="39.75" customHeight="1">
       <c r="A184" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="B184" s="73" t="s">
+      <c r="B184" s="63" t="s">
+        <v>318</v>
+      </c>
+      <c r="C184" s="64" t="s">
+        <v>428</v>
+      </c>
+      <c r="D184" s="65" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185" s="74" t="s">
+        <v>187</v>
+      </c>
+      <c r="B185" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="C185" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="D185" s="11" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186" s="74" t="s">
+        <v>187</v>
+      </c>
+      <c r="B186" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="C186" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="D186" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" s="4" customFormat="1">
+      <c r="A187" s="74" t="s">
+        <v>187</v>
+      </c>
+      <c r="B187" s="73" t="s">
         <v>313</v>
       </c>
-      <c r="C184" s="65" t="s">
+      <c r="C187" s="65" t="s">
         <v>312</v>
       </c>
-      <c r="D184" s="65" t="s">
+      <c r="D187" s="65" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="185" spans="1:4">
-      <c r="A185" s="75" t="s">
+    <row r="188" spans="1:4">
+      <c r="A188" s="75" t="s">
         <v>187</v>
       </c>
-      <c r="B185" s="10" t="s">
+      <c r="B188" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="C185" s="11" t="s">
+      <c r="C188" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="D185" s="65" t="s">
+      <c r="D188" s="65" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="186" spans="1:4">
-      <c r="A186" s="113" t="s">
+    <row r="189" spans="1:4">
+      <c r="A189" s="113" t="s">
         <v>191</v>
       </c>
-      <c r="B186" s="113" t="s">
+      <c r="B189" s="113" t="s">
         <v>189</v>
       </c>
-      <c r="C186" s="115" t="s">
+      <c r="C189" s="115" t="s">
         <v>193</v>
       </c>
-      <c r="D186" s="115" t="s">
+      <c r="D189" s="115" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="187" spans="1:4">
-      <c r="A187" s="113" t="s">
+    <row r="190" spans="1:4">
+      <c r="A190" s="113" t="s">
         <v>191</v>
       </c>
-      <c r="B187" s="113" t="s">
+      <c r="B190" s="113" t="s">
         <v>189</v>
       </c>
-      <c r="C187" s="115" t="s">
+      <c r="C190" s="115" t="s">
         <v>195</v>
       </c>
-      <c r="D187" s="115" t="s">
+      <c r="D190" s="115" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="188" spans="1:4" s="3" customFormat="1">
-      <c r="A188" s="132" t="s">
+    <row r="191" spans="1:4" s="3" customFormat="1">
+      <c r="A191" s="132" t="s">
         <v>250</v>
       </c>
-      <c r="B188" s="157" t="s">
+      <c r="B191" s="157" t="s">
         <v>252</v>
       </c>
-      <c r="C188" s="133" t="s">
+      <c r="C191" s="133" t="s">
         <v>253</v>
       </c>
-      <c r="D188" s="134" t="s">
+      <c r="D191" s="134" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="189" spans="1:4" s="86" customFormat="1">
-      <c r="A189" s="132" t="s">
+    <row r="192" spans="1:4" s="86" customFormat="1">
+      <c r="A192" s="132" t="s">
         <v>250</v>
       </c>
-      <c r="B189" s="157" t="s">
+      <c r="B192" s="157" t="s">
         <v>293</v>
       </c>
-      <c r="C189" s="133" t="s">
+      <c r="C192" s="133" t="s">
         <v>292</v>
       </c>
-      <c r="D189" s="134" t="s">
+      <c r="D192" s="134" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="190" spans="1:4" s="86" customFormat="1">
-      <c r="A190" s="132" t="s">
+    <row r="193" spans="1:4" s="86" customFormat="1">
+      <c r="A193" s="132" t="s">
         <v>250</v>
       </c>
-      <c r="B190" s="157" t="s">
+      <c r="B193" s="157" t="s">
         <v>286</v>
       </c>
-      <c r="C190" s="133" t="s">
+      <c r="C193" s="133" t="s">
         <v>285</v>
       </c>
-      <c r="D190" s="134" t="s">
+      <c r="D193" s="134" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="191" spans="1:4" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A191" s="135" t="s">
+    <row r="194" spans="1:4" s="4" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A194" s="135" t="s">
         <v>250</v>
       </c>
-      <c r="B191" s="157" t="s">
+      <c r="B194" s="157" t="s">
         <v>463</v>
       </c>
-      <c r="C191" s="136" t="s">
+      <c r="C194" s="136" t="s">
         <v>376</v>
       </c>
-      <c r="D191" s="137" t="s">
+      <c r="D194" s="137" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="192" spans="1:4" s="38" customFormat="1" ht="144.75" customHeight="1">
-      <c r="A192" s="138" t="s">
-        <v>250</v>
-      </c>
-      <c r="B192" s="158" t="s">
-        <v>504</v>
-      </c>
-      <c r="C192" s="136" t="s">
-        <v>488</v>
-      </c>
-      <c r="D192" s="137" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4">
-      <c r="A193" s="159" t="s">
-        <v>250</v>
-      </c>
-      <c r="B193" s="160" t="s">
-        <v>512</v>
-      </c>
-      <c r="C193" s="161" t="s">
-        <v>514</v>
-      </c>
-      <c r="D193" s="161" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" s="38" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A194" s="138" t="s">
-        <v>250</v>
-      </c>
-      <c r="B194" s="158" t="s">
-        <v>435</v>
-      </c>
-      <c r="C194" s="139" t="s">
-        <v>458</v>
-      </c>
-      <c r="D194" s="137" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" s="38" customFormat="1" ht="28.5" customHeight="1">
+    <row r="195" spans="1:4" s="38" customFormat="1" ht="144.75" customHeight="1">
       <c r="A195" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B195" s="158" t="s">
-        <v>435</v>
-      </c>
-      <c r="C195" s="139" t="s">
-        <v>459</v>
+        <v>504</v>
+      </c>
+      <c r="C195" s="136" t="s">
+        <v>488</v>
       </c>
       <c r="D195" s="137" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" s="38" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A196" s="138" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" s="159" t="s">
         <v>250</v>
       </c>
-      <c r="B196" s="158" t="s">
-        <v>436</v>
-      </c>
-      <c r="C196" s="140" t="s">
-        <v>441</v>
-      </c>
-      <c r="D196" s="137" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" s="4" customFormat="1" ht="38.25" customHeight="1">
+      <c r="B196" s="160" t="s">
+        <v>512</v>
+      </c>
+      <c r="C196" s="161" t="s">
+        <v>514</v>
+      </c>
+      <c r="D196" s="161" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" s="38" customFormat="1" ht="28.5" customHeight="1">
       <c r="A197" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B197" s="158" t="s">
-        <v>242</v>
-      </c>
-      <c r="C197" s="136" t="s">
-        <v>457</v>
+        <v>435</v>
+      </c>
+      <c r="C197" s="139" t="s">
+        <v>458</v>
       </c>
       <c r="D197" s="137" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" s="38" customFormat="1" ht="28.5" customHeight="1">
       <c r="A198" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B198" s="158" t="s">
-        <v>440</v>
-      </c>
-      <c r="C198" s="136" t="s">
-        <v>517</v>
+        <v>435</v>
+      </c>
+      <c r="C198" s="139" t="s">
+        <v>459</v>
       </c>
       <c r="D198" s="137" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" s="38" customFormat="1" ht="28.5" customHeight="1">
       <c r="A199" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B199" s="158" t="s">
-        <v>455</v>
-      </c>
-      <c r="C199" s="136" t="s">
-        <v>456</v>
+        <v>436</v>
+      </c>
+      <c r="C199" s="140" t="s">
+        <v>441</v>
       </c>
       <c r="D199" s="137" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" s="4" customFormat="1" ht="38.25" customHeight="1">
       <c r="A200" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B200" s="158" t="s">
-        <v>522</v>
+        <v>242</v>
       </c>
       <c r="C200" s="136" t="s">
-        <v>521</v>
+        <v>457</v>
       </c>
       <c r="D200" s="137" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1">
       <c r="A201" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B201" s="158" t="s">
-        <v>520</v>
+        <v>440</v>
       </c>
       <c r="C201" s="136" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D201" s="137" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
       <c r="A202" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B202" s="158" t="s">
+        <v>455</v>
+      </c>
+      <c r="C202" s="136" t="s">
+        <v>456</v>
+      </c>
+      <c r="D202" s="137" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
+      <c r="A203" s="138" t="s">
+        <v>250</v>
+      </c>
+      <c r="B203" s="158" t="s">
+        <v>522</v>
+      </c>
+      <c r="C203" s="136" t="s">
+        <v>521</v>
+      </c>
+      <c r="D203" s="137" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
+      <c r="A204" s="138" t="s">
+        <v>250</v>
+      </c>
+      <c r="B204" s="158" t="s">
+        <v>520</v>
+      </c>
+      <c r="C204" s="136" t="s">
+        <v>519</v>
+      </c>
+      <c r="D204" s="137" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="A205" s="138" t="s">
+        <v>250</v>
+      </c>
+      <c r="B205" s="158" t="s">
         <v>454</v>
       </c>
-      <c r="C202" s="136" t="s">
+      <c r="C205" s="136" t="s">
         <v>452</v>
       </c>
-      <c r="D202" s="137" t="s">
+      <c r="D205" s="137" t="s">
         <v>453</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4">
-      <c r="A203" s="123" t="s">
-        <v>222</v>
-      </c>
-      <c r="B203" s="123" t="s">
-        <v>223</v>
-      </c>
-      <c r="C203" s="36" t="s">
-        <v>248</v>
-      </c>
-      <c r="D203" s="36" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4">
-      <c r="A204" s="123" t="s">
-        <v>222</v>
-      </c>
-      <c r="B204" s="123" t="s">
-        <v>223</v>
-      </c>
-      <c r="C204" s="36" t="s">
-        <v>225</v>
-      </c>
-      <c r="D204" s="36" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4">
-      <c r="A205" s="123" t="s">
-        <v>222</v>
-      </c>
-      <c r="B205" s="123" t="s">
-        <v>223</v>
-      </c>
-      <c r="C205" s="156" t="s">
-        <v>633</v>
-      </c>
-      <c r="D205" s="36" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -12781,11 +12820,11 @@
       <c r="B206" s="123" t="s">
         <v>223</v>
       </c>
-      <c r="C206" s="156" t="s">
-        <v>306</v>
+      <c r="C206" s="36" t="s">
+        <v>248</v>
       </c>
       <c r="D206" s="36" t="s">
-        <v>302</v>
+        <v>224</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -12793,24 +12832,27 @@
         <v>222</v>
       </c>
       <c r="B207" s="123" t="s">
-        <v>626</v>
-      </c>
-      <c r="C207" s="180" t="s">
-        <v>304</v>
+        <v>223</v>
+      </c>
+      <c r="C207" s="36" t="s">
+        <v>225</v>
       </c>
       <c r="D207" s="36" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
     </row>
     <row r="208" spans="1:4">
+      <c r="A208" s="123" t="s">
+        <v>222</v>
+      </c>
       <c r="B208" s="123" t="s">
-        <v>626</v>
-      </c>
-      <c r="C208" s="180" t="s">
-        <v>304</v>
+        <v>223</v>
+      </c>
+      <c r="C208" s="156" t="s">
+        <v>633</v>
       </c>
       <c r="D208" s="36" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -12818,13 +12860,13 @@
         <v>222</v>
       </c>
       <c r="B209" s="123" t="s">
-        <v>626</v>
-      </c>
-      <c r="C209" s="180" t="s">
-        <v>634</v>
+        <v>223</v>
+      </c>
+      <c r="C209" s="156" t="s">
+        <v>306</v>
       </c>
       <c r="D209" s="36" t="s">
-        <v>635</v>
+        <v>302</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -12832,83 +12874,80 @@
         <v>222</v>
       </c>
       <c r="B210" s="123" t="s">
+        <v>626</v>
+      </c>
+      <c r="C210" s="180" t="s">
+        <v>304</v>
+      </c>
+      <c r="D210" s="36" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4">
+      <c r="B211" s="123" t="s">
+        <v>626</v>
+      </c>
+      <c r="C211" s="180" t="s">
+        <v>304</v>
+      </c>
+      <c r="D211" s="36" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
+      <c r="A212" s="123" t="s">
+        <v>222</v>
+      </c>
+      <c r="B212" s="123" t="s">
+        <v>626</v>
+      </c>
+      <c r="C212" s="180" t="s">
+        <v>634</v>
+      </c>
+      <c r="D212" s="36" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
+      <c r="A213" s="123" t="s">
+        <v>222</v>
+      </c>
+      <c r="B213" s="123" t="s">
         <v>628</v>
       </c>
-      <c r="C210" s="180" t="s">
+      <c r="C213" s="180" t="s">
         <v>307</v>
       </c>
-      <c r="D210" s="36" t="s">
+      <c r="D213" s="36" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="211" spans="1:4">
-      <c r="A211" s="123" t="s">
+    <row r="214" spans="1:4">
+      <c r="A214" s="123" t="s">
         <v>222</v>
       </c>
-      <c r="B211" s="123" t="s">
+      <c r="B214" s="123" t="s">
         <v>629</v>
       </c>
-      <c r="C211" s="181" t="s">
+      <c r="C214" s="181" t="s">
         <v>393</v>
       </c>
-      <c r="D211" s="36" t="s">
+      <c r="D214" s="36" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="212" spans="1:4" s="179" customFormat="1" ht="15.75">
-      <c r="A212" s="182" t="s">
-        <v>222</v>
-      </c>
-      <c r="B212" s="182" t="s">
-        <v>629</v>
-      </c>
-      <c r="C212" s="183" t="s">
-        <v>583</v>
-      </c>
-      <c r="D212" s="184" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4">
-      <c r="A213" s="182" t="s">
-        <v>222</v>
-      </c>
-      <c r="B213" s="182" t="s">
-        <v>630</v>
-      </c>
-      <c r="C213" s="185" t="s">
-        <v>584</v>
-      </c>
-      <c r="D213" s="186" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4">
-      <c r="A214" s="182" t="s">
-        <v>222</v>
-      </c>
-      <c r="B214" s="182" t="s">
-        <v>631</v>
-      </c>
-      <c r="C214" s="185" t="s">
-        <v>621</v>
-      </c>
-      <c r="D214" s="186" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4">
+    <row r="215" spans="1:4" s="179" customFormat="1" ht="15.75">
       <c r="A215" s="182" t="s">
         <v>222</v>
       </c>
       <c r="B215" s="182" t="s">
-        <v>631</v>
-      </c>
-      <c r="C215" s="185" t="s">
-        <v>622</v>
-      </c>
-      <c r="D215" s="186" t="s">
-        <v>617</v>
+        <v>629</v>
+      </c>
+      <c r="C215" s="183" t="s">
+        <v>583</v>
+      </c>
+      <c r="D215" s="184" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -12916,13 +12955,13 @@
         <v>222</v>
       </c>
       <c r="B216" s="182" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C216" s="185" t="s">
-        <v>623</v>
+        <v>584</v>
       </c>
       <c r="D216" s="186" t="s">
-        <v>618</v>
+        <v>632</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -12933,10 +12972,10 @@
         <v>631</v>
       </c>
       <c r="C217" s="185" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="D217" s="186" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -12947,10 +12986,10 @@
         <v>631</v>
       </c>
       <c r="C218" s="185" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="D218" s="186" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -12958,17 +12997,59 @@
         <v>222</v>
       </c>
       <c r="B219" s="182" t="s">
+        <v>631</v>
+      </c>
+      <c r="C219" s="185" t="s">
+        <v>623</v>
+      </c>
+      <c r="D219" s="186" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4">
+      <c r="A220" s="182" t="s">
+        <v>222</v>
+      </c>
+      <c r="B220" s="182" t="s">
+        <v>631</v>
+      </c>
+      <c r="C220" s="185" t="s">
+        <v>624</v>
+      </c>
+      <c r="D220" s="186" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4">
+      <c r="A221" s="182" t="s">
+        <v>222</v>
+      </c>
+      <c r="B221" s="182" t="s">
+        <v>631</v>
+      </c>
+      <c r="C221" s="185" t="s">
+        <v>625</v>
+      </c>
+      <c r="D221" s="186" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4">
+      <c r="A222" s="182" t="s">
+        <v>222</v>
+      </c>
+      <c r="B222" s="182" t="s">
         <v>223</v>
       </c>
-      <c r="C219" s="185" t="s">
+      <c r="C222" s="185" t="s">
         <v>585</v>
       </c>
-      <c r="D219" s="186" t="s">
+      <c r="D222" s="186" t="s">
         <v>586</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D210" xr:uid="{85ED3410-72EE-453D-8BB3-FB7E07F682B1}"/>
+  <autoFilter ref="A2:D213" xr:uid="{85ED3410-72EE-453D-8BB3-FB7E07F682B1}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Vacunas actualizado 19-08-2020 a 15;22
</commit_message>
<xml_diff>
--- a/Tutoriales/pandas/Comandos Pandas.xlsx
+++ b/Tutoriales/pandas/Comandos Pandas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoseMaría\Documents\CURSOS\data_science\mitrabajo\mi_repositorio\Tutoriales\pandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C286080B-7CBF-4FF5-BDA9-B3E3E37FB40F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297C0154-DC18-4690-B694-71AD3C30DDE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF4018AA-EEB9-4756-B82D-183D37B3B80A}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="CONCEPTOS" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GENERALES!$A$2:$D$213</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GENERALES!$A$2:$D$214</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="646">
   <si>
     <t>FUNCIONES DE PANDAS</t>
   </si>
@@ -6491,6 +6491,12 @@
   </si>
   <si>
     <t>TO_NUMERIC</t>
+  </si>
+  <si>
+    <t>porcentaje_vac.rename(columns={'Vacunaciones 2019_x':'Vacunados 0-59 años','Vacunaciones 2019_y':'Vacunados &gt; 65 años','vacunaciones 2019':'Vacunados 60_64 años' }, inplace=True)</t>
+  </si>
+  <si>
+    <t>Cambia el nombre de las columnas que yo elija</t>
   </si>
 </sst>
 </file>
@@ -7138,7 +7144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="65" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="213">
+  <cellXfs count="215">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7592,6 +7598,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="14" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7633,7 +7642,10 @@
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -9941,10 +9953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265136A6-C067-4B28-9F45-A6266FF6FD67}">
-  <dimension ref="A1:D222"/>
+  <dimension ref="A1:D223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:XFD56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9956,12 +9968,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="33.75" customHeight="1">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="198" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="102" t="s">
@@ -10390,7 +10402,7 @@
       <c r="B32" s="101" t="s">
         <v>643</v>
       </c>
-      <c r="C32" s="212" t="s">
+      <c r="C32" s="197" t="s">
         <v>641</v>
       </c>
       <c r="D32" s="100" t="s">
@@ -10717,32 +10729,32 @@
         <v>345</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="B56" s="71" t="s">
-        <v>480</v>
-      </c>
-      <c r="C56" s="61" t="s">
-        <v>377</v>
-      </c>
-      <c r="D56" s="61" t="s">
-        <v>378</v>
+    <row r="56" spans="1:4" s="4" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A56" s="141" t="s">
+        <v>492</v>
+      </c>
+      <c r="B56" s="214" t="s">
+        <v>347</v>
+      </c>
+      <c r="C56" s="188" t="s">
+        <v>644</v>
+      </c>
+      <c r="D56" s="213" t="s">
+        <v>645</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="60" t="s">
-        <v>478</v>
+        <v>39</v>
       </c>
       <c r="B57" s="71" t="s">
-        <v>475</v>
-      </c>
-      <c r="C57" s="85" t="s">
-        <v>67</v>
-      </c>
-      <c r="D57" s="103" t="s">
-        <v>68</v>
+        <v>480</v>
+      </c>
+      <c r="C57" s="61" t="s">
+        <v>377</v>
+      </c>
+      <c r="D57" s="61" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -10750,13 +10762,13 @@
         <v>478</v>
       </c>
       <c r="B58" s="71" t="s">
-        <v>6</v>
+        <v>475</v>
       </c>
       <c r="C58" s="85" t="s">
-        <v>115</v>
+        <v>67</v>
       </c>
       <c r="D58" s="103" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -10767,10 +10779,10 @@
         <v>6</v>
       </c>
       <c r="C59" s="85" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D59" s="103" t="s">
-        <v>477</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -10781,10 +10793,10 @@
         <v>6</v>
       </c>
       <c r="C60" s="85" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D60" s="103" t="s">
-        <v>134</v>
+        <v>477</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -10795,10 +10807,10 @@
         <v>6</v>
       </c>
       <c r="C61" s="85" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D61" s="103" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -10809,10 +10821,10 @@
         <v>6</v>
       </c>
       <c r="C62" s="85" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D62" s="103" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -10823,10 +10835,10 @@
         <v>6</v>
       </c>
       <c r="C63" s="85" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="D63" s="103" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -10834,13 +10846,13 @@
         <v>478</v>
       </c>
       <c r="B64" s="71" t="s">
-        <v>114</v>
+        <v>6</v>
       </c>
       <c r="C64" s="85" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="D64" s="103" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -10851,10 +10863,10 @@
         <v>114</v>
       </c>
       <c r="C65" s="85" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D65" s="103" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -10865,10 +10877,10 @@
         <v>114</v>
       </c>
       <c r="C66" s="85" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D66" s="103" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -10879,10 +10891,10 @@
         <v>114</v>
       </c>
       <c r="C67" s="85" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="D67" s="103" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -10893,10 +10905,10 @@
         <v>114</v>
       </c>
       <c r="C68" s="85" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="D68" s="103" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -10907,10 +10919,10 @@
         <v>114</v>
       </c>
       <c r="C69" s="85" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D69" s="103" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -10921,10 +10933,10 @@
         <v>114</v>
       </c>
       <c r="C70" s="85" t="s">
-        <v>637</v>
+        <v>142</v>
       </c>
       <c r="D70" s="103" t="s">
-        <v>638</v>
+        <v>141</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -10935,24 +10947,24 @@
         <v>114</v>
       </c>
       <c r="C71" s="85" t="s">
+        <v>637</v>
+      </c>
+      <c r="D71" s="103" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="60" t="s">
+        <v>478</v>
+      </c>
+      <c r="B72" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="C72" s="85" t="s">
         <v>144</v>
       </c>
-      <c r="D71" s="108" t="s">
+      <c r="D72" s="108" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="104" t="s">
-        <v>472</v>
-      </c>
-      <c r="B72" s="109" t="s">
-        <v>479</v>
-      </c>
-      <c r="C72" s="105" t="s">
-        <v>154</v>
-      </c>
-      <c r="D72" s="106" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -10963,10 +10975,10 @@
         <v>479</v>
       </c>
       <c r="C73" s="105" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D73" s="106" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -10977,10 +10989,10 @@
         <v>479</v>
       </c>
       <c r="C74" s="105" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D74" s="106" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -10990,11 +11002,11 @@
       <c r="B75" s="109" t="s">
         <v>479</v>
       </c>
-      <c r="C75" s="146" t="s">
-        <v>94</v>
-      </c>
-      <c r="D75" s="146" t="s">
-        <v>95</v>
+      <c r="C75" s="105" t="s">
+        <v>160</v>
+      </c>
+      <c r="D75" s="106" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -11002,13 +11014,13 @@
         <v>472</v>
       </c>
       <c r="B76" s="109" t="s">
-        <v>184</v>
-      </c>
-      <c r="C76" s="105" t="s">
-        <v>185</v>
-      </c>
-      <c r="D76" s="106" t="s">
-        <v>186</v>
+        <v>479</v>
+      </c>
+      <c r="C76" s="146" t="s">
+        <v>94</v>
+      </c>
+      <c r="D76" s="146" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -11016,13 +11028,13 @@
         <v>472</v>
       </c>
       <c r="B77" s="109" t="s">
-        <v>114</v>
+        <v>184</v>
       </c>
       <c r="C77" s="105" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="D77" s="106" t="s">
-        <v>159</v>
+        <v>186</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -11033,10 +11045,10 @@
         <v>114</v>
       </c>
       <c r="C78" s="105" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D78" s="106" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -11044,13 +11056,13 @@
         <v>472</v>
       </c>
       <c r="B79" s="109" t="s">
-        <v>490</v>
-      </c>
-      <c r="C79" s="146" t="s">
-        <v>96</v>
-      </c>
-      <c r="D79" s="146" t="s">
-        <v>97</v>
+        <v>114</v>
+      </c>
+      <c r="C79" s="105" t="s">
+        <v>163</v>
+      </c>
+      <c r="D79" s="106" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -11058,27 +11070,27 @@
         <v>472</v>
       </c>
       <c r="B80" s="109" t="s">
+        <v>490</v>
+      </c>
+      <c r="C80" s="146" t="s">
+        <v>96</v>
+      </c>
+      <c r="D80" s="146" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="104" t="s">
+        <v>472</v>
+      </c>
+      <c r="B81" s="109" t="s">
         <v>491</v>
       </c>
-      <c r="C80" s="146" t="s">
+      <c r="C81" s="146" t="s">
         <v>247</v>
       </c>
-      <c r="D80" s="146" t="s">
+      <c r="D81" s="146" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" s="79" t="s">
-        <v>484</v>
-      </c>
-      <c r="B81" s="76" t="s">
-        <v>71</v>
-      </c>
-      <c r="C81" s="77" t="s">
-        <v>83</v>
-      </c>
-      <c r="D81" s="77" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -11086,55 +11098,55 @@
         <v>484</v>
       </c>
       <c r="B82" s="76" t="s">
-        <v>84</v>
-      </c>
-      <c r="C82" s="78" t="s">
-        <v>81</v>
+        <v>71</v>
+      </c>
+      <c r="C82" s="77" t="s">
+        <v>83</v>
       </c>
       <c r="D82" s="77" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="79" t="s">
+        <v>484</v>
+      </c>
+      <c r="B83" s="76" t="s">
+        <v>84</v>
+      </c>
+      <c r="C83" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="D83" s="77" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="79" t="s">
         <v>483</v>
       </c>
-      <c r="B83" s="76" t="s">
+      <c r="B84" s="76" t="s">
         <v>386</v>
       </c>
-      <c r="C83" s="77" t="s">
+      <c r="C84" s="77" t="s">
         <v>385</v>
       </c>
-      <c r="D83" s="77" t="s">
+      <c r="D84" s="77" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="84" spans="1:4" s="4" customFormat="1" ht="30">
-      <c r="A84" s="124" t="s">
+    <row r="85" spans="1:4" s="4" customFormat="1" ht="30">
+      <c r="A85" s="124" t="s">
         <v>483</v>
       </c>
-      <c r="B84" s="125" t="s">
+      <c r="B85" s="125" t="s">
         <v>45</v>
       </c>
-      <c r="C84" s="126" t="s">
+      <c r="C85" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="D84" s="126" t="s">
+      <c r="D85" s="126" t="s">
         <v>350</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="79" t="s">
-        <v>481</v>
-      </c>
-      <c r="B85" s="76" t="s">
-        <v>118</v>
-      </c>
-      <c r="C85" s="77" t="s">
-        <v>539</v>
-      </c>
-      <c r="D85" s="77" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -11142,13 +11154,13 @@
         <v>481</v>
       </c>
       <c r="B86" s="76" t="s">
-        <v>26</v>
+        <v>118</v>
       </c>
       <c r="C86" s="77" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D86" s="77" t="s">
-        <v>117</v>
+        <v>28</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -11159,80 +11171,80 @@
         <v>26</v>
       </c>
       <c r="C87" s="77" t="s">
-        <v>120</v>
+        <v>540</v>
       </c>
       <c r="D87" s="77" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="79" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B88" s="76" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="C88" s="77" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="D88" s="77" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="79" t="s">
-        <v>612</v>
-      </c>
-      <c r="B89" s="79" t="s">
-        <v>613</v>
+        <v>482</v>
+      </c>
+      <c r="B89" s="76" t="s">
+        <v>53</v>
       </c>
       <c r="C89" s="77" t="s">
-        <v>615</v>
+        <v>52</v>
       </c>
       <c r="D89" s="77" t="s">
-        <v>614</v>
+        <v>54</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="79" t="s">
-        <v>487</v>
-      </c>
-      <c r="B90" s="76" t="s">
-        <v>122</v>
+        <v>612</v>
+      </c>
+      <c r="B90" s="79" t="s">
+        <v>613</v>
       </c>
       <c r="C90" s="77" t="s">
-        <v>601</v>
-      </c>
-      <c r="D90" s="128" t="s">
-        <v>602</v>
+        <v>615</v>
+      </c>
+      <c r="D90" s="77" t="s">
+        <v>614</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="79" t="s">
-        <v>249</v>
+        <v>487</v>
       </c>
       <c r="B91" s="76" t="s">
-        <v>230</v>
+        <v>122</v>
       </c>
       <c r="C91" s="77" t="s">
-        <v>246</v>
-      </c>
-      <c r="D91" s="77" t="s">
-        <v>229</v>
+        <v>601</v>
+      </c>
+      <c r="D91" s="128" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="79" t="s">
-        <v>210</v>
+        <v>249</v>
       </c>
       <c r="B92" s="76" t="s">
-        <v>209</v>
+        <v>230</v>
       </c>
       <c r="C92" s="77" t="s">
-        <v>211</v>
+        <v>246</v>
       </c>
       <c r="D92" s="77" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -11240,13 +11252,13 @@
         <v>210</v>
       </c>
       <c r="B93" s="76" t="s">
-        <v>212</v>
-      </c>
-      <c r="C93" s="78" t="s">
-        <v>525</v>
+        <v>209</v>
+      </c>
+      <c r="C93" s="77" t="s">
+        <v>211</v>
       </c>
       <c r="D93" s="77" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -11254,13 +11266,13 @@
         <v>210</v>
       </c>
       <c r="B94" s="76" t="s">
-        <v>232</v>
-      </c>
-      <c r="C94" s="77" t="s">
-        <v>245</v>
+        <v>212</v>
+      </c>
+      <c r="C94" s="78" t="s">
+        <v>525</v>
       </c>
       <c r="D94" s="77" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -11268,13 +11280,13 @@
         <v>210</v>
       </c>
       <c r="B95" s="76" t="s">
-        <v>528</v>
+        <v>232</v>
       </c>
       <c r="C95" s="77" t="s">
-        <v>526</v>
+        <v>245</v>
       </c>
       <c r="D95" s="77" t="s">
-        <v>527</v>
+        <v>231</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -11282,13 +11294,13 @@
         <v>210</v>
       </c>
       <c r="B96" s="76" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C96" s="77" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D96" s="77" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -11296,13 +11308,13 @@
         <v>210</v>
       </c>
       <c r="B97" s="76" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C97" s="77" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D97" s="77" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -11310,41 +11322,41 @@
         <v>210</v>
       </c>
       <c r="B98" s="76" t="s">
+        <v>534</v>
+      </c>
+      <c r="C98" s="77" t="s">
+        <v>532</v>
+      </c>
+      <c r="D98" s="77" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="79" t="s">
+        <v>210</v>
+      </c>
+      <c r="B99" s="76" t="s">
         <v>537</v>
       </c>
-      <c r="C98" s="77" t="s">
+      <c r="C99" s="77" t="s">
         <v>535</v>
       </c>
-      <c r="D98" s="77" t="s">
+      <c r="D99" s="77" t="s">
         <v>536</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="80" t="s">
-        <v>357</v>
-      </c>
-      <c r="B99" s="174" t="s">
-        <v>566</v>
-      </c>
-      <c r="C99" s="173" t="s">
-        <v>567</v>
-      </c>
-      <c r="D99" s="81" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="80" t="s">
         <v>357</v>
       </c>
-      <c r="B100" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="C100" s="81" t="s">
-        <v>78</v>
+      <c r="B100" s="174" t="s">
+        <v>566</v>
+      </c>
+      <c r="C100" s="173" t="s">
+        <v>567</v>
       </c>
       <c r="D100" s="81" t="s">
-        <v>556</v>
+        <v>568</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -11355,38 +11367,38 @@
         <v>79</v>
       </c>
       <c r="C101" s="81" t="s">
-        <v>351</v>
+        <v>78</v>
       </c>
       <c r="D101" s="81" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" s="4" customFormat="1" ht="30">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" s="80" t="s">
         <v>357</v>
       </c>
-      <c r="B102" s="112" t="s">
+      <c r="B102" s="82" t="s">
         <v>79</v>
       </c>
-      <c r="C102" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="D102" s="9" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4">
+      <c r="C102" s="81" t="s">
+        <v>351</v>
+      </c>
+      <c r="D102" s="81" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" s="4" customFormat="1" ht="30">
       <c r="A103" s="80" t="s">
         <v>357</v>
       </c>
-      <c r="B103" s="110" t="s">
-        <v>380</v>
-      </c>
-      <c r="C103" s="98" t="s">
-        <v>381</v>
-      </c>
-      <c r="D103" s="111" t="s">
-        <v>382</v>
+      <c r="B103" s="112" t="s">
+        <v>79</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -11397,38 +11409,38 @@
         <v>380</v>
       </c>
       <c r="C104" s="98" t="s">
+        <v>381</v>
+      </c>
+      <c r="D104" s="111" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="80" t="s">
+        <v>357</v>
+      </c>
+      <c r="B105" s="110" t="s">
+        <v>380</v>
+      </c>
+      <c r="C105" s="98" t="s">
         <v>383</v>
       </c>
-      <c r="D104" s="111" t="s">
+      <c r="D105" s="111" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
-      <c r="A105" s="114" t="s">
-        <v>486</v>
-      </c>
-      <c r="B105" s="113" t="s">
-        <v>40</v>
-      </c>
-      <c r="C105" s="115" t="s">
-        <v>37</v>
-      </c>
-      <c r="D105" s="115" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" s="3" customFormat="1">
+    <row r="106" spans="1:4">
       <c r="A106" s="114" t="s">
         <v>486</v>
       </c>
-      <c r="B106" s="145" t="s">
-        <v>269</v>
-      </c>
-      <c r="C106" s="116" t="s">
-        <v>263</v>
-      </c>
-      <c r="D106" s="117" t="s">
-        <v>261</v>
+      <c r="B106" s="113" t="s">
+        <v>40</v>
+      </c>
+      <c r="C106" s="115" t="s">
+        <v>37</v>
+      </c>
+      <c r="D106" s="115" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="107" spans="1:4" s="3" customFormat="1">
@@ -11439,10 +11451,10 @@
         <v>269</v>
       </c>
       <c r="C107" s="116" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D107" s="117" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="108" spans="1:4" s="3" customFormat="1">
@@ -11450,13 +11462,13 @@
         <v>486</v>
       </c>
       <c r="B108" s="145" t="s">
-        <v>256</v>
-      </c>
-      <c r="C108" s="118" t="s">
-        <v>258</v>
+        <v>269</v>
+      </c>
+      <c r="C108" s="116" t="s">
+        <v>264</v>
       </c>
       <c r="D108" s="117" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
     </row>
     <row r="109" spans="1:4" s="3" customFormat="1">
@@ -11464,13 +11476,13 @@
         <v>486</v>
       </c>
       <c r="B109" s="145" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="C109" s="118" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="D109" s="117" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="110" spans="1:4" s="3" customFormat="1">
@@ -11481,38 +11493,38 @@
         <v>266</v>
       </c>
       <c r="C110" s="118" t="s">
+        <v>265</v>
+      </c>
+      <c r="D110" s="117" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" s="3" customFormat="1">
+      <c r="A111" s="114" t="s">
+        <v>486</v>
+      </c>
+      <c r="B111" s="145" t="s">
+        <v>266</v>
+      </c>
+      <c r="C111" s="118" t="s">
         <v>259</v>
       </c>
-      <c r="D110" s="117" t="s">
+      <c r="D111" s="117" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="111" spans="1:4" s="4" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A111" s="119" t="s">
-        <v>493</v>
-      </c>
-      <c r="B111" s="120" t="s">
-        <v>220</v>
-      </c>
-      <c r="C111" s="121" t="s">
-        <v>485</v>
-      </c>
-      <c r="D111" s="122" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" s="4" customFormat="1" ht="39.75" customHeight="1">
       <c r="A112" s="119" t="s">
         <v>493</v>
       </c>
-      <c r="B112" s="35" t="s">
-        <v>147</v>
-      </c>
-      <c r="C112" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="D112" s="36" t="s">
-        <v>109</v>
+      <c r="B112" s="120" t="s">
+        <v>220</v>
+      </c>
+      <c r="C112" s="121" t="s">
+        <v>485</v>
+      </c>
+      <c r="D112" s="122" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -11520,13 +11532,13 @@
         <v>493</v>
       </c>
       <c r="B113" s="35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C113" s="36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D113" s="36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -11534,13 +11546,13 @@
         <v>493</v>
       </c>
       <c r="B114" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C114" s="36" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D114" s="36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -11548,93 +11560,93 @@
         <v>493</v>
       </c>
       <c r="B115" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="C115" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D115" s="36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="119" t="s">
+        <v>493</v>
+      </c>
+      <c r="B116" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="C115" s="36" t="s">
+      <c r="C116" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="D115" s="36" t="s">
+      <c r="D116" s="36" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15.75">
-      <c r="A116" s="167" t="s">
+    <row r="117" spans="1:4" ht="15.75">
+      <c r="A117" s="167" t="s">
         <v>497</v>
       </c>
-      <c r="B116" s="167" t="s">
+      <c r="B117" s="167" t="s">
         <v>215</v>
       </c>
-      <c r="C116" s="171" t="s">
+      <c r="C117" s="171" t="s">
         <v>563</v>
       </c>
-      <c r="D116" s="168" t="s">
+      <c r="D117" s="168" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="30">
-      <c r="A117" s="169" t="s">
+    <row r="118" spans="1:4" ht="30">
+      <c r="A118" s="169" t="s">
         <v>497</v>
       </c>
-      <c r="B117" s="169" t="s">
+      <c r="B118" s="169" t="s">
         <v>215</v>
       </c>
-      <c r="C117" s="172" t="s">
+      <c r="C118" s="172" t="s">
         <v>564</v>
       </c>
-      <c r="D117" s="170" t="s">
+      <c r="D118" s="170" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="31.5">
-      <c r="A118" s="169"/>
-      <c r="B118" s="169"/>
-      <c r="C118" s="172" t="s">
+    <row r="119" spans="1:4" ht="31.5">
+      <c r="A119" s="169"/>
+      <c r="B119" s="169"/>
+      <c r="C119" s="172" t="s">
         <v>639</v>
       </c>
-      <c r="D118" s="170" t="s">
+      <c r="D119" s="170" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="31.5">
-      <c r="A119" s="169" t="s">
+    <row r="120" spans="1:4" ht="31.5">
+      <c r="A120" s="169" t="s">
         <v>497</v>
       </c>
-      <c r="B119" s="169" t="s">
+      <c r="B120" s="169" t="s">
         <v>215</v>
       </c>
-      <c r="C119" s="172" t="s">
+      <c r="C120" s="172" t="s">
         <v>608</v>
       </c>
-      <c r="D119" s="170" t="s">
+      <c r="D120" s="170" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="120" spans="1:4" s="3" customFormat="1">
-      <c r="A120" s="152" t="s">
+    <row r="121" spans="1:4" s="3" customFormat="1">
+      <c r="A121" s="152" t="s">
         <v>39</v>
       </c>
-      <c r="B120" s="153" t="s">
+      <c r="B121" s="153" t="s">
         <v>242</v>
       </c>
-      <c r="C120" s="154" t="s">
+      <c r="C121" s="154" t="s">
         <v>244</v>
       </c>
-      <c r="D120" s="155" t="s">
+      <c r="D121" s="155" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4">
-      <c r="A121" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="B121" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="C121" s="61" t="s">
-        <v>42</v>
-      </c>
-      <c r="D121" s="61" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -11645,10 +11657,10 @@
         <v>41</v>
       </c>
       <c r="C122" s="61" t="s">
-        <v>275</v>
+        <v>42</v>
       </c>
       <c r="D122" s="61" t="s">
-        <v>274</v>
+        <v>43</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -11656,13 +11668,13 @@
         <v>1</v>
       </c>
       <c r="B123" s="71" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C123" s="61" t="s">
-        <v>23</v>
+        <v>275</v>
       </c>
       <c r="D123" s="61" t="s">
-        <v>22</v>
+        <v>274</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -11670,13 +11682,13 @@
         <v>1</v>
       </c>
       <c r="B124" s="71" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C124" s="61" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D124" s="61" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -11684,13 +11696,13 @@
         <v>1</v>
       </c>
       <c r="B125" s="71" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C125" s="61" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D125" s="61" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -11698,13 +11710,13 @@
         <v>1</v>
       </c>
       <c r="B126" s="71" t="s">
-        <v>298</v>
+        <v>47</v>
       </c>
       <c r="C126" s="61" t="s">
-        <v>294</v>
+        <v>46</v>
       </c>
       <c r="D126" s="61" t="s">
-        <v>299</v>
+        <v>48</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -11712,13 +11724,13 @@
         <v>1</v>
       </c>
       <c r="B127" s="71" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C127" s="61" t="s">
-        <v>183</v>
+        <v>294</v>
       </c>
       <c r="D127" s="61" t="s">
-        <v>102</v>
+        <v>299</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -11729,10 +11741,10 @@
         <v>295</v>
       </c>
       <c r="C128" s="61" t="s">
-        <v>104</v>
+        <v>183</v>
       </c>
       <c r="D128" s="61" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -11740,13 +11752,13 @@
         <v>1</v>
       </c>
       <c r="B129" s="71" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C129" s="61" t="s">
-        <v>239</v>
+        <v>104</v>
       </c>
       <c r="D129" s="61" t="s">
-        <v>240</v>
+        <v>103</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -11754,13 +11766,13 @@
         <v>1</v>
       </c>
       <c r="B130" s="71" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C130" s="61" t="s">
-        <v>587</v>
+        <v>239</v>
       </c>
       <c r="D130" s="61" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -11768,13 +11780,13 @@
         <v>1</v>
       </c>
       <c r="B131" s="71" t="s">
-        <v>87</v>
+        <v>297</v>
       </c>
       <c r="C131" s="61" t="s">
-        <v>85</v>
+        <v>587</v>
       </c>
       <c r="D131" s="61" t="s">
-        <v>86</v>
+        <v>241</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -11782,13 +11794,13 @@
         <v>1</v>
       </c>
       <c r="B132" s="71" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="C132" s="61" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="D132" s="61" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -11796,13 +11808,13 @@
         <v>1</v>
       </c>
       <c r="B133" s="71" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C133" s="61" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D133" s="61" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -11810,13 +11822,13 @@
         <v>1</v>
       </c>
       <c r="B134" s="71" t="s">
-        <v>280</v>
-      </c>
-      <c r="C134" s="83" t="s">
-        <v>281</v>
-      </c>
-      <c r="D134" s="83" t="s">
-        <v>282</v>
+        <v>49</v>
+      </c>
+      <c r="C134" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="D134" s="61" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -11824,13 +11836,13 @@
         <v>1</v>
       </c>
       <c r="B135" s="71" t="s">
-        <v>499</v>
-      </c>
-      <c r="C135" s="61" t="s">
-        <v>69</v>
-      </c>
-      <c r="D135" s="61" t="s">
-        <v>70</v>
+        <v>280</v>
+      </c>
+      <c r="C135" s="83" t="s">
+        <v>281</v>
+      </c>
+      <c r="D135" s="83" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -11838,13 +11850,13 @@
         <v>1</v>
       </c>
       <c r="B136" s="71" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C136" s="61" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D136" s="61" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -11855,10 +11867,10 @@
         <v>500</v>
       </c>
       <c r="C137" s="61" t="s">
-        <v>167</v>
+        <v>73</v>
       </c>
       <c r="D137" s="61" t="s">
-        <v>166</v>
+        <v>74</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -11866,13 +11878,13 @@
         <v>1</v>
       </c>
       <c r="B138" s="71" t="s">
-        <v>76</v>
+        <v>500</v>
       </c>
       <c r="C138" s="61" t="s">
-        <v>75</v>
+        <v>167</v>
       </c>
       <c r="D138" s="61" t="s">
-        <v>77</v>
+        <v>166</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -11883,10 +11895,10 @@
         <v>76</v>
       </c>
       <c r="C139" s="61" t="s">
-        <v>164</v>
+        <v>75</v>
       </c>
       <c r="D139" s="61" t="s">
-        <v>165</v>
+        <v>77</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -11897,10 +11909,10 @@
         <v>76</v>
       </c>
       <c r="C140" s="61" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D140" s="61" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -11910,11 +11922,11 @@
       <c r="B141" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="C141" s="84" t="s">
-        <v>562</v>
+      <c r="C141" s="61" t="s">
+        <v>169</v>
       </c>
       <c r="D141" s="61" t="s">
-        <v>238</v>
+        <v>168</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -11922,13 +11934,13 @@
         <v>1</v>
       </c>
       <c r="B142" s="71" t="s">
-        <v>170</v>
-      </c>
-      <c r="C142" s="61" t="s">
-        <v>172</v>
+        <v>76</v>
+      </c>
+      <c r="C142" s="84" t="s">
+        <v>562</v>
       </c>
       <c r="D142" s="61" t="s">
-        <v>171</v>
+        <v>238</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -11936,13 +11948,13 @@
         <v>1</v>
       </c>
       <c r="B143" s="71" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C143" s="61" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D143" s="61" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -11950,13 +11962,13 @@
         <v>1</v>
       </c>
       <c r="B144" s="71" t="s">
-        <v>218</v>
+        <v>174</v>
       </c>
       <c r="C144" s="61" t="s">
-        <v>217</v>
+        <v>173</v>
       </c>
       <c r="D144" s="61" t="s">
-        <v>219</v>
+        <v>175</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -11964,13 +11976,13 @@
         <v>1</v>
       </c>
       <c r="B145" s="71" t="s">
-        <v>227</v>
-      </c>
-      <c r="C145" s="85" t="s">
-        <v>228</v>
+        <v>218</v>
+      </c>
+      <c r="C145" s="61" t="s">
+        <v>217</v>
       </c>
       <c r="D145" s="61" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -11978,13 +11990,13 @@
         <v>1</v>
       </c>
       <c r="B146" s="71" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C146" s="85" t="s">
-        <v>365</v>
+        <v>228</v>
       </c>
       <c r="D146" s="61" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -11992,13 +12004,13 @@
         <v>1</v>
       </c>
       <c r="B147" s="71" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C147" s="85" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D147" s="61" t="s">
-        <v>364</v>
+        <v>234</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -12009,24 +12021,24 @@
         <v>235</v>
       </c>
       <c r="C148" s="85" t="s">
+        <v>363</v>
+      </c>
+      <c r="D148" s="61" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B149" s="71" t="s">
+        <v>235</v>
+      </c>
+      <c r="C149" s="85" t="s">
         <v>236</v>
       </c>
-      <c r="D148" s="61" t="s">
+      <c r="D149" s="61" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4">
-      <c r="A149" s="80" t="s">
-        <v>80</v>
-      </c>
-      <c r="B149" s="82" t="s">
-        <v>106</v>
-      </c>
-      <c r="C149" s="81" t="s">
-        <v>107</v>
-      </c>
-      <c r="D149" s="81" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -12034,13 +12046,13 @@
         <v>80</v>
       </c>
       <c r="B150" s="82" t="s">
-        <v>181</v>
+        <v>106</v>
       </c>
       <c r="C150" s="81" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D150" s="81" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -12048,13 +12060,13 @@
         <v>80</v>
       </c>
       <c r="B151" s="82" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C151" s="81" t="s">
-        <v>288</v>
+        <v>99</v>
       </c>
       <c r="D151" s="81" t="s">
-        <v>180</v>
+        <v>98</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -12062,13 +12074,13 @@
         <v>80</v>
       </c>
       <c r="B152" s="82" t="s">
-        <v>421</v>
+        <v>182</v>
       </c>
       <c r="C152" s="81" t="s">
-        <v>422</v>
+        <v>288</v>
       </c>
       <c r="D152" s="81" t="s">
-        <v>420</v>
+        <v>180</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -12076,13 +12088,13 @@
         <v>80</v>
       </c>
       <c r="B153" s="82" t="s">
-        <v>199</v>
+        <v>421</v>
       </c>
       <c r="C153" s="81" t="s">
-        <v>198</v>
+        <v>422</v>
       </c>
       <c r="D153" s="81" t="s">
-        <v>200</v>
+        <v>420</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -12093,10 +12105,10 @@
         <v>199</v>
       </c>
       <c r="C154" s="81" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D154" s="81" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -12107,10 +12119,10 @@
         <v>199</v>
       </c>
       <c r="C155" s="81" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D155" s="81" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -12118,16 +12130,16 @@
         <v>80</v>
       </c>
       <c r="B156" s="82" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C156" s="81" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="D156" s="81" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="15.75">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
       <c r="A157" s="80" t="s">
         <v>80</v>
       </c>
@@ -12135,52 +12147,52 @@
         <v>205</v>
       </c>
       <c r="C157" s="81" t="s">
-        <v>576</v>
-      </c>
-      <c r="D157" s="177" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4">
+        <v>197</v>
+      </c>
+      <c r="D157" s="81" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="15.75">
       <c r="A158" s="80" t="s">
         <v>80</v>
       </c>
       <c r="B158" s="82" t="s">
-        <v>580</v>
+        <v>205</v>
       </c>
       <c r="C158" s="81" t="s">
-        <v>578</v>
-      </c>
-      <c r="D158" s="178" t="s">
-        <v>579</v>
+        <v>576</v>
+      </c>
+      <c r="D158" s="177" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="B159" s="130" t="s">
+      <c r="B159" s="82" t="s">
+        <v>580</v>
+      </c>
+      <c r="C159" s="81" t="s">
+        <v>578</v>
+      </c>
+      <c r="D159" s="178" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" s="80" t="s">
+        <v>80</v>
+      </c>
+      <c r="B160" s="130" t="s">
         <v>205</v>
       </c>
-      <c r="C159" s="131" t="s">
+      <c r="C160" s="131" t="s">
         <v>207</v>
       </c>
-      <c r="D159" s="131" t="s">
+      <c r="D160" s="131" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4">
-      <c r="A160" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="B160" s="70" t="s">
-        <v>506</v>
-      </c>
-      <c r="C160" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="D160" s="69" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -12191,10 +12203,10 @@
         <v>506</v>
       </c>
       <c r="C161" s="69" t="s">
-        <v>509</v>
+        <v>66</v>
       </c>
       <c r="D161" s="69" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -12205,10 +12217,10 @@
         <v>506</v>
       </c>
       <c r="C162" s="69" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="D162" s="69" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -12216,13 +12228,13 @@
         <v>8</v>
       </c>
       <c r="B163" s="70" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="C163" s="69" t="s">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="D163" s="69" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -12230,13 +12242,13 @@
         <v>8</v>
       </c>
       <c r="B164" s="70" t="s">
-        <v>447</v>
+        <v>513</v>
       </c>
       <c r="C164" s="69" t="s">
-        <v>287</v>
+        <v>510</v>
       </c>
       <c r="D164" s="69" t="s">
-        <v>443</v>
+        <v>511</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -12247,10 +12259,10 @@
         <v>447</v>
       </c>
       <c r="C165" s="69" t="s">
-        <v>448</v>
+        <v>287</v>
       </c>
       <c r="D165" s="69" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -12258,13 +12270,13 @@
         <v>8</v>
       </c>
       <c r="B166" s="70" t="s">
-        <v>289</v>
+        <v>447</v>
       </c>
       <c r="C166" s="69" t="s">
-        <v>290</v>
+        <v>448</v>
       </c>
       <c r="D166" s="69" t="s">
-        <v>291</v>
+        <v>446</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -12272,13 +12284,13 @@
         <v>8</v>
       </c>
       <c r="B167" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C167" s="68" t="s">
-        <v>9</v>
+        <v>289</v>
+      </c>
+      <c r="C167" s="69" t="s">
+        <v>290</v>
       </c>
       <c r="D167" s="69" t="s">
-        <v>11</v>
+        <v>291</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -12289,10 +12301,10 @@
         <v>8</v>
       </c>
       <c r="C168" s="68" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D168" s="69" t="s">
-        <v>65</v>
+        <v>11</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -12303,10 +12315,10 @@
         <v>8</v>
       </c>
       <c r="C169" s="68" t="s">
-        <v>390</v>
+        <v>20</v>
       </c>
       <c r="D169" s="69" t="s">
-        <v>391</v>
+        <v>65</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -12317,10 +12329,10 @@
         <v>8</v>
       </c>
       <c r="C170" s="68" t="s">
-        <v>9</v>
+        <v>390</v>
       </c>
       <c r="D170" s="69" t="s">
-        <v>11</v>
+        <v>391</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -12331,10 +12343,10 @@
         <v>8</v>
       </c>
       <c r="C171" s="68" t="s">
-        <v>359</v>
+        <v>9</v>
       </c>
       <c r="D171" s="69" t="s">
-        <v>360</v>
+        <v>11</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -12345,10 +12357,10 @@
         <v>8</v>
       </c>
       <c r="C172" s="68" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D172" s="69" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -12356,13 +12368,13 @@
         <v>8</v>
       </c>
       <c r="B173" s="70" t="s">
-        <v>438</v>
+        <v>8</v>
       </c>
       <c r="C173" s="68" t="s">
         <v>361</v>
       </c>
       <c r="D173" s="69" t="s">
-        <v>437</v>
+        <v>362</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -12376,38 +12388,38 @@
         <v>361</v>
       </c>
       <c r="D174" s="69" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="B175" s="70" t="s">
+        <v>438</v>
+      </c>
+      <c r="C175" s="68" t="s">
+        <v>361</v>
+      </c>
+      <c r="D175" s="69" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="175" spans="1:4">
-      <c r="A175" s="71" t="s">
-        <v>327</v>
-      </c>
-      <c r="B175" s="60" t="s">
-        <v>501</v>
-      </c>
-      <c r="C175" s="61" t="s">
-        <v>176</v>
-      </c>
-      <c r="D175" s="61" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1">
+    <row r="176" spans="1:4">
       <c r="A176" s="71" t="s">
         <v>327</v>
       </c>
-      <c r="B176" s="129" t="s">
-        <v>432</v>
-      </c>
-      <c r="C176" s="12" t="s">
-        <v>423</v>
-      </c>
-      <c r="D176" s="12" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" s="3" customFormat="1" ht="30">
+      <c r="B176" s="60" t="s">
+        <v>501</v>
+      </c>
+      <c r="C176" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="D176" s="61" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1">
       <c r="A177" s="71" t="s">
         <v>327</v>
       </c>
@@ -12415,24 +12427,24 @@
         <v>432</v>
       </c>
       <c r="C177" s="12" t="s">
-        <v>444</v>
+        <v>423</v>
       </c>
       <c r="D177" s="12" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A178" s="72" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" s="3" customFormat="1" ht="30">
+      <c r="A178" s="71" t="s">
         <v>327</v>
       </c>
       <c r="B178" s="129" t="s">
         <v>432</v>
       </c>
-      <c r="C178" s="62" t="s">
-        <v>349</v>
+      <c r="C178" s="12" t="s">
+        <v>444</v>
       </c>
       <c r="D178" s="12" t="s">
-        <v>348</v>
+        <v>325</v>
       </c>
     </row>
     <row r="179" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
@@ -12443,38 +12455,38 @@
         <v>432</v>
       </c>
       <c r="C179" s="62" t="s">
-        <v>424</v>
+        <v>349</v>
       </c>
       <c r="D179" s="12" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" s="3" customFormat="1" ht="76.5" customHeight="1">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
       <c r="A180" s="72" t="s">
         <v>327</v>
       </c>
       <c r="B180" s="129" t="s">
-        <v>502</v>
-      </c>
-      <c r="C180" s="12" t="s">
-        <v>330</v>
+        <v>432</v>
+      </c>
+      <c r="C180" s="62" t="s">
+        <v>424</v>
       </c>
       <c r="D180" s="12" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" s="3" customFormat="1" ht="76.5" customHeight="1">
       <c r="A181" s="72" t="s">
         <v>327</v>
       </c>
       <c r="B181" s="129" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C181" s="12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D181" s="12" t="s">
-        <v>431</v>
+        <v>329</v>
       </c>
     </row>
     <row r="182" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
@@ -12482,55 +12494,55 @@
         <v>327</v>
       </c>
       <c r="B182" s="129" t="s">
+        <v>503</v>
+      </c>
+      <c r="C182" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="D182" s="12" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
+      <c r="A183" s="72" t="s">
+        <v>327</v>
+      </c>
+      <c r="B183" s="129" t="s">
         <v>426</v>
       </c>
-      <c r="C182" s="12" t="s">
+      <c r="C183" s="12" t="s">
         <v>427</v>
       </c>
-      <c r="D182" s="12" t="s">
+      <c r="D183" s="12" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="183" spans="1:4">
-      <c r="A183" s="74" t="s">
-        <v>187</v>
-      </c>
-      <c r="B183" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="C183" s="11" t="s">
-        <v>328</v>
-      </c>
-      <c r="D183" s="11" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" s="4" customFormat="1" ht="39.75" customHeight="1">
+    <row r="184" spans="1:4">
       <c r="A184" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="B184" s="63" t="s">
+      <c r="B184" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="C184" s="64" t="s">
-        <v>428</v>
-      </c>
-      <c r="D184" s="65" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4">
+      <c r="C184" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="D184" s="11" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" s="4" customFormat="1" ht="39.75" customHeight="1">
       <c r="A185" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="B185" s="10" t="s">
+      <c r="B185" s="63" t="s">
         <v>318</v>
       </c>
-      <c r="C185" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="D185" s="11" t="s">
-        <v>320</v>
+      <c r="C185" s="64" t="s">
+        <v>428</v>
+      </c>
+      <c r="D185" s="65" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -12541,52 +12553,52 @@
         <v>318</v>
       </c>
       <c r="C186" s="11" t="s">
-        <v>342</v>
+        <v>319</v>
       </c>
       <c r="D186" s="11" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" s="4" customFormat="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
       <c r="A187" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="B187" s="73" t="s">
+      <c r="B187" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="C187" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="D187" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" s="4" customFormat="1">
+      <c r="A188" s="74" t="s">
+        <v>187</v>
+      </c>
+      <c r="B188" s="73" t="s">
         <v>313</v>
       </c>
-      <c r="C187" s="65" t="s">
+      <c r="C188" s="65" t="s">
         <v>312</v>
       </c>
-      <c r="D187" s="65" t="s">
+      <c r="D188" s="65" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="188" spans="1:4">
-      <c r="A188" s="75" t="s">
+    <row r="189" spans="1:4">
+      <c r="A189" s="75" t="s">
         <v>187</v>
       </c>
-      <c r="B188" s="10" t="s">
+      <c r="B189" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="C188" s="11" t="s">
+      <c r="C189" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="D188" s="65" t="s">
+      <c r="D189" s="65" t="s">
         <v>316</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4">
-      <c r="A189" s="113" t="s">
-        <v>191</v>
-      </c>
-      <c r="B189" s="113" t="s">
-        <v>189</v>
-      </c>
-      <c r="C189" s="115" t="s">
-        <v>193</v>
-      </c>
-      <c r="D189" s="115" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -12597,38 +12609,38 @@
         <v>189</v>
       </c>
       <c r="C190" s="115" t="s">
+        <v>193</v>
+      </c>
+      <c r="D190" s="115" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191" s="113" t="s">
+        <v>191</v>
+      </c>
+      <c r="B191" s="113" t="s">
+        <v>189</v>
+      </c>
+      <c r="C191" s="115" t="s">
         <v>195</v>
       </c>
-      <c r="D190" s="115" t="s">
+      <c r="D191" s="115" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="191" spans="1:4" s="3" customFormat="1">
-      <c r="A191" s="132" t="s">
-        <v>250</v>
-      </c>
-      <c r="B191" s="157" t="s">
-        <v>252</v>
-      </c>
-      <c r="C191" s="133" t="s">
-        <v>253</v>
-      </c>
-      <c r="D191" s="134" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" s="86" customFormat="1">
+    <row r="192" spans="1:4" s="3" customFormat="1">
       <c r="A192" s="132" t="s">
         <v>250</v>
       </c>
       <c r="B192" s="157" t="s">
-        <v>293</v>
+        <v>252</v>
       </c>
       <c r="C192" s="133" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
       <c r="D192" s="134" t="s">
-        <v>308</v>
+        <v>251</v>
       </c>
     </row>
     <row r="193" spans="1:4" s="86" customFormat="1">
@@ -12636,69 +12648,69 @@
         <v>250</v>
       </c>
       <c r="B193" s="157" t="s">
+        <v>293</v>
+      </c>
+      <c r="C193" s="133" t="s">
+        <v>292</v>
+      </c>
+      <c r="D193" s="134" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" s="86" customFormat="1">
+      <c r="A194" s="132" t="s">
+        <v>250</v>
+      </c>
+      <c r="B194" s="157" t="s">
         <v>286</v>
       </c>
-      <c r="C193" s="133" t="s">
+      <c r="C194" s="133" t="s">
         <v>285</v>
       </c>
-      <c r="D193" s="134" t="s">
+      <c r="D194" s="134" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="194" spans="1:4" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A194" s="135" t="s">
+    <row r="195" spans="1:4" s="4" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A195" s="135" t="s">
         <v>250</v>
       </c>
-      <c r="B194" s="157" t="s">
+      <c r="B195" s="157" t="s">
         <v>463</v>
       </c>
-      <c r="C194" s="136" t="s">
+      <c r="C195" s="136" t="s">
         <v>376</v>
       </c>
-      <c r="D194" s="137" t="s">
+      <c r="D195" s="137" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="195" spans="1:4" s="38" customFormat="1" ht="144.75" customHeight="1">
-      <c r="A195" s="138" t="s">
+    <row r="196" spans="1:4" s="38" customFormat="1" ht="144.75" customHeight="1">
+      <c r="A196" s="138" t="s">
         <v>250</v>
       </c>
-      <c r="B195" s="158" t="s">
+      <c r="B196" s="158" t="s">
         <v>504</v>
       </c>
-      <c r="C195" s="136" t="s">
+      <c r="C196" s="136" t="s">
         <v>488</v>
       </c>
-      <c r="D195" s="137" t="s">
+      <c r="D196" s="137" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="196" spans="1:4">
-      <c r="A196" s="159" t="s">
+    <row r="197" spans="1:4">
+      <c r="A197" s="159" t="s">
         <v>250</v>
       </c>
-      <c r="B196" s="160" t="s">
+      <c r="B197" s="160" t="s">
         <v>512</v>
       </c>
-      <c r="C196" s="161" t="s">
+      <c r="C197" s="161" t="s">
         <v>514</v>
       </c>
-      <c r="D196" s="161" t="s">
+      <c r="D197" s="161" t="s">
         <v>511</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" s="38" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A197" s="138" t="s">
-        <v>250</v>
-      </c>
-      <c r="B197" s="158" t="s">
-        <v>435</v>
-      </c>
-      <c r="C197" s="139" t="s">
-        <v>458</v>
-      </c>
-      <c r="D197" s="137" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="198" spans="1:4" s="38" customFormat="1" ht="28.5" customHeight="1">
@@ -12709,7 +12721,7 @@
         <v>435</v>
       </c>
       <c r="C198" s="139" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D198" s="137" t="s">
         <v>433</v>
@@ -12720,55 +12732,55 @@
         <v>250</v>
       </c>
       <c r="B199" s="158" t="s">
-        <v>436</v>
-      </c>
-      <c r="C199" s="140" t="s">
-        <v>441</v>
+        <v>435</v>
+      </c>
+      <c r="C199" s="139" t="s">
+        <v>459</v>
       </c>
       <c r="D199" s="137" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" s="4" customFormat="1" ht="38.25" customHeight="1">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" s="38" customFormat="1" ht="28.5" customHeight="1">
       <c r="A200" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B200" s="158" t="s">
-        <v>242</v>
-      </c>
-      <c r="C200" s="136" t="s">
-        <v>457</v>
+        <v>436</v>
+      </c>
+      <c r="C200" s="140" t="s">
+        <v>441</v>
       </c>
       <c r="D200" s="137" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" s="4" customFormat="1" ht="38.25" customHeight="1">
       <c r="A201" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B201" s="158" t="s">
-        <v>440</v>
+        <v>242</v>
       </c>
       <c r="C201" s="136" t="s">
-        <v>517</v>
+        <v>457</v>
       </c>
       <c r="D201" s="137" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1">
       <c r="A202" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B202" s="158" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="C202" s="136" t="s">
-        <v>456</v>
+        <v>517</v>
       </c>
       <c r="D202" s="137" t="s">
-        <v>523</v>
+        <v>451</v>
       </c>
     </row>
     <row r="203" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
@@ -12776,13 +12788,13 @@
         <v>250</v>
       </c>
       <c r="B203" s="158" t="s">
-        <v>522</v>
+        <v>455</v>
       </c>
       <c r="C203" s="136" t="s">
-        <v>521</v>
+        <v>456</v>
       </c>
       <c r="D203" s="137" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="204" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
@@ -12790,41 +12802,41 @@
         <v>250</v>
       </c>
       <c r="B204" s="158" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C204" s="136" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="D204" s="137" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
       <c r="A205" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B205" s="158" t="s">
+        <v>520</v>
+      </c>
+      <c r="C205" s="136" t="s">
+        <v>519</v>
+      </c>
+      <c r="D205" s="137" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="A206" s="138" t="s">
+        <v>250</v>
+      </c>
+      <c r="B206" s="158" t="s">
         <v>454</v>
       </c>
-      <c r="C205" s="136" t="s">
+      <c r="C206" s="136" t="s">
         <v>452</v>
       </c>
-      <c r="D205" s="137" t="s">
+      <c r="D206" s="137" t="s">
         <v>453</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4">
-      <c r="A206" s="123" t="s">
-        <v>222</v>
-      </c>
-      <c r="B206" s="123" t="s">
-        <v>223</v>
-      </c>
-      <c r="C206" s="36" t="s">
-        <v>248</v>
-      </c>
-      <c r="D206" s="36" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -12835,10 +12847,10 @@
         <v>223</v>
       </c>
       <c r="C207" s="36" t="s">
-        <v>225</v>
+        <v>248</v>
       </c>
       <c r="D207" s="36" t="s">
-        <v>260</v>
+        <v>224</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -12848,11 +12860,11 @@
       <c r="B208" s="123" t="s">
         <v>223</v>
       </c>
-      <c r="C208" s="156" t="s">
-        <v>633</v>
+      <c r="C208" s="36" t="s">
+        <v>225</v>
       </c>
       <c r="D208" s="36" t="s">
-        <v>300</v>
+        <v>260</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -12863,10 +12875,10 @@
         <v>223</v>
       </c>
       <c r="C209" s="156" t="s">
-        <v>306</v>
+        <v>633</v>
       </c>
       <c r="D209" s="36" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -12874,16 +12886,19 @@
         <v>222</v>
       </c>
       <c r="B210" s="123" t="s">
-        <v>626</v>
-      </c>
-      <c r="C210" s="180" t="s">
-        <v>304</v>
+        <v>223</v>
+      </c>
+      <c r="C210" s="156" t="s">
+        <v>306</v>
       </c>
       <c r="D210" s="36" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="211" spans="1:4">
+      <c r="A211" s="123" t="s">
+        <v>222</v>
+      </c>
       <c r="B211" s="123" t="s">
         <v>626</v>
       </c>
@@ -12891,21 +12906,18 @@
         <v>304</v>
       </c>
       <c r="D211" s="36" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="212" spans="1:4">
-      <c r="A212" s="123" t="s">
-        <v>222</v>
-      </c>
       <c r="B212" s="123" t="s">
         <v>626</v>
       </c>
       <c r="C212" s="180" t="s">
-        <v>634</v>
+        <v>304</v>
       </c>
       <c r="D212" s="36" t="s">
-        <v>635</v>
+        <v>305</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -12913,13 +12925,13 @@
         <v>222</v>
       </c>
       <c r="B213" s="123" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C213" s="180" t="s">
-        <v>307</v>
+        <v>634</v>
       </c>
       <c r="D213" s="36" t="s">
-        <v>301</v>
+        <v>635</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -12927,41 +12939,41 @@
         <v>222</v>
       </c>
       <c r="B214" s="123" t="s">
+        <v>628</v>
+      </c>
+      <c r="C214" s="180" t="s">
+        <v>307</v>
+      </c>
+      <c r="D214" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4">
+      <c r="A215" s="123" t="s">
+        <v>222</v>
+      </c>
+      <c r="B215" s="123" t="s">
         <v>629</v>
       </c>
-      <c r="C214" s="181" t="s">
+      <c r="C215" s="181" t="s">
         <v>393</v>
       </c>
-      <c r="D214" s="36" t="s">
+      <c r="D215" s="36" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="215" spans="1:4" s="179" customFormat="1" ht="15.75">
-      <c r="A215" s="182" t="s">
-        <v>222</v>
-      </c>
-      <c r="B215" s="182" t="s">
-        <v>629</v>
-      </c>
-      <c r="C215" s="183" t="s">
-        <v>583</v>
-      </c>
-      <c r="D215" s="184" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4">
+    <row r="216" spans="1:4" s="179" customFormat="1" ht="15.75">
       <c r="A216" s="182" t="s">
         <v>222</v>
       </c>
       <c r="B216" s="182" t="s">
-        <v>630</v>
-      </c>
-      <c r="C216" s="185" t="s">
-        <v>584</v>
-      </c>
-      <c r="D216" s="186" t="s">
-        <v>632</v>
+        <v>629</v>
+      </c>
+      <c r="C216" s="183" t="s">
+        <v>583</v>
+      </c>
+      <c r="D216" s="184" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -12969,13 +12981,13 @@
         <v>222</v>
       </c>
       <c r="B217" s="182" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C217" s="185" t="s">
-        <v>621</v>
+        <v>584</v>
       </c>
       <c r="D217" s="186" t="s">
-        <v>616</v>
+        <v>632</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -12986,10 +12998,10 @@
         <v>631</v>
       </c>
       <c r="C218" s="185" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D218" s="186" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -13000,10 +13012,10 @@
         <v>631</v>
       </c>
       <c r="C219" s="185" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D219" s="186" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -13014,10 +13026,10 @@
         <v>631</v>
       </c>
       <c r="C220" s="185" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D220" s="186" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -13028,10 +13040,10 @@
         <v>631</v>
       </c>
       <c r="C221" s="185" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D221" s="186" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -13039,17 +13051,31 @@
         <v>222</v>
       </c>
       <c r="B222" s="182" t="s">
+        <v>631</v>
+      </c>
+      <c r="C222" s="185" t="s">
+        <v>625</v>
+      </c>
+      <c r="D222" s="186" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4">
+      <c r="A223" s="182" t="s">
+        <v>222</v>
+      </c>
+      <c r="B223" s="182" t="s">
         <v>223</v>
       </c>
-      <c r="C222" s="185" t="s">
+      <c r="C223" s="185" t="s">
         <v>585</v>
       </c>
-      <c r="D222" s="186" t="s">
+      <c r="D223" s="186" t="s">
         <v>586</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D213" xr:uid="{85ED3410-72EE-453D-8BB3-FB7E07F682B1}"/>
+  <autoFilter ref="A2:D214" xr:uid="{85ED3410-72EE-453D-8BB3-FB7E07F682B1}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
@@ -13078,13 +13104,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33.75" customHeight="1">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="200" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="201"/>
+      <c r="B1" s="200"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="202"/>
     </row>
     <row r="2" spans="1:5" ht="207" customHeight="1">
       <c r="A2" s="43" t="s">
@@ -13331,22 +13357,22 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="408.95" customHeight="1">
-      <c r="A19" s="210" t="s">
+      <c r="A19" s="211" t="s">
         <v>222</v>
       </c>
-      <c r="B19" s="208" t="s">
+      <c r="B19" s="209" t="s">
         <v>592</v>
       </c>
-      <c r="C19" s="202"/>
-      <c r="D19" s="204"/>
-      <c r="E19" s="206"/>
+      <c r="C19" s="203"/>
+      <c r="D19" s="205"/>
+      <c r="E19" s="207"/>
     </row>
     <row r="20" spans="1:5" ht="351.75" customHeight="1">
-      <c r="A20" s="209"/>
-      <c r="B20" s="209"/>
-      <c r="C20" s="203"/>
-      <c r="D20" s="205"/>
-      <c r="E20" s="207"/>
+      <c r="A20" s="210"/>
+      <c r="B20" s="210"/>
+      <c r="C20" s="204"/>
+      <c r="D20" s="206"/>
+      <c r="E20" s="208"/>
     </row>
     <row r="21" spans="1:5" s="193" customFormat="1" ht="158.25" customHeight="1">
       <c r="A21" s="189" t="s">
@@ -14468,11 +14494,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="33.75" customHeight="1">
-      <c r="A1" s="211" t="s">
+      <c r="A1" s="212" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="211"/>
-      <c r="C1" s="211"/>
+      <c r="B1" s="212"/>
+      <c r="C1" s="212"/>
     </row>
     <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="16" t="s">

</xml_diff>

<commit_message>
Vacunas actualizado 19-08-2020 a 18:56
</commit_message>
<xml_diff>
--- a/Tutoriales/pandas/Comandos Pandas.xlsx
+++ b/Tutoriales/pandas/Comandos Pandas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoseMaría\Documents\CURSOS\data_science\mitrabajo\mi_repositorio\Tutoriales\pandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297C0154-DC18-4690-B694-71AD3C30DDE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2F665C-E0E6-4DFA-A935-6CE07B4D8E91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF4018AA-EEB9-4756-B82D-183D37B3B80A}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="CONCEPTOS" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GENERALES!$A$2:$D$214</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GENERALES!$A$2:$D$216</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="650">
   <si>
     <t>FUNCIONES DE PANDAS</t>
   </si>
@@ -6497,6 +6497,37 @@
   </si>
   <si>
     <t>Cambia el nombre de las columnas que yo elija</t>
+  </si>
+  <si>
+    <t>resident_age1.reindex([0,9,1,2,3,4,5,6,7,8,10,11,12,13,14,15,16,17,18,19,20])</t>
+  </si>
+  <si>
+    <t>He cambiado la posición de la fila que estaba en 9 a la segunda posicion</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>gasto_vacunas_def</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>["Total empadronados CAM"]=x</t>
+    </r>
+  </si>
+  <si>
+    <t>Añado a la tabla gasto vacunas una columna total empadronados con los valores de una lista (de otra tabla) comprendida en la variable x</t>
   </si>
 </sst>
 </file>
@@ -7601,6 +7632,12 @@
     <xf numFmtId="0" fontId="31" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7641,12 +7678,6 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9953,10 +9984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265136A6-C067-4B28-9F45-A6266FF6FD67}">
-  <dimension ref="A1:D223"/>
+  <dimension ref="A1:D225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:XFD56"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52:B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9968,12 +9999,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="33.75" customHeight="1">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="200" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="102" t="s">
@@ -10687,32 +10718,32 @@
         <v>570</v>
       </c>
     </row>
-    <row r="53" spans="1:4" s="3" customFormat="1">
-      <c r="A53" s="7" t="s">
+    <row r="53" spans="1:4" s="4" customFormat="1" ht="30">
+      <c r="A53" s="142" t="s">
+        <v>489</v>
+      </c>
+      <c r="B53" s="72" t="s">
+        <v>270</v>
+      </c>
+      <c r="C53" s="143" t="s">
+        <v>648</v>
+      </c>
+      <c r="D53" s="144" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="3" customFormat="1">
+      <c r="A54" s="7" t="s">
         <v>498</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B54" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="C53" s="151" t="s">
+      <c r="C54" s="151" t="s">
         <v>244</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D54" s="12" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="60" t="s">
-        <v>492</v>
-      </c>
-      <c r="B54" s="71" t="s">
-        <v>343</v>
-      </c>
-      <c r="C54" s="61" t="s">
-        <v>190</v>
-      </c>
-      <c r="D54" s="61" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -10720,55 +10751,55 @@
         <v>492</v>
       </c>
       <c r="B55" s="71" t="s">
+        <v>343</v>
+      </c>
+      <c r="C55" s="61" t="s">
+        <v>190</v>
+      </c>
+      <c r="D55" s="61" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="60" t="s">
+        <v>492</v>
+      </c>
+      <c r="B56" s="71" t="s">
         <v>347</v>
       </c>
-      <c r="C55" s="61" t="s">
+      <c r="C56" s="61" t="s">
         <v>346</v>
       </c>
-      <c r="D55" s="61" t="s">
+      <c r="D56" s="61" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="56" spans="1:4" s="4" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A56" s="141" t="s">
+    <row r="57" spans="1:4" s="4" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A57" s="141" t="s">
         <v>492</v>
       </c>
-      <c r="B56" s="214" t="s">
+      <c r="B57" s="199" t="s">
         <v>347</v>
       </c>
-      <c r="C56" s="188" t="s">
+      <c r="C57" s="188" t="s">
         <v>644</v>
       </c>
-      <c r="D56" s="213" t="s">
+      <c r="D57" s="198" t="s">
         <v>645</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="B57" s="71" t="s">
-        <v>480</v>
-      </c>
-      <c r="C57" s="61" t="s">
-        <v>377</v>
-      </c>
-      <c r="D57" s="61" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="60" t="s">
-        <v>478</v>
+        <v>39</v>
       </c>
       <c r="B58" s="71" t="s">
-        <v>475</v>
-      </c>
-      <c r="C58" s="85" t="s">
-        <v>67</v>
-      </c>
-      <c r="D58" s="103" t="s">
-        <v>68</v>
+        <v>480</v>
+      </c>
+      <c r="C58" s="61" t="s">
+        <v>377</v>
+      </c>
+      <c r="D58" s="61" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -10776,13 +10807,13 @@
         <v>478</v>
       </c>
       <c r="B59" s="71" t="s">
-        <v>6</v>
+        <v>475</v>
       </c>
       <c r="C59" s="85" t="s">
-        <v>115</v>
+        <v>67</v>
       </c>
       <c r="D59" s="103" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -10793,10 +10824,10 @@
         <v>6</v>
       </c>
       <c r="C60" s="85" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D60" s="103" t="s">
-        <v>477</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -10807,10 +10838,10 @@
         <v>6</v>
       </c>
       <c r="C61" s="85" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D61" s="103" t="s">
-        <v>134</v>
+        <v>477</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -10821,10 +10852,10 @@
         <v>6</v>
       </c>
       <c r="C62" s="85" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D62" s="103" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -10835,10 +10866,10 @@
         <v>6</v>
       </c>
       <c r="C63" s="85" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D63" s="103" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -10849,10 +10880,10 @@
         <v>6</v>
       </c>
       <c r="C64" s="85" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="D64" s="103" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -10860,13 +10891,13 @@
         <v>478</v>
       </c>
       <c r="B65" s="71" t="s">
-        <v>114</v>
+        <v>6</v>
       </c>
       <c r="C65" s="85" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="D65" s="103" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -10877,10 +10908,10 @@
         <v>114</v>
       </c>
       <c r="C66" s="85" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D66" s="103" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -10891,10 +10922,10 @@
         <v>114</v>
       </c>
       <c r="C67" s="85" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D67" s="103" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -10905,10 +10936,10 @@
         <v>114</v>
       </c>
       <c r="C68" s="85" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="D68" s="103" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -10919,10 +10950,10 @@
         <v>114</v>
       </c>
       <c r="C69" s="85" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="D69" s="103" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -10933,10 +10964,10 @@
         <v>114</v>
       </c>
       <c r="C70" s="85" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D70" s="103" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -10947,10 +10978,10 @@
         <v>114</v>
       </c>
       <c r="C71" s="85" t="s">
-        <v>637</v>
+        <v>142</v>
       </c>
       <c r="D71" s="103" t="s">
-        <v>638</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -10961,24 +10992,24 @@
         <v>114</v>
       </c>
       <c r="C72" s="85" t="s">
+        <v>637</v>
+      </c>
+      <c r="D72" s="103" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="60" t="s">
+        <v>478</v>
+      </c>
+      <c r="B73" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="C73" s="85" t="s">
         <v>144</v>
       </c>
-      <c r="D72" s="108" t="s">
+      <c r="D73" s="108" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="104" t="s">
-        <v>472</v>
-      </c>
-      <c r="B73" s="109" t="s">
-        <v>479</v>
-      </c>
-      <c r="C73" s="105" t="s">
-        <v>154</v>
-      </c>
-      <c r="D73" s="106" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -10989,10 +11020,10 @@
         <v>479</v>
       </c>
       <c r="C74" s="105" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D74" s="106" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -11003,10 +11034,10 @@
         <v>479</v>
       </c>
       <c r="C75" s="105" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D75" s="106" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -11016,11 +11047,11 @@
       <c r="B76" s="109" t="s">
         <v>479</v>
       </c>
-      <c r="C76" s="146" t="s">
-        <v>94</v>
-      </c>
-      <c r="D76" s="146" t="s">
-        <v>95</v>
+      <c r="C76" s="105" t="s">
+        <v>160</v>
+      </c>
+      <c r="D76" s="106" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -11028,13 +11059,13 @@
         <v>472</v>
       </c>
       <c r="B77" s="109" t="s">
-        <v>184</v>
-      </c>
-      <c r="C77" s="105" t="s">
-        <v>185</v>
-      </c>
-      <c r="D77" s="106" t="s">
-        <v>186</v>
+        <v>479</v>
+      </c>
+      <c r="C77" s="146" t="s">
+        <v>94</v>
+      </c>
+      <c r="D77" s="146" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -11042,13 +11073,13 @@
         <v>472</v>
       </c>
       <c r="B78" s="109" t="s">
-        <v>114</v>
+        <v>184</v>
       </c>
       <c r="C78" s="105" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="D78" s="106" t="s">
-        <v>159</v>
+        <v>186</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -11059,10 +11090,10 @@
         <v>114</v>
       </c>
       <c r="C79" s="105" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D79" s="106" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -11070,13 +11101,13 @@
         <v>472</v>
       </c>
       <c r="B80" s="109" t="s">
-        <v>490</v>
-      </c>
-      <c r="C80" s="146" t="s">
-        <v>96</v>
-      </c>
-      <c r="D80" s="146" t="s">
-        <v>97</v>
+        <v>114</v>
+      </c>
+      <c r="C80" s="105" t="s">
+        <v>163</v>
+      </c>
+      <c r="D80" s="106" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -11084,27 +11115,27 @@
         <v>472</v>
       </c>
       <c r="B81" s="109" t="s">
+        <v>490</v>
+      </c>
+      <c r="C81" s="146" t="s">
+        <v>96</v>
+      </c>
+      <c r="D81" s="146" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="104" t="s">
+        <v>472</v>
+      </c>
+      <c r="B82" s="109" t="s">
         <v>491</v>
       </c>
-      <c r="C81" s="146" t="s">
+      <c r="C82" s="146" t="s">
         <v>247</v>
       </c>
-      <c r="D81" s="146" t="s">
+      <c r="D82" s="146" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" s="79" t="s">
-        <v>484</v>
-      </c>
-      <c r="B82" s="76" t="s">
-        <v>71</v>
-      </c>
-      <c r="C82" s="77" t="s">
-        <v>83</v>
-      </c>
-      <c r="D82" s="77" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -11112,55 +11143,55 @@
         <v>484</v>
       </c>
       <c r="B83" s="76" t="s">
-        <v>84</v>
-      </c>
-      <c r="C83" s="78" t="s">
-        <v>81</v>
+        <v>71</v>
+      </c>
+      <c r="C83" s="77" t="s">
+        <v>83</v>
       </c>
       <c r="D83" s="77" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="79" t="s">
+        <v>484</v>
+      </c>
+      <c r="B84" s="76" t="s">
+        <v>84</v>
+      </c>
+      <c r="C84" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="D84" s="77" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="79" t="s">
         <v>483</v>
       </c>
-      <c r="B84" s="76" t="s">
+      <c r="B85" s="76" t="s">
         <v>386</v>
       </c>
-      <c r="C84" s="77" t="s">
+      <c r="C85" s="77" t="s">
         <v>385</v>
       </c>
-      <c r="D84" s="77" t="s">
+      <c r="D85" s="77" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="85" spans="1:4" s="4" customFormat="1" ht="30">
-      <c r="A85" s="124" t="s">
+    <row r="86" spans="1:4" s="4" customFormat="1" ht="30">
+      <c r="A86" s="124" t="s">
         <v>483</v>
       </c>
-      <c r="B85" s="125" t="s">
+      <c r="B86" s="125" t="s">
         <v>45</v>
       </c>
-      <c r="C85" s="126" t="s">
+      <c r="C86" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="D85" s="126" t="s">
+      <c r="D86" s="126" t="s">
         <v>350</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="79" t="s">
-        <v>481</v>
-      </c>
-      <c r="B86" s="76" t="s">
-        <v>118</v>
-      </c>
-      <c r="C86" s="77" t="s">
-        <v>539</v>
-      </c>
-      <c r="D86" s="77" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -11168,13 +11199,13 @@
         <v>481</v>
       </c>
       <c r="B87" s="76" t="s">
-        <v>26</v>
+        <v>118</v>
       </c>
       <c r="C87" s="77" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D87" s="77" t="s">
-        <v>117</v>
+        <v>28</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -11185,80 +11216,80 @@
         <v>26</v>
       </c>
       <c r="C88" s="77" t="s">
-        <v>120</v>
+        <v>540</v>
       </c>
       <c r="D88" s="77" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="79" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B89" s="76" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="C89" s="77" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="D89" s="77" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="79" t="s">
-        <v>612</v>
-      </c>
-      <c r="B90" s="79" t="s">
-        <v>613</v>
+        <v>482</v>
+      </c>
+      <c r="B90" s="76" t="s">
+        <v>53</v>
       </c>
       <c r="C90" s="77" t="s">
-        <v>615</v>
+        <v>52</v>
       </c>
       <c r="D90" s="77" t="s">
-        <v>614</v>
+        <v>54</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="79" t="s">
-        <v>487</v>
-      </c>
-      <c r="B91" s="76" t="s">
-        <v>122</v>
+        <v>612</v>
+      </c>
+      <c r="B91" s="79" t="s">
+        <v>613</v>
       </c>
       <c r="C91" s="77" t="s">
-        <v>601</v>
-      </c>
-      <c r="D91" s="128" t="s">
-        <v>602</v>
+        <v>615</v>
+      </c>
+      <c r="D91" s="77" t="s">
+        <v>614</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="79" t="s">
-        <v>249</v>
+        <v>487</v>
       </c>
       <c r="B92" s="76" t="s">
-        <v>230</v>
+        <v>122</v>
       </c>
       <c r="C92" s="77" t="s">
-        <v>246</v>
-      </c>
-      <c r="D92" s="77" t="s">
-        <v>229</v>
+        <v>601</v>
+      </c>
+      <c r="D92" s="128" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="79" t="s">
-        <v>210</v>
+        <v>249</v>
       </c>
       <c r="B93" s="76" t="s">
-        <v>209</v>
+        <v>230</v>
       </c>
       <c r="C93" s="77" t="s">
-        <v>211</v>
+        <v>246</v>
       </c>
       <c r="D93" s="77" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -11266,13 +11297,13 @@
         <v>210</v>
       </c>
       <c r="B94" s="76" t="s">
-        <v>212</v>
-      </c>
-      <c r="C94" s="78" t="s">
-        <v>525</v>
+        <v>209</v>
+      </c>
+      <c r="C94" s="77" t="s">
+        <v>211</v>
       </c>
       <c r="D94" s="77" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -11280,13 +11311,13 @@
         <v>210</v>
       </c>
       <c r="B95" s="76" t="s">
-        <v>232</v>
-      </c>
-      <c r="C95" s="77" t="s">
-        <v>245</v>
+        <v>212</v>
+      </c>
+      <c r="C95" s="78" t="s">
+        <v>525</v>
       </c>
       <c r="D95" s="77" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -11294,13 +11325,13 @@
         <v>210</v>
       </c>
       <c r="B96" s="76" t="s">
-        <v>528</v>
+        <v>232</v>
       </c>
       <c r="C96" s="77" t="s">
-        <v>526</v>
+        <v>245</v>
       </c>
       <c r="D96" s="77" t="s">
-        <v>527</v>
+        <v>231</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -11308,13 +11339,13 @@
         <v>210</v>
       </c>
       <c r="B97" s="76" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C97" s="77" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D97" s="77" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -11322,13 +11353,13 @@
         <v>210</v>
       </c>
       <c r="B98" s="76" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C98" s="77" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D98" s="77" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -11336,41 +11367,41 @@
         <v>210</v>
       </c>
       <c r="B99" s="76" t="s">
+        <v>534</v>
+      </c>
+      <c r="C99" s="77" t="s">
+        <v>532</v>
+      </c>
+      <c r="D99" s="77" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="79" t="s">
+        <v>210</v>
+      </c>
+      <c r="B100" s="76" t="s">
         <v>537</v>
       </c>
-      <c r="C99" s="77" t="s">
+      <c r="C100" s="77" t="s">
         <v>535</v>
       </c>
-      <c r="D99" s="77" t="s">
+      <c r="D100" s="77" t="s">
         <v>536</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="80" t="s">
-        <v>357</v>
-      </c>
-      <c r="B100" s="174" t="s">
-        <v>566</v>
-      </c>
-      <c r="C100" s="173" t="s">
-        <v>567</v>
-      </c>
-      <c r="D100" s="81" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="80" t="s">
         <v>357</v>
       </c>
-      <c r="B101" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="C101" s="81" t="s">
-        <v>78</v>
+      <c r="B101" s="174" t="s">
+        <v>566</v>
+      </c>
+      <c r="C101" s="173" t="s">
+        <v>567</v>
       </c>
       <c r="D101" s="81" t="s">
-        <v>556</v>
+        <v>568</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -11381,38 +11412,38 @@
         <v>79</v>
       </c>
       <c r="C102" s="81" t="s">
-        <v>351</v>
+        <v>78</v>
       </c>
       <c r="D102" s="81" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" s="4" customFormat="1" ht="30">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103" s="80" t="s">
         <v>357</v>
       </c>
-      <c r="B103" s="112" t="s">
+      <c r="B103" s="82" t="s">
         <v>79</v>
       </c>
-      <c r="C103" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="D103" s="9" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
+      <c r="C103" s="81" t="s">
+        <v>351</v>
+      </c>
+      <c r="D103" s="81" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" s="4" customFormat="1" ht="30">
       <c r="A104" s="80" t="s">
         <v>357</v>
       </c>
-      <c r="B104" s="110" t="s">
-        <v>380</v>
-      </c>
-      <c r="C104" s="98" t="s">
-        <v>381</v>
-      </c>
-      <c r="D104" s="111" t="s">
-        <v>382</v>
+      <c r="B104" s="112" t="s">
+        <v>79</v>
+      </c>
+      <c r="C104" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="D104" s="9" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -11423,38 +11454,38 @@
         <v>380</v>
       </c>
       <c r="C105" s="98" t="s">
+        <v>381</v>
+      </c>
+      <c r="D105" s="111" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="80" t="s">
+        <v>357</v>
+      </c>
+      <c r="B106" s="110" t="s">
+        <v>380</v>
+      </c>
+      <c r="C106" s="98" t="s">
         <v>383</v>
       </c>
-      <c r="D105" s="111" t="s">
+      <c r="D106" s="111" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="114" t="s">
-        <v>486</v>
-      </c>
-      <c r="B106" s="113" t="s">
-        <v>40</v>
-      </c>
-      <c r="C106" s="115" t="s">
-        <v>37</v>
-      </c>
-      <c r="D106" s="115" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" s="3" customFormat="1">
+    <row r="107" spans="1:4">
       <c r="A107" s="114" t="s">
         <v>486</v>
       </c>
-      <c r="B107" s="145" t="s">
-        <v>269</v>
-      </c>
-      <c r="C107" s="116" t="s">
-        <v>263</v>
-      </c>
-      <c r="D107" s="117" t="s">
-        <v>261</v>
+      <c r="B107" s="113" t="s">
+        <v>40</v>
+      </c>
+      <c r="C107" s="115" t="s">
+        <v>37</v>
+      </c>
+      <c r="D107" s="115" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="108" spans="1:4" s="3" customFormat="1">
@@ -11465,10 +11496,10 @@
         <v>269</v>
       </c>
       <c r="C108" s="116" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D108" s="117" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="109" spans="1:4" s="3" customFormat="1">
@@ -11476,13 +11507,13 @@
         <v>486</v>
       </c>
       <c r="B109" s="145" t="s">
-        <v>256</v>
-      </c>
-      <c r="C109" s="118" t="s">
-        <v>258</v>
+        <v>269</v>
+      </c>
+      <c r="C109" s="116" t="s">
+        <v>264</v>
       </c>
       <c r="D109" s="117" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
     </row>
     <row r="110" spans="1:4" s="3" customFormat="1">
@@ -11490,13 +11521,13 @@
         <v>486</v>
       </c>
       <c r="B110" s="145" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="C110" s="118" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="D110" s="117" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="111" spans="1:4" s="3" customFormat="1">
@@ -11507,38 +11538,38 @@
         <v>266</v>
       </c>
       <c r="C111" s="118" t="s">
+        <v>265</v>
+      </c>
+      <c r="D111" s="117" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" s="3" customFormat="1">
+      <c r="A112" s="114" t="s">
+        <v>486</v>
+      </c>
+      <c r="B112" s="145" t="s">
+        <v>266</v>
+      </c>
+      <c r="C112" s="118" t="s">
         <v>259</v>
       </c>
-      <c r="D111" s="117" t="s">
+      <c r="D112" s="117" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="112" spans="1:4" s="4" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A112" s="119" t="s">
-        <v>493</v>
-      </c>
-      <c r="B112" s="120" t="s">
-        <v>220</v>
-      </c>
-      <c r="C112" s="121" t="s">
-        <v>485</v>
-      </c>
-      <c r="D112" s="122" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" s="4" customFormat="1" ht="39.75" customHeight="1">
       <c r="A113" s="119" t="s">
         <v>493</v>
       </c>
-      <c r="B113" s="35" t="s">
-        <v>147</v>
-      </c>
-      <c r="C113" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="D113" s="36" t="s">
-        <v>109</v>
+      <c r="B113" s="120" t="s">
+        <v>220</v>
+      </c>
+      <c r="C113" s="121" t="s">
+        <v>485</v>
+      </c>
+      <c r="D113" s="122" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -11546,13 +11577,13 @@
         <v>493</v>
       </c>
       <c r="B114" s="35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C114" s="36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D114" s="36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -11560,13 +11591,13 @@
         <v>493</v>
       </c>
       <c r="B115" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C115" s="36" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D115" s="36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -11574,93 +11605,93 @@
         <v>493</v>
       </c>
       <c r="B116" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="C116" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D116" s="36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="119" t="s">
+        <v>493</v>
+      </c>
+      <c r="B117" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="C116" s="36" t="s">
+      <c r="C117" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="D116" s="36" t="s">
+      <c r="D117" s="36" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15.75">
-      <c r="A117" s="167" t="s">
+    <row r="118" spans="1:4" ht="15.75">
+      <c r="A118" s="167" t="s">
         <v>497</v>
       </c>
-      <c r="B117" s="167" t="s">
+      <c r="B118" s="167" t="s">
         <v>215</v>
       </c>
-      <c r="C117" s="171" t="s">
+      <c r="C118" s="171" t="s">
         <v>563</v>
       </c>
-      <c r="D117" s="168" t="s">
+      <c r="D118" s="168" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="30">
-      <c r="A118" s="169" t="s">
+    <row r="119" spans="1:4" ht="30">
+      <c r="A119" s="169" t="s">
         <v>497</v>
       </c>
-      <c r="B118" s="169" t="s">
+      <c r="B119" s="169" t="s">
         <v>215</v>
       </c>
-      <c r="C118" s="172" t="s">
+      <c r="C119" s="172" t="s">
         <v>564</v>
       </c>
-      <c r="D118" s="170" t="s">
+      <c r="D119" s="170" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="31.5">
-      <c r="A119" s="169"/>
-      <c r="B119" s="169"/>
-      <c r="C119" s="172" t="s">
+    <row r="120" spans="1:4" ht="31.5">
+      <c r="A120" s="169"/>
+      <c r="B120" s="169"/>
+      <c r="C120" s="172" t="s">
         <v>639</v>
       </c>
-      <c r="D119" s="170" t="s">
+      <c r="D120" s="170" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="31.5">
-      <c r="A120" s="169" t="s">
+    <row r="121" spans="1:4" ht="31.5">
+      <c r="A121" s="169" t="s">
         <v>497</v>
       </c>
-      <c r="B120" s="169" t="s">
+      <c r="B121" s="169" t="s">
         <v>215</v>
       </c>
-      <c r="C120" s="172" t="s">
+      <c r="C121" s="172" t="s">
         <v>608</v>
       </c>
-      <c r="D120" s="170" t="s">
+      <c r="D121" s="170" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="121" spans="1:4" s="3" customFormat="1">
-      <c r="A121" s="152" t="s">
+    <row r="122" spans="1:4" s="3" customFormat="1">
+      <c r="A122" s="152" t="s">
         <v>39</v>
       </c>
-      <c r="B121" s="153" t="s">
+      <c r="B122" s="153" t="s">
         <v>242</v>
       </c>
-      <c r="C121" s="154" t="s">
+      <c r="C122" s="154" t="s">
         <v>244</v>
       </c>
-      <c r="D121" s="155" t="s">
+      <c r="D122" s="155" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4">
-      <c r="A122" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="B122" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="C122" s="61" t="s">
-        <v>42</v>
-      </c>
-      <c r="D122" s="61" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -11671,10 +11702,10 @@
         <v>41</v>
       </c>
       <c r="C123" s="61" t="s">
-        <v>275</v>
+        <v>42</v>
       </c>
       <c r="D123" s="61" t="s">
-        <v>274</v>
+        <v>43</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -11682,13 +11713,13 @@
         <v>1</v>
       </c>
       <c r="B124" s="71" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C124" s="61" t="s">
-        <v>23</v>
+        <v>275</v>
       </c>
       <c r="D124" s="61" t="s">
-        <v>22</v>
+        <v>274</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -11696,13 +11727,13 @@
         <v>1</v>
       </c>
       <c r="B125" s="71" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C125" s="61" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D125" s="61" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -11710,13 +11741,13 @@
         <v>1</v>
       </c>
       <c r="B126" s="71" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C126" s="61" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D126" s="61" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -11724,13 +11755,13 @@
         <v>1</v>
       </c>
       <c r="B127" s="71" t="s">
-        <v>298</v>
+        <v>47</v>
       </c>
       <c r="C127" s="61" t="s">
-        <v>294</v>
+        <v>46</v>
       </c>
       <c r="D127" s="61" t="s">
-        <v>299</v>
+        <v>48</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -11738,13 +11769,13 @@
         <v>1</v>
       </c>
       <c r="B128" s="71" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C128" s="61" t="s">
-        <v>183</v>
+        <v>294</v>
       </c>
       <c r="D128" s="61" t="s">
-        <v>102</v>
+        <v>299</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -11755,10 +11786,10 @@
         <v>295</v>
       </c>
       <c r="C129" s="61" t="s">
-        <v>104</v>
+        <v>183</v>
       </c>
       <c r="D129" s="61" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -11766,13 +11797,13 @@
         <v>1</v>
       </c>
       <c r="B130" s="71" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C130" s="61" t="s">
-        <v>239</v>
+        <v>104</v>
       </c>
       <c r="D130" s="61" t="s">
-        <v>240</v>
+        <v>103</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -11780,13 +11811,13 @@
         <v>1</v>
       </c>
       <c r="B131" s="71" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C131" s="61" t="s">
-        <v>587</v>
+        <v>239</v>
       </c>
       <c r="D131" s="61" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -11794,13 +11825,13 @@
         <v>1</v>
       </c>
       <c r="B132" s="71" t="s">
-        <v>87</v>
+        <v>297</v>
       </c>
       <c r="C132" s="61" t="s">
-        <v>85</v>
+        <v>587</v>
       </c>
       <c r="D132" s="61" t="s">
-        <v>86</v>
+        <v>241</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -11808,13 +11839,13 @@
         <v>1</v>
       </c>
       <c r="B133" s="71" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="C133" s="61" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="D133" s="61" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -11822,13 +11853,13 @@
         <v>1</v>
       </c>
       <c r="B134" s="71" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C134" s="61" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D134" s="61" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -11836,13 +11867,13 @@
         <v>1</v>
       </c>
       <c r="B135" s="71" t="s">
-        <v>280</v>
-      </c>
-      <c r="C135" s="83" t="s">
-        <v>281</v>
-      </c>
-      <c r="D135" s="83" t="s">
-        <v>282</v>
+        <v>49</v>
+      </c>
+      <c r="C135" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="D135" s="61" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -11850,13 +11881,13 @@
         <v>1</v>
       </c>
       <c r="B136" s="71" t="s">
-        <v>499</v>
-      </c>
-      <c r="C136" s="61" t="s">
-        <v>69</v>
-      </c>
-      <c r="D136" s="61" t="s">
-        <v>70</v>
+        <v>280</v>
+      </c>
+      <c r="C136" s="83" t="s">
+        <v>281</v>
+      </c>
+      <c r="D136" s="83" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -11864,13 +11895,13 @@
         <v>1</v>
       </c>
       <c r="B137" s="71" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C137" s="61" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D137" s="61" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -11881,10 +11912,10 @@
         <v>500</v>
       </c>
       <c r="C138" s="61" t="s">
-        <v>167</v>
+        <v>73</v>
       </c>
       <c r="D138" s="61" t="s">
-        <v>166</v>
+        <v>74</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -11892,13 +11923,13 @@
         <v>1</v>
       </c>
       <c r="B139" s="71" t="s">
-        <v>76</v>
+        <v>500</v>
       </c>
       <c r="C139" s="61" t="s">
-        <v>75</v>
+        <v>167</v>
       </c>
       <c r="D139" s="61" t="s">
-        <v>77</v>
+        <v>166</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -11909,10 +11940,10 @@
         <v>76</v>
       </c>
       <c r="C140" s="61" t="s">
-        <v>164</v>
+        <v>75</v>
       </c>
       <c r="D140" s="61" t="s">
-        <v>165</v>
+        <v>77</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -11923,10 +11954,10 @@
         <v>76</v>
       </c>
       <c r="C141" s="61" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D141" s="61" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -11936,11 +11967,11 @@
       <c r="B142" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="C142" s="84" t="s">
-        <v>562</v>
+      <c r="C142" s="61" t="s">
+        <v>169</v>
       </c>
       <c r="D142" s="61" t="s">
-        <v>238</v>
+        <v>168</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -11948,13 +11979,13 @@
         <v>1</v>
       </c>
       <c r="B143" s="71" t="s">
-        <v>170</v>
-      </c>
-      <c r="C143" s="61" t="s">
-        <v>172</v>
+        <v>76</v>
+      </c>
+      <c r="C143" s="84" t="s">
+        <v>562</v>
       </c>
       <c r="D143" s="61" t="s">
-        <v>171</v>
+        <v>238</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -11962,13 +11993,13 @@
         <v>1</v>
       </c>
       <c r="B144" s="71" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C144" s="61" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D144" s="61" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -11976,13 +12007,13 @@
         <v>1</v>
       </c>
       <c r="B145" s="71" t="s">
-        <v>218</v>
+        <v>174</v>
       </c>
       <c r="C145" s="61" t="s">
-        <v>217</v>
+        <v>173</v>
       </c>
       <c r="D145" s="61" t="s">
-        <v>219</v>
+        <v>175</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -11990,13 +12021,13 @@
         <v>1</v>
       </c>
       <c r="B146" s="71" t="s">
-        <v>227</v>
-      </c>
-      <c r="C146" s="85" t="s">
-        <v>228</v>
+        <v>218</v>
+      </c>
+      <c r="C146" s="61" t="s">
+        <v>217</v>
       </c>
       <c r="D146" s="61" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -12004,13 +12035,13 @@
         <v>1</v>
       </c>
       <c r="B147" s="71" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C147" s="85" t="s">
-        <v>365</v>
+        <v>228</v>
       </c>
       <c r="D147" s="61" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -12018,13 +12049,13 @@
         <v>1</v>
       </c>
       <c r="B148" s="71" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C148" s="85" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D148" s="61" t="s">
-        <v>364</v>
+        <v>234</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -12035,24 +12066,24 @@
         <v>235</v>
       </c>
       <c r="C149" s="85" t="s">
+        <v>363</v>
+      </c>
+      <c r="D149" s="61" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B150" s="71" t="s">
+        <v>235</v>
+      </c>
+      <c r="C150" s="85" t="s">
         <v>236</v>
       </c>
-      <c r="D149" s="61" t="s">
+      <c r="D150" s="61" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4">
-      <c r="A150" s="80" t="s">
-        <v>80</v>
-      </c>
-      <c r="B150" s="82" t="s">
-        <v>106</v>
-      </c>
-      <c r="C150" s="81" t="s">
-        <v>107</v>
-      </c>
-      <c r="D150" s="81" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -12060,13 +12091,13 @@
         <v>80</v>
       </c>
       <c r="B151" s="82" t="s">
-        <v>181</v>
+        <v>106</v>
       </c>
       <c r="C151" s="81" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D151" s="81" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -12074,13 +12105,13 @@
         <v>80</v>
       </c>
       <c r="B152" s="82" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C152" s="81" t="s">
-        <v>288</v>
+        <v>99</v>
       </c>
       <c r="D152" s="81" t="s">
-        <v>180</v>
+        <v>98</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -12088,13 +12119,13 @@
         <v>80</v>
       </c>
       <c r="B153" s="82" t="s">
-        <v>421</v>
+        <v>182</v>
       </c>
       <c r="C153" s="81" t="s">
-        <v>422</v>
+        <v>288</v>
       </c>
       <c r="D153" s="81" t="s">
-        <v>420</v>
+        <v>180</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -12102,13 +12133,13 @@
         <v>80</v>
       </c>
       <c r="B154" s="82" t="s">
-        <v>199</v>
+        <v>421</v>
       </c>
       <c r="C154" s="81" t="s">
-        <v>198</v>
+        <v>422</v>
       </c>
       <c r="D154" s="81" t="s">
-        <v>200</v>
+        <v>420</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -12119,10 +12150,10 @@
         <v>199</v>
       </c>
       <c r="C155" s="81" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D155" s="81" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -12133,10 +12164,10 @@
         <v>199</v>
       </c>
       <c r="C156" s="81" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D156" s="81" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -12144,16 +12175,16 @@
         <v>80</v>
       </c>
       <c r="B157" s="82" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C157" s="81" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="D157" s="81" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" ht="15.75">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
       <c r="A158" s="80" t="s">
         <v>80</v>
       </c>
@@ -12161,52 +12192,52 @@
         <v>205</v>
       </c>
       <c r="C158" s="81" t="s">
-        <v>576</v>
-      </c>
-      <c r="D158" s="177" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4">
+        <v>197</v>
+      </c>
+      <c r="D158" s="81" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="15.75">
       <c r="A159" s="80" t="s">
         <v>80</v>
       </c>
       <c r="B159" s="82" t="s">
-        <v>580</v>
+        <v>205</v>
       </c>
       <c r="C159" s="81" t="s">
-        <v>578</v>
-      </c>
-      <c r="D159" s="178" t="s">
-        <v>579</v>
+        <v>576</v>
+      </c>
+      <c r="D159" s="177" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="B160" s="130" t="s">
+      <c r="B160" s="82" t="s">
+        <v>580</v>
+      </c>
+      <c r="C160" s="81" t="s">
+        <v>578</v>
+      </c>
+      <c r="D160" s="178" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" s="80" t="s">
+        <v>80</v>
+      </c>
+      <c r="B161" s="130" t="s">
         <v>205</v>
       </c>
-      <c r="C160" s="131" t="s">
+      <c r="C161" s="131" t="s">
         <v>207</v>
       </c>
-      <c r="D160" s="131" t="s">
+      <c r="D161" s="131" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4">
-      <c r="A161" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="B161" s="70" t="s">
-        <v>506</v>
-      </c>
-      <c r="C161" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="D161" s="69" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -12217,10 +12248,10 @@
         <v>506</v>
       </c>
       <c r="C162" s="69" t="s">
-        <v>509</v>
+        <v>66</v>
       </c>
       <c r="D162" s="69" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -12231,10 +12262,10 @@
         <v>506</v>
       </c>
       <c r="C163" s="69" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="D163" s="69" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -12242,13 +12273,13 @@
         <v>8</v>
       </c>
       <c r="B164" s="70" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="C164" s="69" t="s">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="D164" s="69" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -12256,13 +12287,13 @@
         <v>8</v>
       </c>
       <c r="B165" s="70" t="s">
-        <v>447</v>
+        <v>513</v>
       </c>
       <c r="C165" s="69" t="s">
-        <v>287</v>
+        <v>510</v>
       </c>
       <c r="D165" s="69" t="s">
-        <v>443</v>
+        <v>511</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -12273,10 +12304,10 @@
         <v>447</v>
       </c>
       <c r="C166" s="69" t="s">
-        <v>448</v>
+        <v>287</v>
       </c>
       <c r="D166" s="69" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -12284,13 +12315,13 @@
         <v>8</v>
       </c>
       <c r="B167" s="70" t="s">
-        <v>289</v>
+        <v>447</v>
       </c>
       <c r="C167" s="69" t="s">
-        <v>290</v>
+        <v>448</v>
       </c>
       <c r="D167" s="69" t="s">
-        <v>291</v>
+        <v>446</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -12298,13 +12329,13 @@
         <v>8</v>
       </c>
       <c r="B168" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C168" s="68" t="s">
-        <v>9</v>
+        <v>289</v>
+      </c>
+      <c r="C168" s="69" t="s">
+        <v>290</v>
       </c>
       <c r="D168" s="69" t="s">
-        <v>11</v>
+        <v>291</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -12315,10 +12346,10 @@
         <v>8</v>
       </c>
       <c r="C169" s="68" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D169" s="69" t="s">
-        <v>65</v>
+        <v>11</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -12329,10 +12360,10 @@
         <v>8</v>
       </c>
       <c r="C170" s="68" t="s">
-        <v>390</v>
+        <v>20</v>
       </c>
       <c r="D170" s="69" t="s">
-        <v>391</v>
+        <v>65</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -12343,10 +12374,10 @@
         <v>8</v>
       </c>
       <c r="C171" s="68" t="s">
-        <v>9</v>
+        <v>390</v>
       </c>
       <c r="D171" s="69" t="s">
-        <v>11</v>
+        <v>391</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -12357,10 +12388,10 @@
         <v>8</v>
       </c>
       <c r="C172" s="68" t="s">
-        <v>359</v>
+        <v>9</v>
       </c>
       <c r="D172" s="69" t="s">
-        <v>360</v>
+        <v>11</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -12371,10 +12402,10 @@
         <v>8</v>
       </c>
       <c r="C173" s="68" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D173" s="69" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -12382,13 +12413,13 @@
         <v>8</v>
       </c>
       <c r="B174" s="70" t="s">
-        <v>438</v>
+        <v>8</v>
       </c>
       <c r="C174" s="68" t="s">
         <v>361</v>
       </c>
       <c r="D174" s="69" t="s">
-        <v>437</v>
+        <v>362</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -12396,97 +12427,97 @@
         <v>8</v>
       </c>
       <c r="B175" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C175" s="68" t="s">
+        <v>646</v>
+      </c>
+      <c r="D175" s="69" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="B176" s="70" t="s">
         <v>438</v>
       </c>
-      <c r="C175" s="68" t="s">
+      <c r="C176" s="68" t="s">
         <v>361</v>
       </c>
-      <c r="D175" s="69" t="s">
+      <c r="D176" s="69" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="B177" s="70" t="s">
+        <v>438</v>
+      </c>
+      <c r="C177" s="68" t="s">
+        <v>361</v>
+      </c>
+      <c r="D177" s="69" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="176" spans="1:4">
-      <c r="A176" s="71" t="s">
-        <v>327</v>
-      </c>
-      <c r="B176" s="60" t="s">
-        <v>501</v>
-      </c>
-      <c r="C176" s="61" t="s">
-        <v>176</v>
-      </c>
-      <c r="D176" s="61" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A177" s="71" t="s">
-        <v>327</v>
-      </c>
-      <c r="B177" s="129" t="s">
-        <v>432</v>
-      </c>
-      <c r="C177" s="12" t="s">
-        <v>423</v>
-      </c>
-      <c r="D177" s="12" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" s="3" customFormat="1" ht="30">
+    <row r="178" spans="1:4">
       <c r="A178" s="71" t="s">
         <v>327</v>
       </c>
-      <c r="B178" s="129" t="s">
-        <v>432</v>
-      </c>
-      <c r="C178" s="12" t="s">
-        <v>444</v>
-      </c>
-      <c r="D178" s="12" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A179" s="72" t="s">
+      <c r="B178" s="60" t="s">
+        <v>501</v>
+      </c>
+      <c r="C178" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="D178" s="61" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A179" s="71" t="s">
         <v>327</v>
       </c>
       <c r="B179" s="129" t="s">
         <v>432</v>
       </c>
-      <c r="C179" s="62" t="s">
-        <v>349</v>
+      <c r="C179" s="12" t="s">
+        <v>423</v>
       </c>
       <c r="D179" s="12" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A180" s="72" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" s="3" customFormat="1" ht="30">
+      <c r="A180" s="71" t="s">
         <v>327</v>
       </c>
       <c r="B180" s="129" t="s">
         <v>432</v>
       </c>
-      <c r="C180" s="62" t="s">
-        <v>424</v>
+      <c r="C180" s="12" t="s">
+        <v>444</v>
       </c>
       <c r="D180" s="12" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" s="3" customFormat="1" ht="76.5" customHeight="1">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
       <c r="A181" s="72" t="s">
         <v>327</v>
       </c>
       <c r="B181" s="129" t="s">
-        <v>502</v>
-      </c>
-      <c r="C181" s="12" t="s">
-        <v>330</v>
+        <v>432</v>
+      </c>
+      <c r="C181" s="62" t="s">
+        <v>349</v>
       </c>
       <c r="D181" s="12" t="s">
-        <v>329</v>
+        <v>348</v>
       </c>
     </row>
     <row r="182" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
@@ -12494,55 +12525,55 @@
         <v>327</v>
       </c>
       <c r="B182" s="129" t="s">
-        <v>503</v>
-      </c>
-      <c r="C182" s="12" t="s">
-        <v>331</v>
+        <v>432</v>
+      </c>
+      <c r="C182" s="62" t="s">
+        <v>424</v>
       </c>
       <c r="D182" s="12" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" s="3" customFormat="1" ht="76.5" customHeight="1">
       <c r="A183" s="72" t="s">
         <v>327</v>
       </c>
       <c r="B183" s="129" t="s">
+        <v>502</v>
+      </c>
+      <c r="C183" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="D183" s="12" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
+      <c r="A184" s="72" t="s">
+        <v>327</v>
+      </c>
+      <c r="B184" s="129" t="s">
+        <v>503</v>
+      </c>
+      <c r="C184" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="D184" s="12" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" s="3" customFormat="1" ht="39.75" customHeight="1">
+      <c r="A185" s="72" t="s">
+        <v>327</v>
+      </c>
+      <c r="B185" s="129" t="s">
         <v>426</v>
       </c>
-      <c r="C183" s="12" t="s">
+      <c r="C185" s="12" t="s">
         <v>427</v>
       </c>
-      <c r="D183" s="12" t="s">
+      <c r="D185" s="12" t="s">
         <v>425</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4">
-      <c r="A184" s="74" t="s">
-        <v>187</v>
-      </c>
-      <c r="B184" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="C184" s="11" t="s">
-        <v>328</v>
-      </c>
-      <c r="D184" s="11" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" s="4" customFormat="1" ht="39.75" customHeight="1">
-      <c r="A185" s="74" t="s">
-        <v>187</v>
-      </c>
-      <c r="B185" s="63" t="s">
-        <v>318</v>
-      </c>
-      <c r="C185" s="64" t="s">
-        <v>428</v>
-      </c>
-      <c r="D185" s="65" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -12553,192 +12584,192 @@
         <v>318</v>
       </c>
       <c r="C186" s="11" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="D186" s="11" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" s="4" customFormat="1" ht="39.75" customHeight="1">
       <c r="A187" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="B187" s="10" t="s">
+      <c r="B187" s="63" t="s">
         <v>318</v>
       </c>
-      <c r="C187" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="D187" s="11" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" s="4" customFormat="1">
+      <c r="C187" s="64" t="s">
+        <v>428</v>
+      </c>
+      <c r="D187" s="65" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
       <c r="A188" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="B188" s="73" t="s">
+      <c r="B188" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="C188" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="D188" s="11" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" s="74" t="s">
+        <v>187</v>
+      </c>
+      <c r="B189" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="C189" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="D189" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" s="4" customFormat="1">
+      <c r="A190" s="74" t="s">
+        <v>187</v>
+      </c>
+      <c r="B190" s="73" t="s">
         <v>313</v>
       </c>
-      <c r="C188" s="65" t="s">
+      <c r="C190" s="65" t="s">
         <v>312</v>
       </c>
-      <c r="D188" s="65" t="s">
+      <c r="D190" s="65" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="189" spans="1:4">
-      <c r="A189" s="75" t="s">
+    <row r="191" spans="1:4">
+      <c r="A191" s="75" t="s">
         <v>187</v>
       </c>
-      <c r="B189" s="10" t="s">
+      <c r="B191" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="C189" s="11" t="s">
+      <c r="C191" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="D189" s="65" t="s">
+      <c r="D191" s="65" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="190" spans="1:4">
-      <c r="A190" s="113" t="s">
+    <row r="192" spans="1:4">
+      <c r="A192" s="113" t="s">
         <v>191</v>
       </c>
-      <c r="B190" s="113" t="s">
+      <c r="B192" s="113" t="s">
         <v>189</v>
       </c>
-      <c r="C190" s="115" t="s">
+      <c r="C192" s="115" t="s">
         <v>193</v>
       </c>
-      <c r="D190" s="115" t="s">
+      <c r="D192" s="115" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="191" spans="1:4">
-      <c r="A191" s="113" t="s">
+    <row r="193" spans="1:4">
+      <c r="A193" s="113" t="s">
         <v>191</v>
       </c>
-      <c r="B191" s="113" t="s">
+      <c r="B193" s="113" t="s">
         <v>189</v>
       </c>
-      <c r="C191" s="115" t="s">
+      <c r="C193" s="115" t="s">
         <v>195</v>
       </c>
-      <c r="D191" s="115" t="s">
+      <c r="D193" s="115" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="192" spans="1:4" s="3" customFormat="1">
-      <c r="A192" s="132" t="s">
-        <v>250</v>
-      </c>
-      <c r="B192" s="157" t="s">
-        <v>252</v>
-      </c>
-      <c r="C192" s="133" t="s">
-        <v>253</v>
-      </c>
-      <c r="D192" s="134" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" s="86" customFormat="1">
-      <c r="A193" s="132" t="s">
-        <v>250</v>
-      </c>
-      <c r="B193" s="157" t="s">
-        <v>293</v>
-      </c>
-      <c r="C193" s="133" t="s">
-        <v>292</v>
-      </c>
-      <c r="D193" s="134" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" s="86" customFormat="1">
+    <row r="194" spans="1:4" s="3" customFormat="1">
       <c r="A194" s="132" t="s">
         <v>250</v>
       </c>
       <c r="B194" s="157" t="s">
+        <v>252</v>
+      </c>
+      <c r="C194" s="133" t="s">
+        <v>253</v>
+      </c>
+      <c r="D194" s="134" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" s="86" customFormat="1">
+      <c r="A195" s="132" t="s">
+        <v>250</v>
+      </c>
+      <c r="B195" s="157" t="s">
+        <v>293</v>
+      </c>
+      <c r="C195" s="133" t="s">
+        <v>292</v>
+      </c>
+      <c r="D195" s="134" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" s="86" customFormat="1">
+      <c r="A196" s="132" t="s">
+        <v>250</v>
+      </c>
+      <c r="B196" s="157" t="s">
         <v>286</v>
       </c>
-      <c r="C194" s="133" t="s">
+      <c r="C196" s="133" t="s">
         <v>285</v>
       </c>
-      <c r="D194" s="134" t="s">
+      <c r="D196" s="134" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="195" spans="1:4" s="4" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A195" s="135" t="s">
+    <row r="197" spans="1:4" s="4" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A197" s="135" t="s">
         <v>250</v>
       </c>
-      <c r="B195" s="157" t="s">
+      <c r="B197" s="157" t="s">
         <v>463</v>
       </c>
-      <c r="C195" s="136" t="s">
+      <c r="C197" s="136" t="s">
         <v>376</v>
       </c>
-      <c r="D195" s="137" t="s">
+      <c r="D197" s="137" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="196" spans="1:4" s="38" customFormat="1" ht="144.75" customHeight="1">
-      <c r="A196" s="138" t="s">
-        <v>250</v>
-      </c>
-      <c r="B196" s="158" t="s">
-        <v>504</v>
-      </c>
-      <c r="C196" s="136" t="s">
-        <v>488</v>
-      </c>
-      <c r="D196" s="137" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4">
-      <c r="A197" s="159" t="s">
-        <v>250</v>
-      </c>
-      <c r="B197" s="160" t="s">
-        <v>512</v>
-      </c>
-      <c r="C197" s="161" t="s">
-        <v>514</v>
-      </c>
-      <c r="D197" s="161" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" s="38" customFormat="1" ht="28.5" customHeight="1">
+    <row r="198" spans="1:4" s="38" customFormat="1" ht="144.75" customHeight="1">
       <c r="A198" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B198" s="158" t="s">
-        <v>435</v>
-      </c>
-      <c r="C198" s="139" t="s">
-        <v>458</v>
+        <v>504</v>
+      </c>
+      <c r="C198" s="136" t="s">
+        <v>488</v>
       </c>
       <c r="D198" s="137" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" s="38" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A199" s="138" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" s="159" t="s">
         <v>250</v>
       </c>
-      <c r="B199" s="158" t="s">
-        <v>435</v>
-      </c>
-      <c r="C199" s="139" t="s">
-        <v>459</v>
-      </c>
-      <c r="D199" s="137" t="s">
-        <v>433</v>
+      <c r="B199" s="160" t="s">
+        <v>512</v>
+      </c>
+      <c r="C199" s="161" t="s">
+        <v>514</v>
+      </c>
+      <c r="D199" s="161" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="200" spans="1:4" s="38" customFormat="1" ht="28.5" customHeight="1">
@@ -12746,69 +12777,69 @@
         <v>250</v>
       </c>
       <c r="B200" s="158" t="s">
-        <v>436</v>
-      </c>
-      <c r="C200" s="140" t="s">
-        <v>441</v>
+        <v>435</v>
+      </c>
+      <c r="C200" s="139" t="s">
+        <v>458</v>
       </c>
       <c r="D200" s="137" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" s="4" customFormat="1" ht="38.25" customHeight="1">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" s="38" customFormat="1" ht="28.5" customHeight="1">
       <c r="A201" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B201" s="158" t="s">
-        <v>242</v>
-      </c>
-      <c r="C201" s="136" t="s">
-        <v>457</v>
+        <v>435</v>
+      </c>
+      <c r="C201" s="139" t="s">
+        <v>459</v>
       </c>
       <c r="D201" s="137" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" s="38" customFormat="1" ht="28.5" customHeight="1">
       <c r="A202" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B202" s="158" t="s">
-        <v>440</v>
-      </c>
-      <c r="C202" s="136" t="s">
-        <v>517</v>
+        <v>436</v>
+      </c>
+      <c r="C202" s="140" t="s">
+        <v>441</v>
       </c>
       <c r="D202" s="137" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" s="4" customFormat="1" ht="38.25" customHeight="1">
       <c r="A203" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B203" s="158" t="s">
-        <v>455</v>
+        <v>242</v>
       </c>
       <c r="C203" s="136" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D203" s="137" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1">
       <c r="A204" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B204" s="158" t="s">
-        <v>522</v>
+        <v>440</v>
       </c>
       <c r="C204" s="136" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="D204" s="137" t="s">
-        <v>524</v>
+        <v>451</v>
       </c>
     </row>
     <row r="205" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
@@ -12816,55 +12847,55 @@
         <v>250</v>
       </c>
       <c r="B205" s="158" t="s">
-        <v>520</v>
+        <v>455</v>
       </c>
       <c r="C205" s="136" t="s">
-        <v>519</v>
+        <v>456</v>
       </c>
       <c r="D205" s="137" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
       <c r="A206" s="138" t="s">
         <v>250</v>
       </c>
       <c r="B206" s="158" t="s">
+        <v>522</v>
+      </c>
+      <c r="C206" s="136" t="s">
+        <v>521</v>
+      </c>
+      <c r="D206" s="137" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" s="4" customFormat="1" ht="36.75" customHeight="1">
+      <c r="A207" s="138" t="s">
+        <v>250</v>
+      </c>
+      <c r="B207" s="158" t="s">
+        <v>520</v>
+      </c>
+      <c r="C207" s="136" t="s">
+        <v>519</v>
+      </c>
+      <c r="D207" s="137" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" s="4" customFormat="1" ht="29.25" customHeight="1">
+      <c r="A208" s="138" t="s">
+        <v>250</v>
+      </c>
+      <c r="B208" s="158" t="s">
         <v>454</v>
       </c>
-      <c r="C206" s="136" t="s">
+      <c r="C208" s="136" t="s">
         <v>452</v>
       </c>
-      <c r="D206" s="137" t="s">
+      <c r="D208" s="137" t="s">
         <v>453</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4">
-      <c r="A207" s="123" t="s">
-        <v>222</v>
-      </c>
-      <c r="B207" s="123" t="s">
-        <v>223</v>
-      </c>
-      <c r="C207" s="36" t="s">
-        <v>248</v>
-      </c>
-      <c r="D207" s="36" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4">
-      <c r="A208" s="123" t="s">
-        <v>222</v>
-      </c>
-      <c r="B208" s="123" t="s">
-        <v>223</v>
-      </c>
-      <c r="C208" s="36" t="s">
-        <v>225</v>
-      </c>
-      <c r="D208" s="36" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -12874,11 +12905,11 @@
       <c r="B209" s="123" t="s">
         <v>223</v>
       </c>
-      <c r="C209" s="156" t="s">
-        <v>633</v>
+      <c r="C209" s="36" t="s">
+        <v>248</v>
       </c>
       <c r="D209" s="36" t="s">
-        <v>300</v>
+        <v>224</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -12888,11 +12919,11 @@
       <c r="B210" s="123" t="s">
         <v>223</v>
       </c>
-      <c r="C210" s="156" t="s">
-        <v>306</v>
+      <c r="C210" s="36" t="s">
+        <v>225</v>
       </c>
       <c r="D210" s="36" t="s">
-        <v>302</v>
+        <v>260</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -12900,24 +12931,27 @@
         <v>222</v>
       </c>
       <c r="B211" s="123" t="s">
-        <v>626</v>
-      </c>
-      <c r="C211" s="180" t="s">
-        <v>304</v>
+        <v>223</v>
+      </c>
+      <c r="C211" s="156" t="s">
+        <v>633</v>
       </c>
       <c r="D211" s="36" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="212" spans="1:4">
+      <c r="A212" s="123" t="s">
+        <v>222</v>
+      </c>
       <c r="B212" s="123" t="s">
-        <v>626</v>
-      </c>
-      <c r="C212" s="180" t="s">
-        <v>304</v>
+        <v>223</v>
+      </c>
+      <c r="C212" s="156" t="s">
+        <v>306</v>
       </c>
       <c r="D212" s="36" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -12928,24 +12962,21 @@
         <v>626</v>
       </c>
       <c r="C213" s="180" t="s">
-        <v>634</v>
+        <v>304</v>
       </c>
       <c r="D213" s="36" t="s">
-        <v>635</v>
+        <v>303</v>
       </c>
     </row>
     <row r="214" spans="1:4">
-      <c r="A214" s="123" t="s">
-        <v>222</v>
-      </c>
       <c r="B214" s="123" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C214" s="180" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D214" s="36" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -12953,55 +12984,55 @@
         <v>222</v>
       </c>
       <c r="B215" s="123" t="s">
+        <v>626</v>
+      </c>
+      <c r="C215" s="180" t="s">
+        <v>634</v>
+      </c>
+      <c r="D215" s="36" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4">
+      <c r="A216" s="123" t="s">
+        <v>222</v>
+      </c>
+      <c r="B216" s="123" t="s">
+        <v>628</v>
+      </c>
+      <c r="C216" s="180" t="s">
+        <v>307</v>
+      </c>
+      <c r="D216" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
+      <c r="A217" s="123" t="s">
+        <v>222</v>
+      </c>
+      <c r="B217" s="123" t="s">
         <v>629</v>
       </c>
-      <c r="C215" s="181" t="s">
+      <c r="C217" s="181" t="s">
         <v>393</v>
       </c>
-      <c r="D215" s="36" t="s">
+      <c r="D217" s="36" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="216" spans="1:4" s="179" customFormat="1" ht="15.75">
-      <c r="A216" s="182" t="s">
-        <v>222</v>
-      </c>
-      <c r="B216" s="182" t="s">
-        <v>629</v>
-      </c>
-      <c r="C216" s="183" t="s">
-        <v>583</v>
-      </c>
-      <c r="D216" s="184" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4">
-      <c r="A217" s="182" t="s">
-        <v>222</v>
-      </c>
-      <c r="B217" s="182" t="s">
-        <v>630</v>
-      </c>
-      <c r="C217" s="185" t="s">
-        <v>584</v>
-      </c>
-      <c r="D217" s="186" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4">
+    <row r="218" spans="1:4" s="179" customFormat="1" ht="15.75">
       <c r="A218" s="182" t="s">
         <v>222</v>
       </c>
       <c r="B218" s="182" t="s">
-        <v>631</v>
-      </c>
-      <c r="C218" s="185" t="s">
-        <v>621</v>
-      </c>
-      <c r="D218" s="186" t="s">
-        <v>616</v>
+        <v>629</v>
+      </c>
+      <c r="C218" s="183" t="s">
+        <v>583</v>
+      </c>
+      <c r="D218" s="184" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -13009,13 +13040,13 @@
         <v>222</v>
       </c>
       <c r="B219" s="182" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C219" s="185" t="s">
-        <v>622</v>
+        <v>584</v>
       </c>
       <c r="D219" s="186" t="s">
-        <v>617</v>
+        <v>632</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -13026,10 +13057,10 @@
         <v>631</v>
       </c>
       <c r="C220" s="185" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D220" s="186" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -13040,10 +13071,10 @@
         <v>631</v>
       </c>
       <c r="C221" s="185" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D221" s="186" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -13054,10 +13085,10 @@
         <v>631</v>
       </c>
       <c r="C222" s="185" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D222" s="186" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -13065,17 +13096,45 @@
         <v>222</v>
       </c>
       <c r="B223" s="182" t="s">
+        <v>631</v>
+      </c>
+      <c r="C223" s="185" t="s">
+        <v>624</v>
+      </c>
+      <c r="D223" s="186" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4">
+      <c r="A224" s="182" t="s">
+        <v>222</v>
+      </c>
+      <c r="B224" s="182" t="s">
+        <v>631</v>
+      </c>
+      <c r="C224" s="185" t="s">
+        <v>625</v>
+      </c>
+      <c r="D224" s="186" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4">
+      <c r="A225" s="182" t="s">
+        <v>222</v>
+      </c>
+      <c r="B225" s="182" t="s">
         <v>223</v>
       </c>
-      <c r="C223" s="185" t="s">
+      <c r="C225" s="185" t="s">
         <v>585</v>
       </c>
-      <c r="D223" s="186" t="s">
+      <c r="D225" s="186" t="s">
         <v>586</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D214" xr:uid="{85ED3410-72EE-453D-8BB3-FB7E07F682B1}"/>
+  <autoFilter ref="A2:D216" xr:uid="{85ED3410-72EE-453D-8BB3-FB7E07F682B1}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
@@ -13104,13 +13163,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33.75" customHeight="1">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="202" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="202"/>
+      <c r="B1" s="202"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="203"/>
+      <c r="E1" s="204"/>
     </row>
     <row r="2" spans="1:5" ht="207" customHeight="1">
       <c r="A2" s="43" t="s">
@@ -13357,22 +13416,22 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="408.95" customHeight="1">
-      <c r="A19" s="211" t="s">
+      <c r="A19" s="213" t="s">
         <v>222</v>
       </c>
-      <c r="B19" s="209" t="s">
+      <c r="B19" s="211" t="s">
         <v>592</v>
       </c>
-      <c r="C19" s="203"/>
-      <c r="D19" s="205"/>
-      <c r="E19" s="207"/>
+      <c r="C19" s="205"/>
+      <c r="D19" s="207"/>
+      <c r="E19" s="209"/>
     </row>
     <row r="20" spans="1:5" ht="351.75" customHeight="1">
-      <c r="A20" s="210"/>
-      <c r="B20" s="210"/>
-      <c r="C20" s="204"/>
-      <c r="D20" s="206"/>
-      <c r="E20" s="208"/>
+      <c r="A20" s="212"/>
+      <c r="B20" s="212"/>
+      <c r="C20" s="206"/>
+      <c r="D20" s="208"/>
+      <c r="E20" s="210"/>
     </row>
     <row r="21" spans="1:5" s="193" customFormat="1" ht="158.25" customHeight="1">
       <c r="A21" s="189" t="s">
@@ -14494,11 +14553,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="33.75" customHeight="1">
-      <c r="A1" s="212" t="s">
+      <c r="A1" s="214" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="212"/>
-      <c r="C1" s="212"/>
+      <c r="B1" s="214"/>
+      <c r="C1" s="214"/>
     </row>
     <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="16" t="s">

</xml_diff>

<commit_message>
Vacunas actualizado 21-08-2020 at 13:44
</commit_message>
<xml_diff>
--- a/Tutoriales/pandas/Comandos Pandas.xlsx
+++ b/Tutoriales/pandas/Comandos Pandas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoseMaría\Documents\CURSOS\data_science\mitrabajo\mi_repositorio\Tutoriales\pandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AFD3CA-062C-4381-9BAD-F578718ACC7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2189F6-EE4A-492A-A22F-B5720224DFD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF4018AA-EEB9-4756-B82D-183D37B3B80A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{AF4018AA-EEB9-4756-B82D-183D37B3B80A}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERALES" sheetId="1" r:id="rId1"/>
@@ -10022,8 +10022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265136A6-C067-4B28-9F45-A6266FF6FD67}">
   <dimension ref="A1:D227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C157" sqref="C157"/>
+    <sheetView topLeftCell="B129" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="C138" sqref="C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -13215,8 +13215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C42D88-9A2B-46D3-B46D-33526406379A}">
   <dimension ref="A1:E228"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26.25"/>

</xml_diff>

<commit_message>
Proyecto agosto 2020 versión final
</commit_message>
<xml_diff>
--- a/Tutoriales/pandas/Comandos Pandas.xlsx
+++ b/Tutoriales/pandas/Comandos Pandas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoseMaría\Documents\CURSOS\data_science\mitrabajo\mi_repositorio\Tutoriales\pandas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoseMaría\Documents\cursos\data_science\mitrabajo\mi_repositorio\Tutoriales\pandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2189F6-EE4A-492A-A22F-B5720224DFD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0351DD-A04A-46B0-812B-536C988512E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{AF4018AA-EEB9-4756-B82D-183D37B3B80A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF4018AA-EEB9-4756-B82D-183D37B3B80A}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERALES" sheetId="1" r:id="rId1"/>
@@ -7665,6 +7665,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="66" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7705,15 +7714,6 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10022,8 +10022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265136A6-C067-4B28-9F45-A6266FF6FD67}">
   <dimension ref="A1:D227"/>
   <sheetViews>
-    <sheetView topLeftCell="B129" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C138" sqref="C138"/>
+    <sheetView tabSelected="1" topLeftCell="C34" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10035,12 +10035,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="33.75" customHeight="1">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="203" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="201"/>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
+      <c r="B1" s="204"/>
+      <c r="C1" s="204"/>
+      <c r="D1" s="204"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="102" t="s">
@@ -12290,14 +12290,14 @@
         <v>507</v>
       </c>
     </row>
-    <row r="163" spans="1:4" s="217" customFormat="1" ht="30">
+    <row r="163" spans="1:4" s="202" customFormat="1" ht="30">
       <c r="A163" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="B163" s="216" t="s">
+      <c r="B163" s="201" t="s">
         <v>656</v>
       </c>
-      <c r="C163" s="215" t="s">
+      <c r="C163" s="200" t="s">
         <v>655</v>
       </c>
       <c r="D163" s="92" t="s">
@@ -13215,7 +13215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C42D88-9A2B-46D3-B46D-33526406379A}">
   <dimension ref="A1:E228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -13230,13 +13230,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33.75" customHeight="1">
-      <c r="A1" s="202" t="s">
+      <c r="A1" s="205" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="202"/>
-      <c r="C1" s="202"/>
-      <c r="D1" s="203"/>
-      <c r="E1" s="204"/>
+      <c r="B1" s="205"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="206"/>
+      <c r="E1" s="207"/>
     </row>
     <row r="2" spans="1:5" ht="207" customHeight="1">
       <c r="A2" s="43" t="s">
@@ -13483,22 +13483,22 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="408.95" customHeight="1">
-      <c r="A19" s="213" t="s">
+      <c r="A19" s="216" t="s">
         <v>222</v>
       </c>
-      <c r="B19" s="211" t="s">
+      <c r="B19" s="214" t="s">
         <v>592</v>
       </c>
-      <c r="C19" s="205"/>
-      <c r="D19" s="207"/>
-      <c r="E19" s="209"/>
+      <c r="C19" s="208"/>
+      <c r="D19" s="210"/>
+      <c r="E19" s="212"/>
     </row>
     <row r="20" spans="1:5" ht="351.75" customHeight="1">
-      <c r="A20" s="212"/>
-      <c r="B20" s="212"/>
-      <c r="C20" s="206"/>
-      <c r="D20" s="208"/>
-      <c r="E20" s="210"/>
+      <c r="A20" s="215"/>
+      <c r="B20" s="215"/>
+      <c r="C20" s="209"/>
+      <c r="D20" s="211"/>
+      <c r="E20" s="213"/>
     </row>
     <row r="21" spans="1:5" s="193" customFormat="1" ht="158.25" customHeight="1">
       <c r="A21" s="189" t="s">
@@ -14620,11 +14620,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="33.75" customHeight="1">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="217" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="214"/>
-      <c r="C1" s="214"/>
+      <c r="B1" s="217"/>
+      <c r="C1" s="217"/>
     </row>
     <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="16" t="s">

</xml_diff>